<commit_message>
Enhance index.html with new sorting functionality for verified results, allowing users to sort by score, date, or model name. Refactor progress chart initialization for improved reliability and add date display in leaderboard. Update default filter settings for clarity. Update osworld_verified_results.xlsx to ensure data accuracy.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="97">
   <si>
     <t>Model</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Score Std@3</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
   <si>
     <t>chrome</t>
@@ -999,18 +1002,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1029,14 +1032,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1519,10 +1525,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V1040"/>
+  <dimension ref="A1:W1040"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -1540,7 +1546,7 @@
     <col min="16" max="16" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.75" customHeight="1" spans="1:22">
+    <row r="1" ht="16.75" customHeight="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1607,25 +1613,28 @@
       <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" ht="16.75" customHeight="1" spans="1:23">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2" s="4">
         <v>15</v>
@@ -1639,7 +1648,9 @@
         <v>26</v>
       </c>
       <c r="L2" s="11"/>
-      <c r="M2" s="2"/>
+      <c r="M2" s="15">
+        <v>45869</v>
+      </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -1649,25 +1660,26 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-    </row>
-    <row r="3" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W2" s="2"/>
+    </row>
+    <row r="3" ht="16.75" customHeight="1" spans="1:23">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="4">
         <v>50</v>
@@ -1681,7 +1693,9 @@
         <v>31.3</v>
       </c>
       <c r="L3" s="11"/>
-      <c r="M3" s="2"/>
+      <c r="M3" s="15">
+        <v>45869</v>
+      </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -1691,25 +1705,26 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-    </row>
-    <row r="4" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W3" s="2"/>
+    </row>
+    <row r="4" ht="16.75" customHeight="1" spans="1:23">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="4">
         <v>100</v>
@@ -1723,7 +1738,9 @@
         <v>31.4</v>
       </c>
       <c r="L4" s="11"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="15">
+        <v>45869</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -1733,29 +1750,30 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
-    </row>
-    <row r="5" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W4" s="2"/>
+    </row>
+    <row r="5" ht="16.75" customHeight="1" spans="1:23">
       <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1771,29 +1789,30 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
-    </row>
-    <row r="6" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W5" s="2"/>
+    </row>
+    <row r="6" ht="16.75" customHeight="1" spans="1:23">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1809,25 +1828,26 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
-    </row>
-    <row r="7" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" ht="16.75" customHeight="1" spans="1:23">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="4">
         <v>15</v>
@@ -1841,7 +1861,9 @@
         <v>9.1</v>
       </c>
       <c r="L7" s="11"/>
-      <c r="M7" s="2"/>
+      <c r="M7" s="15">
+        <v>45869</v>
+      </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -1851,25 +1873,26 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-    </row>
-    <row r="8" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W7" s="2"/>
+    </row>
+    <row r="8" ht="16.75" customHeight="1" spans="1:23">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G8" s="4">
         <v>50</v>
@@ -1883,7 +1906,9 @@
         <v>17.2</v>
       </c>
       <c r="L8" s="11"/>
-      <c r="M8" s="2"/>
+      <c r="M8" s="15">
+        <v>45869</v>
+      </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
@@ -1893,25 +1918,26 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-    </row>
-    <row r="9" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W8" s="2"/>
+    </row>
+    <row r="9" ht="16.75" customHeight="1" spans="1:23">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G9" s="4">
         <v>100</v>
@@ -1925,7 +1951,9 @@
         <v>23</v>
       </c>
       <c r="L9" s="11"/>
-      <c r="M9" s="2"/>
+      <c r="M9" s="15">
+        <v>45869</v>
+      </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
@@ -1935,25 +1963,26 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
-    </row>
-    <row r="10" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W9" s="2"/>
+    </row>
+    <row r="10" ht="16.75" customHeight="1" spans="1:23">
       <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" s="4">
         <v>15</v>
@@ -1967,37 +1996,40 @@
         <v>27.1</v>
       </c>
       <c r="L10" s="11"/>
-      <c r="M10" s="2"/>
+      <c r="M10" s="15">
+        <v>45869</v>
+      </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-    </row>
-    <row r="11" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W10" s="2"/>
+    </row>
+    <row r="11" ht="16.75" customHeight="1" spans="1:23">
       <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G11" s="4">
         <v>50</v>
@@ -2011,37 +2043,40 @@
         <v>35.8</v>
       </c>
       <c r="L11" s="11"/>
-      <c r="M11" s="2"/>
+      <c r="M11" s="15">
+        <v>45869</v>
+      </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-    </row>
-    <row r="12" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W11" s="2"/>
+    </row>
+    <row r="12" ht="16.75" customHeight="1" spans="1:23">
       <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G12" s="4">
         <v>100</v>
@@ -2055,37 +2090,40 @@
         <v>35.6</v>
       </c>
       <c r="L12" s="11"/>
-      <c r="M12" s="2"/>
+      <c r="M12" s="15">
+        <v>45869</v>
+      </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-    </row>
-    <row r="13" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W12" s="2"/>
+    </row>
+    <row r="13" ht="16.75" customHeight="1" spans="1:23">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G13" s="4">
         <v>15</v>
@@ -2099,37 +2137,40 @@
         <v>31.2</v>
       </c>
       <c r="L13" s="11"/>
-      <c r="M13" s="2"/>
+      <c r="M13" s="15">
+        <v>45869</v>
+      </c>
       <c r="N13" s="2"/>
-      <c r="O13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-    </row>
-    <row r="14" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W13" s="2"/>
+    </row>
+    <row r="14" ht="16.75" customHeight="1" spans="1:23">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G14" s="4">
         <v>50</v>
@@ -2143,37 +2184,40 @@
         <v>43.9</v>
       </c>
       <c r="L14" s="11"/>
-      <c r="M14" s="2"/>
+      <c r="M14" s="15">
+        <v>45869</v>
+      </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-    </row>
-    <row r="15" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W14" s="2"/>
+    </row>
+    <row r="15" ht="16.75" customHeight="1" spans="1:23">
       <c r="A15" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G15" s="4">
         <v>100</v>
@@ -2187,37 +2231,40 @@
         <v>41.4</v>
       </c>
       <c r="L15" s="11"/>
-      <c r="M15" s="2"/>
+      <c r="M15" s="15">
+        <v>45869</v>
+      </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-    </row>
-    <row r="16" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W15" s="2"/>
+    </row>
+    <row r="16" ht="16.75" customHeight="1" spans="1:23">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G16" s="4">
         <v>15</v>
@@ -2231,7 +2278,9 @@
         <v>27.8</v>
       </c>
       <c r="L16" s="11"/>
-      <c r="M16" s="2"/>
+      <c r="M16" s="15">
+        <v>45869</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -2241,25 +2290,26 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-    </row>
-    <row r="17" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W16" s="2"/>
+    </row>
+    <row r="17" ht="16.75" customHeight="1" spans="1:23">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G17" s="4">
         <v>100</v>
@@ -2273,7 +2323,9 @@
         <v>33.8</v>
       </c>
       <c r="L17" s="11"/>
-      <c r="M17" s="2"/>
+      <c r="M17" s="15">
+        <v>45869</v>
+      </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
@@ -2283,25 +2335,26 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-    </row>
-    <row r="18" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W17" s="2"/>
+    </row>
+    <row r="18" ht="16.75" customHeight="1" spans="1:23">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G18" s="4">
         <v>15</v>
@@ -2315,7 +2368,9 @@
         <v>31.9</v>
       </c>
       <c r="L18" s="11"/>
-      <c r="M18" s="2"/>
+      <c r="M18" s="15">
+        <v>45869</v>
+      </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -2325,25 +2380,26 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-    </row>
-    <row r="19" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W18" s="2"/>
+    </row>
+    <row r="19" ht="16.75" customHeight="1" spans="1:23">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G19" s="4">
         <v>100</v>
@@ -2357,7 +2413,9 @@
         <v>40</v>
       </c>
       <c r="L19" s="11"/>
-      <c r="M19" s="2"/>
+      <c r="M19" s="15">
+        <v>45869</v>
+      </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -2367,25 +2425,26 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
-    </row>
-    <row r="20" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W19" s="2"/>
+    </row>
+    <row r="20" ht="16.75" customHeight="1" spans="1:23">
       <c r="A20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="F20" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G20" s="4">
         <v>15</v>
@@ -2401,7 +2460,9 @@
         <v>24.5</v>
       </c>
       <c r="L20" s="11"/>
-      <c r="M20" s="2"/>
+      <c r="M20" s="15">
+        <v>45869</v>
+      </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -2411,25 +2472,26 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-    </row>
-    <row r="21" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W20" s="2"/>
+    </row>
+    <row r="21" ht="16.75" customHeight="1" spans="1:23">
       <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="F21" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G21" s="4">
         <v>50</v>
@@ -2445,7 +2507,9 @@
         <v>27.3</v>
       </c>
       <c r="L21" s="11"/>
-      <c r="M21" s="2"/>
+      <c r="M21" s="15">
+        <v>45869</v>
+      </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -2455,25 +2519,26 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-    </row>
-    <row r="22" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W21" s="2"/>
+    </row>
+    <row r="22" ht="16.75" customHeight="1" spans="1:23">
       <c r="A22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="F22" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G22" s="4">
         <v>100</v>
@@ -2489,7 +2554,9 @@
         <v>27.4</v>
       </c>
       <c r="L22" s="11"/>
-      <c r="M22" s="2"/>
+      <c r="M22" s="15">
+        <v>45869</v>
+      </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -2499,25 +2566,26 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-    </row>
-    <row r="23" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W22" s="2"/>
+    </row>
+    <row r="23" ht="16.75" customHeight="1" spans="1:23">
       <c r="A23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="G23" s="4">
         <v>15</v>
@@ -2531,7 +2599,9 @@
         <v>24</v>
       </c>
       <c r="L23" s="11"/>
-      <c r="M23" s="2"/>
+      <c r="M23" s="15">
+        <v>45869</v>
+      </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -2541,25 +2611,26 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-    </row>
-    <row r="24" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W23" s="2"/>
+    </row>
+    <row r="24" ht="16.75" customHeight="1" spans="1:23">
       <c r="A24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="G24" s="4">
         <v>50</v>
@@ -2573,7 +2644,9 @@
         <v>25.8</v>
       </c>
       <c r="L24" s="11"/>
-      <c r="M24" s="2"/>
+      <c r="M24" s="15">
+        <v>45869</v>
+      </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -2583,25 +2656,26 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-    </row>
-    <row r="25" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W24" s="2"/>
+    </row>
+    <row r="25" ht="16.75" customHeight="1" spans="1:23">
       <c r="A25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="G25" s="4">
         <v>100</v>
@@ -2615,7 +2689,9 @@
         <v>27.1</v>
       </c>
       <c r="L25" s="11"/>
-      <c r="M25" s="2"/>
+      <c r="M25" s="15">
+        <v>45869</v>
+      </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
@@ -2625,25 +2701,26 @@
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-    </row>
-    <row r="26" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W25" s="2"/>
+    </row>
+    <row r="26" ht="16.75" customHeight="1" spans="1:23">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G26" s="4">
         <v>15</v>
@@ -2657,7 +2734,9 @@
         <v>16.9</v>
       </c>
       <c r="L26" s="11"/>
-      <c r="M26" s="2"/>
+      <c r="M26" s="15">
+        <v>45869</v>
+      </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
@@ -2667,25 +2746,26 @@
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
-    </row>
-    <row r="27" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W26" s="2"/>
+    </row>
+    <row r="27" ht="16.75" customHeight="1" spans="1:23">
       <c r="A27" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G27" s="4">
         <v>50</v>
@@ -2699,7 +2779,9 @@
         <v>19.9</v>
       </c>
       <c r="L27" s="11"/>
-      <c r="M27" s="2"/>
+      <c r="M27" s="15">
+        <v>45869</v>
+      </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -2709,25 +2791,26 @@
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
-    </row>
-    <row r="28" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W27" s="2"/>
+    </row>
+    <row r="28" ht="16.75" customHeight="1" spans="1:23">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G28" s="4">
         <v>100</v>
@@ -2741,7 +2824,9 @@
         <v>18.8</v>
       </c>
       <c r="L28" s="11"/>
-      <c r="M28" s="2"/>
+      <c r="M28" s="15">
+        <v>45869</v>
+      </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -2751,25 +2836,26 @@
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
-    </row>
-    <row r="29" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W28" s="2"/>
+    </row>
+    <row r="29" ht="16.75" customHeight="1" spans="1:23">
       <c r="A29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="E29" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G29" s="4">
         <v>15</v>
@@ -2783,7 +2869,9 @@
         <v>19.9</v>
       </c>
       <c r="L29" s="11"/>
-      <c r="M29" s="2"/>
+      <c r="M29" s="15">
+        <v>45869</v>
+      </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
@@ -2793,25 +2881,26 @@
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
-    </row>
-    <row r="30" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W29" s="2"/>
+    </row>
+    <row r="30" ht="16.75" customHeight="1" spans="1:23">
       <c r="A30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="E30" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G30" s="4">
         <v>50</v>
@@ -2825,7 +2914,9 @@
         <v>20.6</v>
       </c>
       <c r="L30" s="11"/>
-      <c r="M30" s="2"/>
+      <c r="M30" s="15">
+        <v>45869</v>
+      </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
@@ -2835,25 +2926,26 @@
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
-    </row>
-    <row r="31" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W30" s="2"/>
+    </row>
+    <row r="31" ht="16.75" customHeight="1" spans="1:23">
       <c r="A31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="E31" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G31" s="4">
         <v>100</v>
@@ -2867,7 +2959,9 @@
         <v>23.1</v>
       </c>
       <c r="L31" s="11"/>
-      <c r="M31" s="2"/>
+      <c r="M31" s="15">
+        <v>45869</v>
+      </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
@@ -2877,25 +2971,26 @@
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
-    </row>
-    <row r="32" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W31" s="2"/>
+    </row>
+    <row r="32" ht="16.75" customHeight="1" spans="1:23">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G32" s="4">
         <v>15</v>
@@ -2915,7 +3010,9 @@
       <c r="L32" s="12">
         <v>1.7</v>
       </c>
-      <c r="M32" s="2"/>
+      <c r="M32" s="15">
+        <v>45869</v>
+      </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
@@ -2925,25 +3022,26 @@
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
-    </row>
-    <row r="33" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W32" s="2"/>
+    </row>
+    <row r="33" ht="16.75" customHeight="1" spans="1:23">
       <c r="A33" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G33" s="4">
         <v>50</v>
@@ -2963,7 +3061,9 @@
       <c r="L33" s="12">
         <v>0.82</v>
       </c>
-      <c r="M33" s="2"/>
+      <c r="M33" s="15">
+        <v>45869</v>
+      </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
@@ -2973,25 +3073,26 @@
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
-    </row>
-    <row r="34" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W33" s="2"/>
+    </row>
+    <row r="34" ht="16.75" customHeight="1" spans="1:23">
       <c r="A34" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G34" s="4">
         <v>100</v>
@@ -3011,7 +3112,9 @@
       <c r="L34" s="12">
         <v>0.55</v>
       </c>
-      <c r="M34" s="2"/>
+      <c r="M34" s="15">
+        <v>45869</v>
+      </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
@@ -3021,25 +3124,26 @@
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
-    </row>
-    <row r="35" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W34" s="2"/>
+    </row>
+    <row r="35" ht="16.75" customHeight="1" spans="1:23">
       <c r="A35" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G35" s="4">
         <v>15</v>
@@ -3059,7 +3163,9 @@
       <c r="L35" s="12">
         <v>1.36</v>
       </c>
-      <c r="M35" s="2"/>
+      <c r="M35" s="15">
+        <v>45869</v>
+      </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
@@ -3069,25 +3175,26 @@
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
-    </row>
-    <row r="36" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W35" s="2"/>
+    </row>
+    <row r="36" ht="16.75" customHeight="1" spans="1:23">
       <c r="A36" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G36" s="4">
         <v>50</v>
@@ -3107,7 +3214,9 @@
       <c r="L36" s="12">
         <v>0.85</v>
       </c>
-      <c r="M36" s="2"/>
+      <c r="M36" s="15">
+        <v>45869</v>
+      </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
@@ -3117,25 +3226,26 @@
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
-    </row>
-    <row r="37" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W36" s="2"/>
+    </row>
+    <row r="37" ht="16.75" customHeight="1" spans="1:23">
       <c r="A37" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G37" s="4">
         <v>100</v>
@@ -3155,7 +3265,9 @@
       <c r="L37" s="12">
         <v>0.95</v>
       </c>
-      <c r="M37" s="2"/>
+      <c r="M37" s="15">
+        <v>45869</v>
+      </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
@@ -3165,25 +3277,26 @@
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
-    </row>
-    <row r="38" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W37" s="2"/>
+    </row>
+    <row r="38" ht="16.75" customHeight="1" spans="1:23">
       <c r="A38" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G38" s="4">
         <v>15</v>
@@ -3197,7 +3310,9 @@
         <v>3</v>
       </c>
       <c r="L38" s="11"/>
-      <c r="M38" s="2"/>
+      <c r="M38" s="15">
+        <v>45869</v>
+      </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
@@ -3207,25 +3322,26 @@
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
-    </row>
-    <row r="39" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W38" s="2"/>
+    </row>
+    <row r="39" ht="16.75" customHeight="1" spans="1:23">
       <c r="A39" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G39" s="4">
         <v>100</v>
@@ -3239,7 +3355,9 @@
         <v>3.9</v>
       </c>
       <c r="L39" s="11"/>
-      <c r="M39" s="2"/>
+      <c r="M39" s="15">
+        <v>45869</v>
+      </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
@@ -3249,25 +3367,26 @@
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
-    </row>
-    <row r="40" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W39" s="2"/>
+    </row>
+    <row r="40" ht="16.75" customHeight="1" spans="1:23">
       <c r="A40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="E40" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G40" s="4">
         <v>15</v>
@@ -3281,7 +3400,9 @@
         <v>4.4</v>
       </c>
       <c r="L40" s="11"/>
-      <c r="M40" s="2"/>
+      <c r="M40" s="15">
+        <v>45869</v>
+      </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
@@ -3291,25 +3412,26 @@
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
-    </row>
-    <row r="41" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W40" s="2"/>
+    </row>
+    <row r="41" ht="16.75" customHeight="1" spans="1:23">
       <c r="A41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="E41" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G41" s="4">
         <v>100</v>
@@ -3323,7 +3445,9 @@
         <v>5</v>
       </c>
       <c r="L41" s="11"/>
-      <c r="M41" s="2"/>
+      <c r="M41" s="15">
+        <v>45869</v>
+      </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
@@ -3333,25 +3457,26 @@
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
-    </row>
-    <row r="42" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W41" s="2"/>
+    </row>
+    <row r="42" ht="16.75" customHeight="1" spans="1:23">
       <c r="A42" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G42" s="4">
         <v>15</v>
@@ -3365,7 +3490,9 @@
         <v>9.7</v>
       </c>
       <c r="L42" s="11"/>
-      <c r="M42" s="2"/>
+      <c r="M42" s="15">
+        <v>45869</v>
+      </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
@@ -3375,25 +3502,26 @@
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
-    </row>
-    <row r="43" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W42" s="2"/>
+    </row>
+    <row r="43" ht="16.75" customHeight="1" spans="1:23">
       <c r="A43" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G43" s="4">
         <v>100</v>
@@ -3407,7 +3535,9 @@
         <v>10.3</v>
       </c>
       <c r="L43" s="11"/>
-      <c r="M43" s="2"/>
+      <c r="M43" s="15">
+        <v>45869</v>
+      </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
@@ -3417,25 +3547,26 @@
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
-    </row>
-    <row r="44" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W43" s="2"/>
+    </row>
+    <row r="44" ht="16.75" customHeight="1" spans="1:23">
       <c r="A44" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G44" s="4">
         <v>50</v>
@@ -3449,7 +3580,9 @@
         <v>45.8</v>
       </c>
       <c r="L44" s="11"/>
-      <c r="M44" s="2"/>
+      <c r="M44" s="15">
+        <v>45869</v>
+      </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
@@ -3459,31 +3592,32 @@
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
-    </row>
-    <row r="45" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W44" s="2"/>
+    </row>
+    <row r="45" ht="16.75" customHeight="1" spans="1:23">
       <c r="A45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="F45" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G45" s="4">
         <v>50</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -3499,25 +3633,26 @@
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
-    </row>
-    <row r="46" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W45" s="2"/>
+    </row>
+    <row r="46" ht="16.75" customHeight="1" spans="1:23">
       <c r="A46" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G46" s="4">
         <v>15</v>
@@ -3531,7 +3666,9 @@
         <v>26.8</v>
       </c>
       <c r="L46" s="11"/>
-      <c r="M46" s="2"/>
+      <c r="M46" s="15">
+        <v>45869</v>
+      </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
@@ -3541,25 +3678,26 @@
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
-    </row>
-    <row r="47" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W46" s="2"/>
+    </row>
+    <row r="47" ht="16.75" customHeight="1" spans="1:23">
       <c r="A47" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G47" s="4">
         <v>50</v>
@@ -3573,7 +3711,9 @@
         <v>27</v>
       </c>
       <c r="L47" s="11"/>
-      <c r="M47" s="2"/>
+      <c r="M47" s="15">
+        <v>45869</v>
+      </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
@@ -3583,25 +3723,26 @@
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
-    </row>
-    <row r="48" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W47" s="2"/>
+    </row>
+    <row r="48" ht="16.75" customHeight="1" spans="1:23">
       <c r="A48" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G48" s="4">
         <v>100</v>
@@ -3615,7 +3756,9 @@
         <v>29.3</v>
       </c>
       <c r="L48" s="11"/>
-      <c r="M48" s="2"/>
+      <c r="M48" s="15">
+        <v>45869</v>
+      </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
@@ -3625,25 +3768,26 @@
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
-    </row>
-    <row r="49" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W48" s="2"/>
+    </row>
+    <row r="49" ht="16.75" customHeight="1" spans="1:23">
       <c r="A49" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="E49" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G49" s="4">
         <v>15</v>
@@ -3657,7 +3801,9 @@
         <v>42.4</v>
       </c>
       <c r="L49" s="11"/>
-      <c r="M49" s="2"/>
+      <c r="M49" s="15">
+        <v>45869</v>
+      </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
@@ -3667,25 +3813,26 @@
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
-    </row>
-    <row r="50" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W49" s="2"/>
+    </row>
+    <row r="50" ht="16.75" customHeight="1" spans="1:23">
       <c r="A50" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="E50" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G50" s="4">
         <v>50</v>
@@ -3699,7 +3846,9 @@
         <v>50.6</v>
       </c>
       <c r="L50" s="11"/>
-      <c r="M50" s="2"/>
+      <c r="M50" s="15">
+        <v>45869</v>
+      </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
@@ -3709,25 +3858,26 @@
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
-    </row>
-    <row r="51" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W50" s="2"/>
+    </row>
+    <row r="51" ht="16.75" customHeight="1" spans="1:23">
       <c r="A51" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="E51" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G51" s="4">
         <v>100</v>
@@ -3741,7 +3891,9 @@
         <v>51</v>
       </c>
       <c r="L51" s="11"/>
-      <c r="M51" s="2"/>
+      <c r="M51" s="15">
+        <v>45869</v>
+      </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
@@ -3751,25 +3903,26 @@
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
-    </row>
-    <row r="52" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W51" s="2"/>
+    </row>
+    <row r="52" ht="16.75" customHeight="1" spans="1:23">
       <c r="A52" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G52" s="4">
         <v>50</v>
@@ -3783,7 +3936,9 @@
         <v>48.6</v>
       </c>
       <c r="L52" s="11"/>
-      <c r="M52" s="2"/>
+      <c r="M52" s="15">
+        <v>45869</v>
+      </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
@@ -3793,25 +3948,26 @@
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
-    </row>
-    <row r="53" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W52" s="2"/>
+    </row>
+    <row r="53" ht="16.75" customHeight="1" spans="1:23">
       <c r="A53" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G53" s="4">
         <v>100</v>
@@ -3825,7 +3981,9 @@
         <v>53.1</v>
       </c>
       <c r="L53" s="11"/>
-      <c r="M53" s="2"/>
+      <c r="M53" s="15">
+        <v>45869</v>
+      </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
@@ -3835,31 +3993,32 @@
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
-    </row>
-    <row r="54" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W53" s="2"/>
+    </row>
+    <row r="54" ht="16.75" customHeight="1" spans="1:23">
       <c r="A54" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G54" s="4">
         <v>15</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -3875,31 +4034,32 @@
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
-    </row>
-    <row r="55" ht="16.75" customHeight="1" spans="1:22">
+      <c r="W54" s="2"/>
+    </row>
+    <row r="55" ht="16.75" customHeight="1" spans="1:23">
       <c r="A55" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G55" s="4">
         <v>100</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -3915,6 +4075,7 @@
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
+      <c r="W55" s="2"/>
     </row>
     <row r="56" ht="15.2" spans="6:12">
       <c r="F56" s="9"/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx to incorporate the latest verified data, ensuring continued accuracy for analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -748,12 +748,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -878,7 +893,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -890,34 +905,34 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1002,7 +1017,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
@@ -1040,7 +1055,10 @@
     </xf>
     <xf numFmtId="176" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1528,7 +1546,7 @@
   <dimension ref="A1:W1040"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -1649,7 +1667,7 @@
       </c>
       <c r="L2" s="11"/>
       <c r="M2" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -1694,7 +1712,7 @@
       </c>
       <c r="L3" s="11"/>
       <c r="M3" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1739,7 +1757,7 @@
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1779,7 +1797,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="16"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -1818,7 +1836,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="2"/>
+      <c r="M6" s="16"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -1862,7 +1880,7 @@
       </c>
       <c r="L7" s="11"/>
       <c r="M7" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -1907,7 +1925,7 @@
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -1952,7 +1970,7 @@
       </c>
       <c r="L9" s="11"/>
       <c r="M9" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -1997,7 +2015,7 @@
       </c>
       <c r="L10" s="11"/>
       <c r="M10" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -2044,7 +2062,7 @@
       </c>
       <c r="L11" s="11"/>
       <c r="M11" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2091,7 +2109,7 @@
       </c>
       <c r="L12" s="11"/>
       <c r="M12" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -2138,7 +2156,7 @@
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -2185,7 +2203,7 @@
       </c>
       <c r="L14" s="11"/>
       <c r="M14" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -2232,7 +2250,7 @@
       </c>
       <c r="L15" s="11"/>
       <c r="M15" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -2279,7 +2297,7 @@
       </c>
       <c r="L16" s="11"/>
       <c r="M16" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -2324,7 +2342,7 @@
       </c>
       <c r="L17" s="11"/>
       <c r="M17" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -2369,7 +2387,7 @@
       </c>
       <c r="L18" s="11"/>
       <c r="M18" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -2414,7 +2432,7 @@
       </c>
       <c r="L19" s="11"/>
       <c r="M19" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -2461,7 +2479,7 @@
       </c>
       <c r="L20" s="11"/>
       <c r="M20" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -2508,7 +2526,7 @@
       </c>
       <c r="L21" s="11"/>
       <c r="M21" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -2555,7 +2573,7 @@
       </c>
       <c r="L22" s="11"/>
       <c r="M22" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -2600,7 +2618,7 @@
       </c>
       <c r="L23" s="11"/>
       <c r="M23" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -2645,7 +2663,7 @@
       </c>
       <c r="L24" s="11"/>
       <c r="M24" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -2690,7 +2708,7 @@
       </c>
       <c r="L25" s="11"/>
       <c r="M25" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -2735,7 +2753,7 @@
       </c>
       <c r="L26" s="11"/>
       <c r="M26" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -2780,7 +2798,7 @@
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -2825,7 +2843,7 @@
       </c>
       <c r="L28" s="11"/>
       <c r="M28" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
@@ -2870,7 +2888,7 @@
       </c>
       <c r="L29" s="11"/>
       <c r="M29" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -2915,7 +2933,7 @@
       </c>
       <c r="L30" s="11"/>
       <c r="M30" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -2960,7 +2978,7 @@
       </c>
       <c r="L31" s="11"/>
       <c r="M31" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -3011,7 +3029,7 @@
         <v>1.7</v>
       </c>
       <c r="M32" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -3062,7 +3080,7 @@
         <v>0.82</v>
       </c>
       <c r="M33" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -3113,7 +3131,7 @@
         <v>0.55</v>
       </c>
       <c r="M34" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -3164,7 +3182,7 @@
         <v>1.36</v>
       </c>
       <c r="M35" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -3215,7 +3233,7 @@
         <v>0.85</v>
       </c>
       <c r="M36" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -3266,7 +3284,7 @@
         <v>0.95</v>
       </c>
       <c r="M37" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -3311,7 +3329,7 @@
       </c>
       <c r="L38" s="11"/>
       <c r="M38" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -3356,7 +3374,7 @@
       </c>
       <c r="L39" s="11"/>
       <c r="M39" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -3401,7 +3419,7 @@
       </c>
       <c r="L40" s="11"/>
       <c r="M40" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -3446,7 +3464,7 @@
       </c>
       <c r="L41" s="11"/>
       <c r="M41" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -3491,7 +3509,7 @@
       </c>
       <c r="L42" s="11"/>
       <c r="M42" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -3536,7 +3554,7 @@
       </c>
       <c r="L43" s="11"/>
       <c r="M43" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -3581,7 +3599,7 @@
       </c>
       <c r="L44" s="11"/>
       <c r="M44" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -3623,7 +3641,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
-      <c r="M45" s="2"/>
+      <c r="M45" s="16"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
@@ -3667,7 +3685,7 @@
       </c>
       <c r="L46" s="11"/>
       <c r="M46" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -3712,7 +3730,7 @@
       </c>
       <c r="L47" s="11"/>
       <c r="M47" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -3757,7 +3775,7 @@
       </c>
       <c r="L48" s="11"/>
       <c r="M48" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -3802,7 +3820,7 @@
       </c>
       <c r="L49" s="11"/>
       <c r="M49" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -3847,7 +3865,7 @@
       </c>
       <c r="L50" s="11"/>
       <c r="M50" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -3892,7 +3910,7 @@
       </c>
       <c r="L51" s="11"/>
       <c r="M51" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -3937,7 +3955,7 @@
       </c>
       <c r="L52" s="11"/>
       <c r="M52" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -3982,7 +4000,7 @@
       </c>
       <c r="L53" s="11"/>
       <c r="M53" s="15">
-        <v>45869</v>
+        <v>45866</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with latest verified data and enhance index.css to apply 'Noto Sans' font across performance tables for improved consistency and readability.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="97">
   <si>
     <t>Model</t>
   </si>
@@ -1543,10 +1543,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W1040"/>
+  <dimension ref="A1:W1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -3614,7 +3614,7 @@
     </row>
     <row r="45" ht="16.75" customHeight="1" spans="1:23">
       <c r="A45" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>79</v>
@@ -3632,16 +3632,20 @@
         <v>28</v>
       </c>
       <c r="G45" s="4">
-        <v>50</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>84</v>
+        <v>15</v>
+      </c>
+      <c r="H45" s="2">
+        <v>34.64</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="11"/>
+      <c r="K45" s="11">
+        <v>34.64</v>
+      </c>
       <c r="L45" s="11"/>
-      <c r="M45" s="16"/>
+      <c r="M45" s="15">
+        <v>45869</v>
+      </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
@@ -3655,16 +3659,16 @@
     </row>
     <row r="46" ht="16.75" customHeight="1" spans="1:23">
       <c r="A46" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>82</v>
@@ -3673,20 +3677,16 @@
         <v>28</v>
       </c>
       <c r="G46" s="4">
-        <v>15</v>
-      </c>
-      <c r="H46" s="4">
-        <v>26.8</v>
+        <v>50</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-      <c r="K46" s="12">
-        <v>26.8</v>
-      </c>
+      <c r="K46" s="11"/>
       <c r="L46" s="11"/>
-      <c r="M46" s="15">
-        <v>45866</v>
-      </c>
+      <c r="M46" s="16"/>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
@@ -3718,15 +3718,15 @@
         <v>28</v>
       </c>
       <c r="G47" s="4">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H47" s="4">
-        <v>27</v>
+        <v>26.8</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="12">
-        <v>27</v>
+        <v>26.8</v>
       </c>
       <c r="L47" s="11"/>
       <c r="M47" s="15">
@@ -3763,15 +3763,15 @@
         <v>28</v>
       </c>
       <c r="G48" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H48" s="4">
-        <v>29.3</v>
+        <v>27</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="12">
-        <v>29.3</v>
+        <v>27</v>
       </c>
       <c r="L48" s="11"/>
       <c r="M48" s="15">
@@ -3790,7 +3790,7 @@
     </row>
     <row r="49" ht="16.75" customHeight="1" spans="1:23">
       <c r="A49" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>86</v>
@@ -3808,15 +3808,15 @@
         <v>28</v>
       </c>
       <c r="G49" s="4">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="H49" s="4">
-        <v>42.4</v>
+        <v>29.3</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="12">
-        <v>42.4</v>
+        <v>29.3</v>
       </c>
       <c r="L49" s="11"/>
       <c r="M49" s="15">
@@ -3853,15 +3853,15 @@
         <v>28</v>
       </c>
       <c r="G50" s="4">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H50" s="4">
-        <v>50.6</v>
+        <v>42.4</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="12">
-        <v>50.6</v>
+        <v>42.4</v>
       </c>
       <c r="L50" s="11"/>
       <c r="M50" s="15">
@@ -3898,15 +3898,15 @@
         <v>28</v>
       </c>
       <c r="G51" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H51" s="4">
-        <v>51</v>
+        <v>50.6</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="12">
-        <v>51</v>
+        <v>50.6</v>
       </c>
       <c r="L51" s="11"/>
       <c r="M51" s="15">
@@ -3925,16 +3925,16 @@
     </row>
     <row r="52" ht="16.75" customHeight="1" spans="1:23">
       <c r="A52" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>82</v>
@@ -3943,15 +3943,15 @@
         <v>28</v>
       </c>
       <c r="G52" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H52" s="4">
-        <v>48.59</v>
+        <v>51</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="12">
-        <v>48.6</v>
+        <v>51</v>
       </c>
       <c r="L52" s="11"/>
       <c r="M52" s="15">
@@ -3988,15 +3988,15 @@
         <v>28</v>
       </c>
       <c r="G53" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H53" s="4">
-        <v>53.1</v>
+        <v>48.59</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="12">
-        <v>53.1</v>
+        <v>48.6</v>
       </c>
       <c r="L53" s="11"/>
       <c r="M53" s="15">
@@ -4015,34 +4015,38 @@
     </row>
     <row r="54" ht="16.75" customHeight="1" spans="1:23">
       <c r="A54" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>56</v>
+        <v>93</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="G54" s="4">
-        <v>15</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>31</v>
+        <v>100</v>
+      </c>
+      <c r="H54" s="4">
+        <v>53.1</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
-      <c r="K54" s="11"/>
+      <c r="K54" s="12">
+        <v>53.1</v>
+      </c>
       <c r="L54" s="11"/>
-      <c r="M54" s="2"/>
+      <c r="M54" s="15">
+        <v>45866</v>
+      </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
@@ -4074,7 +4078,7 @@
         <v>58</v>
       </c>
       <c r="G55" s="4">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>31</v>
@@ -4095,11 +4099,46 @@
       <c r="V55" s="2"/>
       <c r="W55" s="2"/>
     </row>
-    <row r="56" ht="15.2" spans="6:12">
-      <c r="F56" s="9"/>
-      <c r="H56" s="10"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="14"/>
+    <row r="56" ht="16.75" customHeight="1" spans="1:23">
+      <c r="A56" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G56" s="4">
+        <v>100</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+      <c r="V56" s="2"/>
+      <c r="W56" s="2"/>
     </row>
     <row r="57" ht="15.2" spans="6:12">
       <c r="F57" s="9"/>
@@ -10005,8 +10044,14 @@
       <c r="K1040" s="13"/>
       <c r="L1040" s="14"/>
     </row>
+    <row r="1041" ht="15.2" spans="6:12">
+      <c r="F1041" s="9"/>
+      <c r="H1041" s="10"/>
+      <c r="K1041" s="13"/>
+      <c r="L1041" s="14"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1040">
+  <conditionalFormatting sqref="F1:F1041">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -10057,17 +10102,18 @@
     <hyperlink ref="C42" r:id="rId12" display="https://arxiv.org/abs/2504.07491" tooltip="https://arxiv.org/abs/2504.07491"/>
     <hyperlink ref="C43" r:id="rId12" display="https://arxiv.org/abs/2504.07491" tooltip="https://arxiv.org/abs/2504.07491"/>
     <hyperlink ref="C44" r:id="rId13" display="https://github.com/simular-ai/Agent-S" tooltip="https://github.com/simular-ai/Agent-S"/>
-    <hyperlink ref="C45" r:id="rId13" display="https://github.com/simular-ai/Agent-S" tooltip="https://github.com/simular-ai/Agent-S"/>
-    <hyperlink ref="C46" r:id="rId14" display="https://osworld-grounding.github.io/" tooltip="https://osworld-grounding.github.io/"/>
+    <hyperlink ref="C46" r:id="rId13" display="https://github.com/simular-ai/Agent-S" tooltip="https://github.com/simular-ai/Agent-S"/>
     <hyperlink ref="C47" r:id="rId14" display="https://osworld-grounding.github.io/" tooltip="https://osworld-grounding.github.io/"/>
     <hyperlink ref="C48" r:id="rId14" display="https://osworld-grounding.github.io/" tooltip="https://osworld-grounding.github.io/"/>
     <hyperlink ref="C49" r:id="rId14" display="https://osworld-grounding.github.io/" tooltip="https://osworld-grounding.github.io/"/>
     <hyperlink ref="C50" r:id="rId14" display="https://osworld-grounding.github.io/" tooltip="https://osworld-grounding.github.io/"/>
     <hyperlink ref="C51" r:id="rId14" display="https://osworld-grounding.github.io/" tooltip="https://osworld-grounding.github.io/"/>
-    <hyperlink ref="C52" r:id="rId15" display="https://arxiv.org/abs/2507.05791" tooltip="https://arxiv.org/abs/2507.05791"/>
+    <hyperlink ref="C52" r:id="rId14" display="https://osworld-grounding.github.io/" tooltip="https://osworld-grounding.github.io/"/>
     <hyperlink ref="C53" r:id="rId15" display="https://arxiv.org/abs/2507.05791" tooltip="https://arxiv.org/abs/2507.05791"/>
-    <hyperlink ref="C54" r:id="rId16" display="https://aguvis-project.github.io/" tooltip="https://aguvis-project.github.io/"/>
+    <hyperlink ref="C54" r:id="rId15" display="https://arxiv.org/abs/2507.05791" tooltip="https://arxiv.org/abs/2507.05791"/>
     <hyperlink ref="C55" r:id="rId16" display="https://aguvis-project.github.io/" tooltip="https://aguvis-project.github.io/"/>
+    <hyperlink ref="C56" r:id="rId16" display="https://aguvis-project.github.io/" tooltip="https://aguvis-project.github.io/"/>
+    <hyperlink ref="C45" r:id="rId13" display="https://github.com/simular-ai/Agent-S" tooltip="https://github.com/simular-ai/Agent-S"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with the latest verified data to ensure continued accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -1583,8 +1583,8 @@
   </sheetPr>
   <dimension ref="A1:W1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add category data aggregation and display in index.html for enhanced analysis
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="331">
   <si>
     <t>Model</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>vs_code</t>
-  </si>
-  <si>
-    <t>vc_code</t>
   </si>
   <si>
     <t>computer-use-preview</t>
@@ -2221,8 +2218,8 @@
   </sheetPr>
   <dimension ref="A1:AC1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="I30" workbookViewId="0">
+      <selection activeCell="W43" sqref="W43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -2299,31 +2296,25 @@
       <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
     </row>
     <row r="2" ht="16.75" customHeight="1" spans="1:22">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F2" s="6">
         <v>15</v>
@@ -2335,37 +2326,37 @@
         <v>26</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
@@ -2373,19 +2364,19 @@
     </row>
     <row r="3" ht="16.75" customHeight="1" spans="1:22">
       <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F3" s="6">
         <v>50</v>
@@ -2397,37 +2388,37 @@
         <v>31.3</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="S3" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
@@ -2435,19 +2426,19 @@
     </row>
     <row r="4" ht="16.75" customHeight="1" spans="1:22">
       <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F4" s="6">
         <v>100</v>
@@ -2459,37 +2450,37 @@
         <v>31.4</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
@@ -2497,19 +2488,19 @@
     </row>
     <row r="5" ht="16.75" customHeight="1" spans="1:22">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F5" s="6">
         <v>100</v>
@@ -2521,37 +2512,37 @@
         <v>29.63</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="R5" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="S5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
@@ -2559,24 +2550,24 @@
     </row>
     <row r="6" ht="16.75" customHeight="1" spans="1:22">
       <c r="A6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -2595,24 +2586,24 @@
     </row>
     <row r="7" ht="16.75" customHeight="1" spans="1:22">
       <c r="A7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -2631,19 +2622,19 @@
     </row>
     <row r="8" ht="16.75" customHeight="1" spans="1:22">
       <c r="A8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>70</v>
       </c>
       <c r="F8" s="6">
         <v>15</v>
@@ -2655,37 +2646,37 @@
         <v>9.1</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="S8" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="T8" s="11"/>
       <c r="U8" s="11"/>
@@ -2693,19 +2684,19 @@
     </row>
     <row r="9" ht="16.75" customHeight="1" spans="1:22">
       <c r="A9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>70</v>
       </c>
       <c r="F9" s="6">
         <v>50</v>
@@ -2717,37 +2708,37 @@
         <v>17.17</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="O9" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q9" s="3" t="s">
+      <c r="R9" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="R9" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="S9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T9" s="11"/>
       <c r="U9" s="11"/>
@@ -2755,19 +2746,19 @@
     </row>
     <row r="10" ht="16.75" customHeight="1" spans="1:22">
       <c r="A10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>70</v>
       </c>
       <c r="F10" s="6">
         <v>100</v>
@@ -2779,37 +2770,37 @@
         <v>23</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="R10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="S10" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="T10" s="11"/>
       <c r="U10" s="11"/>
@@ -2817,19 +2808,19 @@
     </row>
     <row r="11" ht="16.75" customHeight="1" spans="1:22">
       <c r="A11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E11" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="6">
         <v>15</v>
@@ -2841,37 +2832,37 @@
         <v>27.1</v>
       </c>
       <c r="I11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q11" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q11" s="3" t="s">
+      <c r="R11" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="R11" s="3" t="s">
+      <c r="S11" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="T11" s="11"/>
       <c r="U11" s="11"/>
@@ -2879,19 +2870,19 @@
     </row>
     <row r="12" ht="16.75" customHeight="1" spans="1:22">
       <c r="A12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E12" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F12" s="6">
         <v>50</v>
@@ -2903,37 +2894,37 @@
         <v>35.8</v>
       </c>
       <c r="I12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="N12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="N12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O12" s="3" t="s">
+      <c r="P12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R12" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R12" s="3" t="s">
+      <c r="S12" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="T12" s="11"/>
       <c r="U12" s="11"/>
@@ -2941,19 +2932,19 @@
     </row>
     <row r="13" ht="16.75" customHeight="1" spans="1:22">
       <c r="A13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="E13" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="6">
         <v>100</v>
@@ -2965,37 +2956,37 @@
         <v>35.6</v>
       </c>
       <c r="I13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M13" s="3" t="s">
+      <c r="N13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="3" t="s">
+      <c r="P13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R13" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="S13" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T13" s="11"/>
       <c r="U13" s="11"/>
@@ -3003,19 +2994,19 @@
     </row>
     <row r="14" ht="16.75" customHeight="1" spans="1:22">
       <c r="A14" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14" s="6">
         <v>15</v>
@@ -3027,37 +3018,37 @@
         <v>31.2</v>
       </c>
       <c r="I14" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="N14" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O14" s="3" t="s">
+      <c r="P14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R14" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="P14" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="S14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T14" s="11"/>
       <c r="U14" s="11"/>
@@ -3065,19 +3056,19 @@
     </row>
     <row r="15" ht="16.75" customHeight="1" spans="1:22">
       <c r="A15" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="6">
         <v>50</v>
@@ -3089,37 +3080,37 @@
         <v>43.9</v>
       </c>
       <c r="I15" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M15" s="3" t="s">
+      <c r="N15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="N15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="O15" s="3" t="s">
+      <c r="P15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q15" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q15" s="3" t="s">
+      <c r="R15" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="R15" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="S15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
@@ -3127,19 +3118,19 @@
     </row>
     <row r="16" s="1" customFormat="1" ht="16.75" customHeight="1" spans="1:29">
       <c r="A16" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="6">
         <v>100</v>
@@ -3151,37 +3142,37 @@
         <v>41.4</v>
       </c>
       <c r="I16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="K16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="O16" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="P16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R16" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="P16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="S16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
@@ -3196,19 +3187,19 @@
     </row>
     <row r="17" s="1" customFormat="1" ht="16.75" customHeight="1" spans="1:29">
       <c r="A17" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="E17" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" s="6">
         <v>15</v>
@@ -3220,37 +3211,37 @@
         <v>27.8</v>
       </c>
       <c r="I17" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="K17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="K17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="P17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="S17" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
@@ -3265,19 +3256,19 @@
     </row>
     <row r="18" ht="16.75" customHeight="1" spans="1:22">
       <c r="A18" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="E18" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="6">
         <v>100</v>
@@ -3289,37 +3280,37 @@
         <v>33.8</v>
       </c>
       <c r="I18" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="N18" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="N18" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O18" s="3" t="s">
+      <c r="P18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R18" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="P18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="S18" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T18" s="11"/>
       <c r="U18" s="11"/>
@@ -3327,19 +3318,19 @@
     </row>
     <row r="19" ht="16.75" customHeight="1" spans="1:22">
       <c r="A19" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="E19" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="6">
         <v>15</v>
@@ -3351,37 +3342,37 @@
         <v>31.9</v>
       </c>
       <c r="I19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="K19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="K19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="M19" s="3" t="s">
+      <c r="N19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O19" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="N19" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O19" s="3" t="s">
+      <c r="P19" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="P19" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="Q19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T19" s="11"/>
       <c r="U19" s="11"/>
@@ -3389,19 +3380,19 @@
     </row>
     <row r="20" ht="16.75" customHeight="1" spans="1:22">
       <c r="A20" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="E20" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="6">
         <v>100</v>
@@ -3413,37 +3404,37 @@
         <v>40</v>
       </c>
       <c r="I20" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="K20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="M20" s="3" t="s">
+      <c r="N20" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="N20" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="P20" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T20" s="11"/>
       <c r="U20" s="11"/>
@@ -3451,19 +3442,19 @@
     </row>
     <row r="21" ht="16.75" customHeight="1" spans="1:22">
       <c r="A21" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="F21" s="6">
         <v>15</v>
@@ -3491,19 +3482,19 @@
     </row>
     <row r="22" ht="16.75" customHeight="1" spans="1:22">
       <c r="A22" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="F22" s="6">
         <v>15</v>
@@ -3515,37 +3506,37 @@
         <v>23.3</v>
       </c>
       <c r="I22" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="K22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="O22" s="3" t="s">
+      <c r="P22" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="P22" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="Q22" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T22" s="11"/>
       <c r="U22" s="11"/>
@@ -3553,19 +3544,19 @@
     </row>
     <row r="23" ht="16.75" customHeight="1" spans="1:22">
       <c r="A23" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="F23" s="6">
         <v>50</v>
@@ -3593,19 +3584,19 @@
     </row>
     <row r="24" ht="16.75" customHeight="1" spans="1:22">
       <c r="A24" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E24" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="F24" s="6">
         <v>50</v>
@@ -3633,19 +3624,19 @@
     </row>
     <row r="25" ht="16.75" customHeight="1" spans="1:22">
       <c r="A25" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="E25" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="F25" s="6">
         <v>100</v>
@@ -3673,19 +3664,19 @@
     </row>
     <row r="26" ht="16.75" customHeight="1" spans="1:22">
       <c r="A26" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="F26" s="6">
         <v>100</v>
@@ -3713,19 +3704,19 @@
     </row>
     <row r="27" ht="16.75" customHeight="1" spans="1:22">
       <c r="A27" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="E27" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F27" s="6">
         <v>15</v>
@@ -3737,37 +3728,37 @@
         <v>24</v>
       </c>
       <c r="I27" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="K27" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="L27" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="M27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="M27" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O27" s="3" t="s">
+      <c r="P27" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q27" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="P27" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="R27" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T27" s="11"/>
       <c r="U27" s="11"/>
@@ -3775,19 +3766,19 @@
     </row>
     <row r="28" ht="16.75" customHeight="1" spans="1:22">
       <c r="A28" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="E28" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F28" s="6">
         <v>50</v>
@@ -3799,37 +3790,37 @@
         <v>25.8</v>
       </c>
       <c r="I28" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J28" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="K28" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L28" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="K28" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="L28" s="3" t="s">
+      <c r="M28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O28" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="M28" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="P28" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T28" s="11"/>
       <c r="U28" s="11"/>
@@ -3837,19 +3828,19 @@
     </row>
     <row r="29" ht="16.75" customHeight="1" spans="1:22">
       <c r="A29" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="E29" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F29" s="6">
         <v>100</v>
@@ -3861,37 +3852,37 @@
         <v>27.1</v>
       </c>
       <c r="I29" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J29" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="K29" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="L29" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="N29" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="O29" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="N29" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="P29" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R29" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T29" s="11"/>
       <c r="U29" s="11"/>
@@ -3899,19 +3890,19 @@
     </row>
     <row r="30" ht="16.75" customHeight="1" spans="1:22">
       <c r="A30" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E30" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F30" s="6">
         <v>15</v>
@@ -3923,37 +3914,37 @@
         <v>16.9</v>
       </c>
       <c r="I30" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="J30" s="3" t="s">
+      <c r="K30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L30" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L30" s="3" t="s">
+      <c r="M30" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="M30" s="3" t="s">
+      <c r="N30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O30" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="N30" s="3" t="s">
+      <c r="P30" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q30" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="O30" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="R30" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T30" s="11"/>
       <c r="U30" s="11"/>
@@ -3961,19 +3952,19 @@
     </row>
     <row r="31" ht="16.75" customHeight="1" spans="1:22">
       <c r="A31" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E31" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F31" s="6">
         <v>50</v>
@@ -3985,37 +3976,37 @@
         <v>19.9</v>
       </c>
       <c r="I31" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="M31" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="J31" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="M31" s="3" t="s">
+      <c r="N31" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="O31" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="N31" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="O31" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="P31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q31" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Q31" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="R31" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T31" s="11"/>
       <c r="U31" s="11"/>
@@ -4023,19 +4014,19 @@
     </row>
     <row r="32" ht="16.75" customHeight="1" spans="1:22">
       <c r="A32" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E32" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F32" s="6">
         <v>100</v>
@@ -4047,37 +4038,37 @@
         <v>17.7</v>
       </c>
       <c r="I32" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="J32" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="K32" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M32" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="M32" s="3" t="s">
+      <c r="N32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P32" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="N32" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="O32" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="P32" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="Q32" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T32" s="11"/>
       <c r="U32" s="11"/>
@@ -4085,19 +4076,19 @@
     </row>
     <row r="33" ht="16.75" customHeight="1" spans="1:22">
       <c r="A33" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E33" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F33" s="6">
         <v>15</v>
@@ -4109,37 +4100,37 @@
         <v>19.9</v>
       </c>
       <c r="I33" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J33" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="K33" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M33" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="K33" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M33" s="3" t="s">
+      <c r="N33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="O33" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="N33" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="O33" s="3" t="s">
-        <v>210</v>
-      </c>
       <c r="P33" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T33" s="11"/>
       <c r="U33" s="11"/>
@@ -4147,19 +4138,19 @@
     </row>
     <row r="34" ht="16.75" customHeight="1" spans="1:22">
       <c r="A34" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E34" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F34" s="6">
         <v>50</v>
@@ -4171,37 +4162,37 @@
         <v>20.6</v>
       </c>
       <c r="I34" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="J34" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="J34" s="3" t="s">
+      <c r="K34" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="L34" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O34" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="L34" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N34" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O34" s="3" t="s">
+      <c r="P34" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="P34" s="3" t="s">
-        <v>215</v>
-      </c>
       <c r="Q34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R34" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="S34" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T34" s="11"/>
       <c r="U34" s="11"/>
@@ -4209,19 +4200,19 @@
     </row>
     <row r="35" ht="16.75" customHeight="1" spans="1:22">
       <c r="A35" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E35" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F35" s="6">
         <v>100</v>
@@ -4233,37 +4224,37 @@
         <v>23.1</v>
       </c>
       <c r="I35" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O35" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="J35" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N35" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="O35" s="3" t="s">
+      <c r="P35" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="P35" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="Q35" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="R35" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T35" s="11"/>
       <c r="U35" s="11"/>
@@ -4271,19 +4262,19 @@
     </row>
     <row r="36" ht="16.75" customHeight="1" spans="1:22">
       <c r="A36" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E36" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F36" s="6">
         <v>15</v>
@@ -4295,37 +4286,37 @@
         <v>26.2</v>
       </c>
       <c r="I36" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O36" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="J36" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M36" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="N36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O36" s="3" t="s">
-        <v>221</v>
-      </c>
       <c r="P36" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="R36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T36" s="11"/>
       <c r="U36" s="11"/>
@@ -4333,19 +4324,19 @@
     </row>
     <row r="37" ht="16.75" customHeight="1" spans="1:22">
       <c r="A37" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E37" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F37" s="6">
         <v>15</v>
@@ -4357,37 +4348,37 @@
         <v>23.6</v>
       </c>
       <c r="I37" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M37" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="J37" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M37" s="3" t="s">
+      <c r="N37" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O37" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="N37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O37" s="3" t="s">
-        <v>224</v>
-      </c>
       <c r="P37" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T37" s="11"/>
       <c r="U37" s="11"/>
@@ -4395,19 +4386,19 @@
     </row>
     <row r="38" ht="16.75" customHeight="1" spans="1:22">
       <c r="A38" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E38" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F38" s="6">
         <v>15</v>
@@ -4419,37 +4410,37 @@
         <v>23</v>
       </c>
       <c r="I38" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M38" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="J38" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M38" s="3" t="s">
+      <c r="N38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O38" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="N38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="O38" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="P38" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R38" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T38" s="11"/>
       <c r="U38" s="11"/>
@@ -4457,19 +4448,19 @@
     </row>
     <row r="39" ht="16.75" customHeight="1" spans="1:22">
       <c r="A39" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E39" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F39" s="6">
         <v>50</v>
@@ -4497,19 +4488,19 @@
     </row>
     <row r="40" ht="16.75" customHeight="1" spans="1:22">
       <c r="A40" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E40" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F40" s="6">
         <v>50</v>
@@ -4537,19 +4528,19 @@
     </row>
     <row r="41" ht="16.75" customHeight="1" spans="1:22">
       <c r="A41" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E41" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F41" s="6">
         <v>50</v>
@@ -4577,19 +4568,19 @@
     </row>
     <row r="42" ht="16.75" customHeight="1" spans="1:22">
       <c r="A42" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E42" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F42" s="6">
         <v>100</v>
@@ -4617,19 +4608,19 @@
     </row>
     <row r="43" ht="16.75" customHeight="1" spans="1:22">
       <c r="A43" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E43" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F43" s="6">
         <v>100</v>
@@ -4657,19 +4648,19 @@
     </row>
     <row r="44" ht="16.75" customHeight="1" spans="1:22">
       <c r="A44" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E44" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F44" s="6">
         <v>100</v>
@@ -4697,19 +4688,19 @@
     </row>
     <row r="45" ht="16.75" customHeight="1" spans="1:22">
       <c r="A45" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E45" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F45" s="6">
         <v>15</v>
@@ -4737,19 +4728,19 @@
     </row>
     <row r="46" ht="16.75" customHeight="1" spans="1:22">
       <c r="A46" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E46" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F46" s="6">
         <v>15</v>
@@ -4777,19 +4768,19 @@
     </row>
     <row r="47" ht="16.75" customHeight="1" spans="1:22">
       <c r="A47" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="D47" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E47" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F47" s="6">
         <v>15</v>
@@ -4817,19 +4808,19 @@
     </row>
     <row r="48" ht="16.75" customHeight="1" spans="1:22">
       <c r="A48" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E48" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F48" s="6">
         <v>50</v>
@@ -4857,19 +4848,19 @@
     </row>
     <row r="49" ht="16.75" customHeight="1" spans="1:22">
       <c r="A49" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E49" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F49" s="6">
         <v>50</v>
@@ -4897,19 +4888,19 @@
     </row>
     <row r="50" ht="16.75" customHeight="1" spans="1:22">
       <c r="A50" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E50" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F50" s="6">
         <v>50</v>
@@ -4937,19 +4928,19 @@
     </row>
     <row r="51" ht="16.75" customHeight="1" spans="1:22">
       <c r="A51" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="D51" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E51" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F51" s="6">
         <v>100</v>
@@ -4977,19 +4968,19 @@
     </row>
     <row r="52" ht="16.75" customHeight="1" spans="1:22">
       <c r="A52" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="D52" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E52" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F52" s="6">
         <v>100</v>
@@ -5017,19 +5008,19 @@
     </row>
     <row r="53" ht="16.75" customHeight="1" spans="1:22">
       <c r="A53" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="D53" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="E53" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F53" s="6">
         <v>100</v>
@@ -5057,19 +5048,19 @@
     </row>
     <row r="54" ht="16.75" customHeight="1" spans="1:22">
       <c r="A54" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="C54" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="D54" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="E54" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F54" s="6">
         <v>15</v>
@@ -5081,37 +5072,37 @@
         <v>3.04</v>
       </c>
       <c r="I54" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K54" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="J54" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="K54" s="3" t="s">
+      <c r="L54" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M54" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="L54" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="M54" s="3" t="s">
+      <c r="N54" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="O54" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="N54" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="O54" s="3" t="s">
+      <c r="P54" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="P54" s="3" t="s">
+      <c r="Q54" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="Q54" s="3" t="s">
+      <c r="R54" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="R54" s="3" t="s">
+      <c r="S54" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="S54" s="3" t="s">
-        <v>240</v>
       </c>
       <c r="T54" s="11"/>
       <c r="U54" s="11"/>
@@ -5119,19 +5110,19 @@
     </row>
     <row r="55" ht="16.75" customHeight="1" spans="1:22">
       <c r="A55" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="E55" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F55" s="6">
         <v>100</v>
@@ -5143,37 +5134,37 @@
         <v>3.88</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q55" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R55" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="T55" s="11"/>
       <c r="U55" s="11"/>
@@ -5181,19 +5172,19 @@
     </row>
     <row r="56" ht="16.75" customHeight="1" spans="1:22">
       <c r="A56" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="D56" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="E56" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F56" s="6">
         <v>15</v>
@@ -5205,37 +5196,37 @@
         <v>4.43</v>
       </c>
       <c r="I56" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="J56" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="J56" s="3" t="s">
+      <c r="K56" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="K56" s="3" t="s">
+      <c r="L56" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M56" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="P56" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q56" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="L56" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="M56" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N56" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="O56" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="P56" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q56" s="3" t="s">
+      <c r="R56" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="R56" s="3" t="s">
-        <v>247</v>
-      </c>
       <c r="S56" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T56" s="11"/>
       <c r="U56" s="11"/>
@@ -5243,19 +5234,19 @@
     </row>
     <row r="57" ht="16.75" customHeight="1" spans="1:22">
       <c r="A57" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="E57" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F57" s="6">
         <v>100</v>
@@ -5267,37 +5258,37 @@
         <v>5</v>
       </c>
       <c r="I57" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="J57" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="J57" s="3" t="s">
-        <v>249</v>
-      </c>
       <c r="K57" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M57" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N57" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="P57" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="S57" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="N57" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="O57" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="P57" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q57" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="R57" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="S57" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="T57" s="11"/>
       <c r="U57" s="11"/>
@@ -5305,19 +5296,19 @@
     </row>
     <row r="58" ht="16.75" customHeight="1" spans="1:22">
       <c r="A58" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="D58" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="E58" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F58" s="6">
         <v>15</v>
@@ -5345,19 +5336,19 @@
     </row>
     <row r="59" ht="16.75" customHeight="1" spans="1:22">
       <c r="A59" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="E59" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F59" s="6">
         <v>100</v>
@@ -5385,19 +5376,19 @@
     </row>
     <row r="60" ht="31" spans="1:22">
       <c r="A60" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="D60" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="E60" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>258</v>
       </c>
       <c r="F60" s="6">
         <v>15</v>
@@ -5425,19 +5416,19 @@
     </row>
     <row r="61" ht="31" spans="1:22">
       <c r="A61" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="D61" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="E61" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>258</v>
       </c>
       <c r="F61" s="6">
         <v>50</v>
@@ -5449,37 +5440,37 @@
         <v>45.76</v>
       </c>
       <c r="I61" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="J61" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="J61" s="3" t="s">
+      <c r="K61" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="K61" s="3" t="s">
+      <c r="L61" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="L61" s="3" t="s">
+      <c r="M61" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N61" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O61" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="M61" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N61" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O61" s="3" t="s">
+      <c r="P61" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q61" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R61" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="P61" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q61" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R61" s="3" t="s">
-        <v>264</v>
-      </c>
       <c r="S61" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
@@ -5487,19 +5478,19 @@
     </row>
     <row r="62" ht="31" spans="1:22">
       <c r="A62" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="D62" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="E62" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>258</v>
       </c>
       <c r="F62" s="6">
         <v>15</v>
@@ -5527,19 +5518,19 @@
     </row>
     <row r="63" ht="31" spans="1:22">
       <c r="A63" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="D63" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="E63" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>258</v>
       </c>
       <c r="F63" s="6">
         <v>50</v>
@@ -5551,37 +5542,37 @@
         <v>54.2</v>
       </c>
       <c r="I63" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K63" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="J63" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K63" s="3" t="s">
+      <c r="L63" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="L63" s="3" t="s">
+      <c r="M63" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="M63" s="3" t="s">
+      <c r="N63" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O63" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="N63" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O63" s="3" t="s">
+      <c r="P63" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="P63" s="3" t="s">
+      <c r="Q63" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="R63" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="Q63" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="R63" s="3" t="s">
+      <c r="S63" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="S63" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
@@ -5589,19 +5580,19 @@
     </row>
     <row r="64" ht="31" spans="1:22">
       <c r="A64" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="D64" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="E64" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>258</v>
       </c>
       <c r="F64" s="6">
         <v>100</v>
@@ -5613,37 +5604,37 @@
         <v>56</v>
       </c>
       <c r="I64" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="L64" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="J64" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K64" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="L64" s="3" t="s">
+      <c r="M64" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="N64" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O64" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="M64" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="N64" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O64" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="P64" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q64" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="R64" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="Q64" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="R64" s="3" t="s">
+      <c r="S64" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="S64" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
@@ -5651,26 +5642,26 @@
     </row>
     <row r="65" ht="31" spans="1:22">
       <c r="A65" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="D65" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="E65" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>258</v>
       </c>
       <c r="F65" s="6">
         <v>50</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
@@ -5689,19 +5680,19 @@
     </row>
     <row r="66" ht="46" spans="1:22">
       <c r="A66" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="C66" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="D66" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="E66" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F66" s="6">
         <v>15</v>
@@ -5713,37 +5704,37 @@
         <v>26.8</v>
       </c>
       <c r="I66" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J66" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="J66" s="3" t="s">
+      <c r="K66" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="K66" s="3" t="s">
+      <c r="L66" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M66" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="L66" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="M66" s="3" t="s">
+      <c r="N66" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O66" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="N66" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O66" s="3" t="s">
+      <c r="P66" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q66" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R66" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="P66" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q66" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R66" s="3" t="s">
-        <v>288</v>
-      </c>
       <c r="S66" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
@@ -5751,19 +5742,19 @@
     </row>
     <row r="67" ht="46" spans="1:22">
       <c r="A67" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="C67" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="D67" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="E67" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F67" s="6">
         <v>50</v>
@@ -5775,37 +5766,37 @@
         <v>27</v>
       </c>
       <c r="I67" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L67" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M67" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="J67" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="L67" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="M67" s="3" t="s">
+      <c r="N67" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O67" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="N67" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O67" s="3" t="s">
-        <v>291</v>
-      </c>
       <c r="P67" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q67" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Q67" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="R67" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
@@ -5813,19 +5804,19 @@
     </row>
     <row r="68" ht="46" spans="1:22">
       <c r="A68" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C68" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="D68" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="E68" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F68" s="6">
         <v>100</v>
@@ -5837,37 +5828,37 @@
         <v>29.3</v>
       </c>
       <c r="I68" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="J68" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="J68" s="3" t="s">
+      <c r="K68" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="L68" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M68" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N68" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="O68" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="K68" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="L68" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M68" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="N68" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="O68" s="3" t="s">
+      <c r="P68" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="S68" s="3" t="s">
         <v>294</v>
-      </c>
-      <c r="P68" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q68" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="R68" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="S68" s="3" t="s">
-        <v>295</v>
       </c>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
@@ -5875,19 +5866,19 @@
     </row>
     <row r="69" ht="46" spans="1:22">
       <c r="A69" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="D69" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="E69" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F69" s="6">
         <v>15</v>
@@ -5899,37 +5890,37 @@
         <v>42.4</v>
       </c>
       <c r="I69" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L69" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M69" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="J69" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="L69" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="M69" s="3" t="s">
+      <c r="N69" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="O69" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="N69" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="O69" s="3" t="s">
+      <c r="P69" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q69" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="R69" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="P69" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q69" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="R69" s="3" t="s">
-        <v>300</v>
-      </c>
       <c r="S69" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
@@ -5937,19 +5928,19 @@
     </row>
     <row r="70" ht="46" spans="1:22">
       <c r="A70" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="E70" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F70" s="6">
         <v>50</v>
@@ -5961,37 +5952,37 @@
         <v>50.6</v>
       </c>
       <c r="I70" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="J70" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="J70" s="3" t="s">
+      <c r="K70" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="K70" s="3" t="s">
+      <c r="L70" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="L70" s="3" t="s">
+      <c r="M70" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="M70" s="3" t="s">
+      <c r="N70" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="O70" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="N70" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="O70" s="3" t="s">
+      <c r="P70" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="P70" s="3" t="s">
+      <c r="Q70" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="Q70" s="3" t="s">
+      <c r="R70" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="R70" s="3" t="s">
-        <v>309</v>
-      </c>
       <c r="S70" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
@@ -5999,19 +5990,19 @@
     </row>
     <row r="71" ht="46" spans="1:22">
       <c r="A71" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="D71" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>282</v>
-      </c>
       <c r="E71" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F71" s="6">
         <v>100</v>
@@ -6023,37 +6014,37 @@
         <v>51</v>
       </c>
       <c r="I71" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="J71" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="J71" s="3" t="s">
+      <c r="K71" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="L71" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="K71" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="L71" s="3" t="s">
+      <c r="M71" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="M71" s="3" t="s">
+      <c r="N71" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O71" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="N71" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="O71" s="3" t="s">
+      <c r="P71" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q71" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="R71" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="P71" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q71" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="R71" s="3" t="s">
+      <c r="S71" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="S71" s="3" t="s">
-        <v>316</v>
       </c>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
@@ -6061,19 +6052,19 @@
     </row>
     <row r="72" ht="92" spans="1:22">
       <c r="A72" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="C72" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="D72" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>320</v>
-      </c>
       <c r="E72" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F72" s="6">
         <v>50</v>
@@ -6085,37 +6076,37 @@
         <v>48.59</v>
       </c>
       <c r="I72" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="M72" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="N72" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="J72" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K72" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="L72" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="M72" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="N72" s="3" t="s">
+      <c r="O72" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="O72" s="3" t="s">
+      <c r="P72" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q72" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="P72" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q72" s="3" t="s">
+      <c r="R72" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="R72" s="3" t="s">
-        <v>325</v>
-      </c>
       <c r="S72" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
@@ -6123,19 +6114,19 @@
     </row>
     <row r="73" ht="92" spans="1:22">
       <c r="A73" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C73" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="D73" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>320</v>
-      </c>
       <c r="E73" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F73" s="6">
         <v>100</v>
@@ -6147,37 +6138,37 @@
         <v>53.1</v>
       </c>
       <c r="I73" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="M73" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N73" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="O73" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="J73" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="L73" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="M73" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="N73" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="O73" s="3" t="s">
+      <c r="P73" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q73" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="R73" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="P73" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q73" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="R73" s="3" t="s">
-        <v>328</v>
-      </c>
       <c r="S73" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
@@ -6185,26 +6176,26 @@
     </row>
     <row r="74" ht="46" spans="1:22">
       <c r="A74" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C74" s="4" t="s">
+      <c r="D74" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="E74" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F74" s="6">
         <v>15</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
@@ -6223,26 +6214,26 @@
     </row>
     <row r="75" ht="46" spans="1:22">
       <c r="A75" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C75" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C75" s="4" t="s">
+      <c r="D75" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>331</v>
-      </c>
       <c r="E75" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F75" s="6">
         <v>100</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with the latest verified data to ensure accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="401">
   <si>
     <t>Model</t>
   </si>
@@ -524,6 +524,30 @@
     <t>Specialized model</t>
   </si>
   <si>
+    <t>92.50/359</t>
+  </si>
+  <si>
+    <t>10.92/45</t>
+  </si>
+  <si>
+    <t>15.00/26</t>
+  </si>
+  <si>
+    <t>6.00/47</t>
+  </si>
+  <si>
+    <t>5.00/93</t>
+  </si>
+  <si>
+    <t>8.00/23</t>
+  </si>
+  <si>
+    <t>5.62/17</t>
+  </si>
+  <si>
+    <t>15.00/23</t>
+  </si>
+  <si>
     <t>83.87/360</t>
   </si>
   <si>
@@ -533,7 +557,61 @@
     <t>2.00/93</t>
   </si>
   <si>
-    <t>8.00/23</t>
+    <t>90.04/359</t>
+  </si>
+  <si>
+    <t>12.96/45</t>
+  </si>
+  <si>
+    <t>9.09/93</t>
+  </si>
+  <si>
+    <t>6.00/24</t>
+  </si>
+  <si>
+    <t>3.00/16</t>
+  </si>
+  <si>
+    <t>105.60/359</t>
+  </si>
+  <si>
+    <t>16.92/46</t>
+  </si>
+  <si>
+    <t>6.91/93</t>
+  </si>
+  <si>
+    <t>4.81/16</t>
+  </si>
+  <si>
+    <t>90.97/358</t>
+  </si>
+  <si>
+    <t>16.00/45</t>
+  </si>
+  <si>
+    <t>8.01/91</t>
+  </si>
+  <si>
+    <t>7.00/24</t>
+  </si>
+  <si>
+    <t>6.00/15</t>
+  </si>
+  <si>
+    <t>106.95/361</t>
+  </si>
+  <si>
+    <t>18.92/46</t>
+  </si>
+  <si>
+    <t>18.96/47</t>
+  </si>
+  <si>
+    <t>8.45/93</t>
+  </si>
+  <si>
+    <t>4.63/17</t>
   </si>
   <si>
     <t>uitars-72b-dpo</t>
@@ -560,18 +638,12 @@
     <t>4.58/93</t>
   </si>
   <si>
-    <t>6.00/15</t>
-  </si>
-  <si>
     <t>93.16/360</t>
   </si>
   <si>
     <t>14.96/45</t>
   </si>
   <si>
-    <t>6.00/47</t>
-  </si>
-  <si>
     <t>6.24/93</t>
   </si>
   <si>
@@ -617,9 +689,6 @@
     <t>8.99/47</t>
   </si>
   <si>
-    <t>5.00/93</t>
-  </si>
-  <si>
     <t>4.00/24</t>
   </si>
   <si>
@@ -680,9 +749,6 @@
     <t>6.09/92</t>
   </si>
   <si>
-    <t>6.00/24</t>
-  </si>
-  <si>
     <t>opencua-7b</t>
   </si>
   <si>
@@ -710,9 +776,171 @@
     <t>8.73/93</t>
   </si>
   <si>
+    <t>104.14/361</t>
+  </si>
+  <si>
+    <t>6.79/47</t>
+  </si>
+  <si>
+    <t>13.04/47</t>
+  </si>
+  <si>
+    <t>13.35/93</t>
+  </si>
+  <si>
+    <t>99.05/357</t>
+  </si>
+  <si>
+    <t>17.96/45</t>
+  </si>
+  <si>
+    <t>8.69/93</t>
+  </si>
+  <si>
+    <t>10.00/22</t>
+  </si>
+  <si>
+    <t>5.44/17</t>
+  </si>
+  <si>
+    <t>11.00/22</t>
+  </si>
+  <si>
+    <t>100.25/358</t>
+  </si>
+  <si>
+    <t>6.71/46</t>
+  </si>
+  <si>
+    <t>15.96/47</t>
+  </si>
+  <si>
+    <t>11.62/92</t>
+  </si>
+  <si>
+    <t>97.57/359</t>
+  </si>
+  <si>
+    <t>15.99/47</t>
+  </si>
+  <si>
+    <t>8.62/92</t>
+  </si>
+  <si>
+    <t>94.08/361</t>
+  </si>
+  <si>
+    <t>12.99/47</t>
+  </si>
+  <si>
+    <t>10.13/93</t>
+  </si>
+  <si>
+    <t>10.00/24</t>
+  </si>
+  <si>
+    <t>95.65/360</t>
+  </si>
+  <si>
+    <t>13.96/46</t>
+  </si>
+  <si>
+    <t>16.00/47</t>
+  </si>
+  <si>
     <t>opencua-32b</t>
   </si>
   <si>
+    <t>100.42/357</t>
+  </si>
+  <si>
+    <t>13.99/46</t>
+  </si>
+  <si>
+    <t>9.58/92</t>
+  </si>
+  <si>
+    <t>3.89/17</t>
+  </si>
+  <si>
+    <t>109.80/360</t>
+  </si>
+  <si>
+    <t>20.96/46</t>
+  </si>
+  <si>
+    <t>4.88/17</t>
+  </si>
+  <si>
+    <t>109.34/360</t>
+  </si>
+  <si>
+    <t>14.04/47</t>
+  </si>
+  <si>
+    <t>8.35/93</t>
+  </si>
+  <si>
+    <t>121.57/360</t>
+  </si>
+  <si>
+    <t>19.96/46</t>
+  </si>
+  <si>
+    <t>17.99/47</t>
+  </si>
+  <si>
+    <t>15.62/93</t>
+  </si>
+  <si>
+    <t>120.31/359</t>
+  </si>
+  <si>
+    <t>18.00/26</t>
+  </si>
+  <si>
+    <t>12.35/92</t>
+  </si>
+  <si>
+    <t>126.49/360</t>
+  </si>
+  <si>
+    <t>17.00/26</t>
+  </si>
+  <si>
+    <t>19.99/47</t>
+  </si>
+  <si>
+    <t>13.54/93</t>
+  </si>
+  <si>
+    <t>121.83/360</t>
+  </si>
+  <si>
+    <t>15.96/46</t>
+  </si>
+  <si>
+    <t>15.04/47</t>
+  </si>
+  <si>
+    <t>16.83/93</t>
+  </si>
+  <si>
+    <t>125.22/360</t>
+  </si>
+  <si>
+    <t>16.27/93</t>
+  </si>
+  <si>
+    <t>127.95/358</t>
+  </si>
+  <si>
+    <t>12.00/92</t>
+  </si>
+  <si>
+    <t>15.00/22</t>
+  </si>
+  <si>
     <t>qwen2.5-vl-32b-instruct</t>
   </si>
   <si>
@@ -806,12 +1034,6 @@
     <t>168.84/369</t>
   </si>
   <si>
-    <t>20.96/46</t>
-  </si>
-  <si>
-    <t>17.00/26</t>
-  </si>
-  <si>
     <t>21.00/47</t>
   </si>
   <si>
@@ -881,9 +1103,6 @@
     <t>13.96/45</t>
   </si>
   <si>
-    <t>18.00/26</t>
-  </si>
-  <si>
     <t>6.96/47</t>
   </si>
   <si>
@@ -905,22 +1124,13 @@
     <t>105.80/361</t>
   </si>
   <si>
-    <t>13.96/46</t>
-  </si>
-  <si>
     <t>12.85/93</t>
   </si>
   <si>
-    <t>15.00/23</t>
-  </si>
-  <si>
     <t>Jedi-7B w/ o3</t>
   </si>
   <si>
     <t>152.95/361</t>
-  </si>
-  <si>
-    <t>19.99/47</t>
   </si>
   <si>
     <t>19.00/93</t>
@@ -2218,8 +2428,8 @@
   </sheetPr>
   <dimension ref="A1:AC1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="I30" workbookViewId="0">
-      <selection activeCell="W43" sqref="W43"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -3465,17 +3675,39 @@
       <c r="H21" s="6">
         <v>25.7</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="T21" s="11"/>
       <c r="U21" s="11"/>
       <c r="V21" s="11"/>
@@ -3506,10 +3738,10 @@
         <v>23.3</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>55</v>
@@ -3524,10 +3756,10 @@
         <v>94</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>92</v>
@@ -3567,17 +3799,39 @@
       <c r="H23" s="6">
         <v>25.1</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="T23" s="11"/>
       <c r="U23" s="11"/>
       <c r="V23" s="11"/>
@@ -3607,17 +3861,39 @@
       <c r="H24" s="6">
         <v>29.4</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
+      <c r="I24" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="T24" s="11"/>
       <c r="U24" s="11"/>
       <c r="V24" s="11"/>
@@ -3647,17 +3923,39 @@
       <c r="H25" s="6">
         <v>25.2</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="T25" s="11"/>
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
@@ -3687,33 +3985,55 @@
       <c r="H26" s="6">
         <v>29.6</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
+      <c r="I26" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="T26" s="11"/>
       <c r="U26" s="11"/>
       <c r="V26" s="11"/>
     </row>
     <row r="27" ht="16.75" customHeight="1" spans="1:22">
       <c r="A27" s="3" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>164</v>
@@ -3728,16 +4048,16 @@
         <v>24</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>56</v>
@@ -3746,13 +4066,13 @@
         <v>29</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="P27" s="3" t="s">
         <v>155</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="R27" s="3" t="s">
         <v>149</v>
@@ -3766,16 +4086,16 @@
     </row>
     <row r="28" ht="16.75" customHeight="1" spans="1:22">
       <c r="A28" s="3" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>164</v>
@@ -3790,16 +4110,16 @@
         <v>25.8</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>28</v>
@@ -3808,7 +4128,7 @@
         <v>103</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="P28" s="3" t="s">
         <v>155</v>
@@ -3828,16 +4148,16 @@
     </row>
     <row r="29" ht="16.75" customHeight="1" spans="1:22">
       <c r="A29" s="3" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>161</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>164</v>
@@ -3852,25 +4172,25 @@
         <v>27.1</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="P29" s="3" t="s">
         <v>76</v>
@@ -3890,16 +4210,16 @@
     </row>
     <row r="30" ht="16.75" customHeight="1" spans="1:22">
       <c r="A30" s="3" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>164</v>
@@ -3914,28 +4234,28 @@
         <v>16.9</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>82</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="N30" s="3" t="s">
         <v>85</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="Q30" s="3" t="s">
         <v>86</v>
@@ -3944,7 +4264,7 @@
         <v>109</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="T30" s="11"/>
       <c r="U30" s="11"/>
@@ -3952,16 +4272,16 @@
     </row>
     <row r="31" ht="16.75" customHeight="1" spans="1:22">
       <c r="A31" s="3" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>164</v>
@@ -3976,25 +4296,25 @@
         <v>19.9</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>145</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="P31" s="3" t="s">
         <v>76</v>
@@ -4014,16 +4334,16 @@
     </row>
     <row r="32" ht="16.75" customHeight="1" spans="1:22">
       <c r="A32" s="3" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>164</v>
@@ -4038,28 +4358,28 @@
         <v>17.7</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>145</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="N32" s="3" t="s">
         <v>57</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
       <c r="Q32" s="3" t="s">
         <v>86</v>
@@ -4076,16 +4396,16 @@
     </row>
     <row r="33" ht="16.75" customHeight="1" spans="1:22">
       <c r="A33" s="3" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>164</v>
@@ -4100,10 +4420,10 @@
         <v>19.9</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>82</v>
@@ -4112,19 +4432,19 @@
         <v>83</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="R33" s="3" t="s">
         <v>33</v>
@@ -4138,16 +4458,16 @@
     </row>
     <row r="34" ht="16.75" customHeight="1" spans="1:22">
       <c r="A34" s="3" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>164</v>
@@ -4162,16 +4482,16 @@
         <v>20.6</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="M34" s="3" t="s">
         <v>56</v>
@@ -4180,10 +4500,10 @@
         <v>103</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="Q34" s="3" t="s">
         <v>32</v>
@@ -4200,16 +4520,16 @@
     </row>
     <row r="35" ht="16.75" customHeight="1" spans="1:22">
       <c r="A35" s="3" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>164</v>
@@ -4224,10 +4544,10 @@
         <v>23.1</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>215</v>
+        <v>238</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="K35" s="3" t="s">
         <v>82</v>
@@ -4242,10 +4562,10 @@
         <v>103</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="Q35" s="3" t="s">
         <v>101</v>
@@ -4262,16 +4582,16 @@
     </row>
     <row r="36" ht="16.75" customHeight="1" spans="1:22">
       <c r="A36" s="3" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>164</v>
@@ -4286,7 +4606,7 @@
         <v>26.2</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>25</v>
@@ -4304,7 +4624,7 @@
         <v>38</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="P36" s="3" t="s">
         <v>29</v>
@@ -4324,16 +4644,16 @@
     </row>
     <row r="37" ht="16.75" customHeight="1" spans="1:22">
       <c r="A37" s="3" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>164</v>
@@ -4348,7 +4668,7 @@
         <v>23.6</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>45</v>
@@ -4360,19 +4680,19 @@
         <v>83</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="N37" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="P37" s="3" t="s">
         <v>103</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="R37" s="3" t="s">
         <v>149</v>
@@ -4386,16 +4706,16 @@
     </row>
     <row r="38" ht="16.75" customHeight="1" spans="1:22">
       <c r="A38" s="3" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>164</v>
@@ -4410,10 +4730,10 @@
         <v>23</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="K38" s="3" t="s">
         <v>82</v>
@@ -4422,19 +4742,19 @@
         <v>83</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="N38" s="3" t="s">
         <v>85</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="R38" s="3" t="s">
         <v>109</v>
@@ -4448,16 +4768,16 @@
     </row>
     <row r="39" ht="16.75" customHeight="1" spans="1:22">
       <c r="A39" s="3" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>164</v>
@@ -4471,33 +4791,55 @@
       <c r="H39" s="6">
         <v>28.8</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
+      <c r="I39" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="O39" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="P39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="T39" s="11"/>
       <c r="U39" s="11"/>
       <c r="V39" s="11"/>
     </row>
     <row r="40" ht="16.75" customHeight="1" spans="1:22">
       <c r="A40" s="3" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>164</v>
@@ -4511,33 +4853,55 @@
       <c r="H40" s="6">
         <v>27.7</v>
       </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
+      <c r="I40" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>258</v>
+      </c>
       <c r="T40" s="11"/>
       <c r="U40" s="11"/>
       <c r="V40" s="11"/>
     </row>
     <row r="41" ht="16.75" customHeight="1" spans="1:22">
       <c r="A41" s="3" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>164</v>
@@ -4549,35 +4913,57 @@
         <v>45866</v>
       </c>
       <c r="H41" s="6">
-        <v>27.2</v>
-      </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S41" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="T41" s="11"/>
       <c r="U41" s="11"/>
       <c r="V41" s="11"/>
     </row>
     <row r="42" ht="16.75" customHeight="1" spans="1:22">
       <c r="A42" s="3" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>164</v>
@@ -4591,33 +4977,55 @@
       <c r="H42" s="6">
         <v>27.2</v>
       </c>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
+      <c r="I42" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="T42" s="11"/>
       <c r="U42" s="11"/>
       <c r="V42" s="11"/>
     </row>
     <row r="43" ht="16.75" customHeight="1" spans="1:22">
       <c r="A43" s="3" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>164</v>
@@ -4631,33 +5039,55 @@
       <c r="H43" s="6">
         <v>26.1</v>
       </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
+      <c r="I43" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="P43" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S43" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="T43" s="11"/>
       <c r="U43" s="11"/>
       <c r="V43" s="11"/>
     </row>
     <row r="44" ht="16.75" customHeight="1" spans="1:22">
       <c r="A44" s="3" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E44" s="9" t="s">
         <v>164</v>
@@ -4671,33 +5101,55 @@
       <c r="H44" s="6">
         <v>26.6</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
+      <c r="I44" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O44" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="P44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="T44" s="11"/>
       <c r="U44" s="11"/>
       <c r="V44" s="11"/>
     </row>
     <row r="45" ht="16.75" customHeight="1" spans="1:22">
       <c r="A45" s="3" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E45" s="9" t="s">
         <v>164</v>
@@ -4711,33 +5163,55 @@
       <c r="H45" s="6">
         <v>28.1</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
+      <c r="I45" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R45" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>256</v>
+      </c>
       <c r="T45" s="11"/>
       <c r="U45" s="11"/>
       <c r="V45" s="11"/>
     </row>
     <row r="46" ht="16.75" customHeight="1" spans="1:22">
       <c r="A46" s="3" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>164</v>
@@ -4751,33 +5225,55 @@
       <c r="H46" s="6">
         <v>30.5</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
+      <c r="I46" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="P46" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="T46" s="11"/>
       <c r="U46" s="11"/>
       <c r="V46" s="11"/>
     </row>
     <row r="47" ht="16.75" customHeight="1" spans="1:22">
       <c r="A47" s="3" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E47" s="9" t="s">
         <v>164</v>
@@ -4791,33 +5287,55 @@
       <c r="H47" s="6">
         <v>30.4</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3"/>
-      <c r="S47" s="3"/>
+      <c r="I47" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="P47" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q47" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R47" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="S47" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="T47" s="11"/>
       <c r="U47" s="11"/>
       <c r="V47" s="11"/>
     </row>
     <row r="48" ht="16.75" customHeight="1" spans="1:22">
       <c r="A48" s="3" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E48" s="9" t="s">
         <v>164</v>
@@ -4831,33 +5349,55 @@
       <c r="H48" s="6">
         <v>33.8</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
+      <c r="I48" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="P48" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="T48" s="11"/>
       <c r="U48" s="11"/>
       <c r="V48" s="11"/>
     </row>
     <row r="49" ht="16.75" customHeight="1" spans="1:22">
       <c r="A49" s="3" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>164</v>
@@ -4871,33 +5411,55 @@
       <c r="H49" s="6">
         <v>33.5</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
+      <c r="I49" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S49" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="T49" s="11"/>
       <c r="U49" s="11"/>
       <c r="V49" s="11"/>
     </row>
     <row r="50" ht="16.75" customHeight="1" spans="1:22">
       <c r="A50" s="3" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>164</v>
@@ -4911,33 +5473,55 @@
       <c r="H50" s="6">
         <v>35.1</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
+      <c r="I50" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="N50" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="P50" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q50" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="T50" s="11"/>
       <c r="U50" s="11"/>
       <c r="V50" s="11"/>
     </row>
     <row r="51" ht="16.75" customHeight="1" spans="1:22">
       <c r="A51" s="3" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>164</v>
@@ -4951,33 +5535,55 @@
       <c r="H51" s="6">
         <v>33.8</v>
       </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
+      <c r="I51" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="P51" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q51" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R51" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="S51" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="T51" s="11"/>
       <c r="U51" s="11"/>
       <c r="V51" s="11"/>
     </row>
     <row r="52" ht="16.75" customHeight="1" spans="1:22">
       <c r="A52" s="3" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>164</v>
@@ -4991,33 +5597,55 @@
       <c r="H52" s="6">
         <v>35.7</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
+      <c r="I52" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="T52" s="11"/>
       <c r="U52" s="11"/>
       <c r="V52" s="11"/>
     </row>
     <row r="53" ht="16.75" customHeight="1" spans="1:22">
       <c r="A53" s="3" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>164</v>
@@ -5031,33 +5659,55 @@
       <c r="H53" s="6">
         <v>34.8</v>
       </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
-      <c r="R53" s="3"/>
-      <c r="S53" s="3"/>
+      <c r="I53" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q53" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R53" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="S53" s="3" t="s">
+        <v>303</v>
+      </c>
       <c r="T53" s="11"/>
       <c r="U53" s="11"/>
       <c r="V53" s="11"/>
     </row>
     <row r="54" ht="16.75" customHeight="1" spans="1:22">
       <c r="A54" s="3" t="s">
-        <v>228</v>
+        <v>304</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>230</v>
+        <v>306</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>231</v>
+        <v>307</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>69</v>
@@ -5072,37 +5722,37 @@
         <v>3.04</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>232</v>
+        <v>308</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>233</v>
+        <v>309</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>73</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>234</v>
+        <v>310</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>235</v>
+        <v>311</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>236</v>
+        <v>312</v>
       </c>
       <c r="Q54" s="3" t="s">
-        <v>237</v>
+        <v>313</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>238</v>
+        <v>314</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>239</v>
+        <v>315</v>
       </c>
       <c r="T54" s="11"/>
       <c r="U54" s="11"/>
@@ -5110,16 +5760,16 @@
     </row>
     <row r="55" ht="16.75" customHeight="1" spans="1:22">
       <c r="A55" s="3" t="s">
-        <v>228</v>
+        <v>304</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>230</v>
+        <v>306</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>231</v>
+        <v>307</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>69</v>
@@ -5134,13 +5784,13 @@
         <v>3.88</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>240</v>
+        <v>316</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>233</v>
+        <v>309</v>
       </c>
       <c r="L55" s="3" t="s">
         <v>73</v>
@@ -5149,22 +5799,22 @@
         <v>73</v>
       </c>
       <c r="N55" s="3" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="P55" s="3" t="s">
-        <v>236</v>
+        <v>312</v>
       </c>
       <c r="Q55" s="3" t="s">
         <v>77</v>
       </c>
       <c r="R55" s="3" t="s">
-        <v>238</v>
+        <v>314</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="T55" s="11"/>
       <c r="U55" s="11"/>
@@ -5172,16 +5822,16 @@
     </row>
     <row r="56" ht="16.75" customHeight="1" spans="1:22">
       <c r="A56" s="3" t="s">
-        <v>241</v>
+        <v>317</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>230</v>
+        <v>306</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>231</v>
+        <v>307</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>69</v>
@@ -5196,13 +5846,13 @@
         <v>4.43</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>242</v>
+        <v>318</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>243</v>
+        <v>319</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>244</v>
+        <v>320</v>
       </c>
       <c r="L56" s="3" t="s">
         <v>84</v>
@@ -5214,19 +5864,19 @@
         <v>74</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>236</v>
+        <v>312</v>
       </c>
       <c r="Q56" s="3" t="s">
-        <v>245</v>
+        <v>321</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>246</v>
+        <v>322</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>239</v>
+        <v>315</v>
       </c>
       <c r="T56" s="11"/>
       <c r="U56" s="11"/>
@@ -5234,16 +5884,16 @@
     </row>
     <row r="57" ht="16.75" customHeight="1" spans="1:22">
       <c r="A57" s="3" t="s">
-        <v>241</v>
+        <v>317</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>230</v>
+        <v>306</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>231</v>
+        <v>307</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>69</v>
@@ -5258,34 +5908,34 @@
         <v>5</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>247</v>
+        <v>323</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>248</v>
+        <v>324</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>244</v>
+        <v>320</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="M57" s="3" t="s">
         <v>73</v>
       </c>
       <c r="N57" s="3" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>237</v>
+        <v>313</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>246</v>
+        <v>322</v>
       </c>
       <c r="S57" s="3" t="s">
         <v>74</v>
@@ -5296,16 +5946,16 @@
     </row>
     <row r="58" ht="16.75" customHeight="1" spans="1:22">
       <c r="A58" s="3" t="s">
-        <v>249</v>
+        <v>325</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>250</v>
+        <v>326</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>251</v>
+        <v>327</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>252</v>
+        <v>328</v>
       </c>
       <c r="E58" s="8" t="s">
         <v>69</v>
@@ -5336,16 +5986,16 @@
     </row>
     <row r="59" ht="16.75" customHeight="1" spans="1:22">
       <c r="A59" s="3" t="s">
-        <v>249</v>
+        <v>325</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>250</v>
+        <v>326</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>251</v>
+        <v>327</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>252</v>
+        <v>328</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>69</v>
@@ -5376,19 +6026,19 @@
     </row>
     <row r="60" ht="31" spans="1:22">
       <c r="A60" s="3" t="s">
-        <v>253</v>
+        <v>329</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>255</v>
+        <v>331</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F60" s="6">
         <v>15</v>
@@ -5416,19 +6066,19 @@
     </row>
     <row r="61" ht="31" spans="1:22">
       <c r="A61" s="3" t="s">
-        <v>253</v>
+        <v>329</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>255</v>
+        <v>331</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F61" s="6">
         <v>50</v>
@@ -5440,16 +6090,16 @@
         <v>45.76</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>258</v>
+        <v>334</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>260</v>
+        <v>292</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>261</v>
+        <v>335</v>
       </c>
       <c r="M61" s="3" t="s">
         <v>107</v>
@@ -5458,7 +6108,7 @@
         <v>43</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>262</v>
+        <v>336</v>
       </c>
       <c r="P61" s="3" t="s">
         <v>91</v>
@@ -5467,7 +6117,7 @@
         <v>41</v>
       </c>
       <c r="R61" s="3" t="s">
-        <v>263</v>
+        <v>337</v>
       </c>
       <c r="S61" s="3" t="s">
         <v>43</v>
@@ -5478,19 +6128,19 @@
     </row>
     <row r="62" ht="31" spans="1:22">
       <c r="A62" s="3" t="s">
-        <v>264</v>
+        <v>338</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>255</v>
+        <v>331</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F62" s="6">
         <v>15</v>
@@ -5518,19 +6168,19 @@
     </row>
     <row r="63" ht="31" spans="1:22">
       <c r="A63" s="3" t="s">
-        <v>264</v>
+        <v>338</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>255</v>
+        <v>331</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F63" s="6">
         <v>50</v>
@@ -5542,37 +6192,37 @@
         <v>54.2</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>265</v>
+        <v>339</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>105</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>266</v>
+        <v>340</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>267</v>
+        <v>341</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>268</v>
+        <v>342</v>
       </c>
       <c r="N63" s="3" t="s">
         <v>34</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>269</v>
+        <v>343</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>270</v>
+        <v>344</v>
       </c>
       <c r="Q63" s="3" t="s">
         <v>127</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>271</v>
+        <v>345</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>272</v>
+        <v>346</v>
       </c>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
@@ -5580,19 +6230,19 @@
     </row>
     <row r="64" ht="31" spans="1:22">
       <c r="A64" s="3" t="s">
-        <v>264</v>
+        <v>338</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>255</v>
+        <v>331</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F64" s="6">
         <v>100</v>
@@ -5604,37 +6254,37 @@
         <v>56</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>273</v>
+        <v>347</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>105</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>266</v>
+        <v>340</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>274</v>
+        <v>348</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>268</v>
+        <v>342</v>
       </c>
       <c r="N64" s="3" t="s">
         <v>34</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>275</v>
+        <v>349</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>270</v>
+        <v>344</v>
       </c>
       <c r="Q64" s="3" t="s">
         <v>127</v>
       </c>
       <c r="R64" s="3" t="s">
-        <v>271</v>
+        <v>345</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>272</v>
+        <v>346</v>
       </c>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
@@ -5642,26 +6292,26 @@
     </row>
     <row r="65" ht="31" spans="1:22">
       <c r="A65" s="3" t="s">
-        <v>276</v>
+        <v>350</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>254</v>
+        <v>330</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>255</v>
+        <v>331</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>256</v>
+        <v>332</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F65" s="6">
         <v>50</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3" t="s">
-        <v>277</v>
+        <v>351</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
@@ -5680,19 +6330,19 @@
     </row>
     <row r="66" ht="46" spans="1:22">
       <c r="A66" s="3" t="s">
-        <v>278</v>
+        <v>352</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>280</v>
+        <v>354</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F66" s="6">
         <v>15</v>
@@ -5704,25 +6354,25 @@
         <v>26.8</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>282</v>
+        <v>356</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>283</v>
+        <v>357</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>285</v>
+        <v>358</v>
       </c>
       <c r="N66" s="3" t="s">
         <v>34</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>286</v>
+        <v>359</v>
       </c>
       <c r="P66" s="3" t="s">
         <v>31</v>
@@ -5731,7 +6381,7 @@
         <v>60</v>
       </c>
       <c r="R66" s="3" t="s">
-        <v>287</v>
+        <v>360</v>
       </c>
       <c r="S66" s="3" t="s">
         <v>133</v>
@@ -5742,19 +6392,19 @@
     </row>
     <row r="67" ht="46" spans="1:22">
       <c r="A67" s="3" t="s">
-        <v>278</v>
+        <v>352</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>280</v>
+        <v>354</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F67" s="6">
         <v>50</v>
@@ -5766,25 +6416,25 @@
         <v>27</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>288</v>
+        <v>361</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>289</v>
+        <v>362</v>
       </c>
       <c r="N67" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>290</v>
+        <v>363</v>
       </c>
       <c r="P67" s="3" t="s">
         <v>31</v>
@@ -5793,7 +6443,7 @@
         <v>32</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>287</v>
+        <v>360</v>
       </c>
       <c r="S67" s="3" t="s">
         <v>34</v>
@@ -5804,19 +6454,19 @@
     </row>
     <row r="68" ht="46" spans="1:22">
       <c r="A68" s="3" t="s">
-        <v>278</v>
+        <v>352</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>280</v>
+        <v>354</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F68" s="6">
         <v>100</v>
@@ -5828,13 +6478,13 @@
         <v>29.3</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>291</v>
+        <v>364</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>266</v>
+        <v>340</v>
       </c>
       <c r="L68" s="3" t="s">
         <v>83</v>
@@ -5843,10 +6493,10 @@
         <v>120</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>293</v>
+        <v>365</v>
       </c>
       <c r="P68" s="3" t="s">
         <v>59</v>
@@ -5858,7 +6508,7 @@
         <v>149</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>294</v>
+        <v>172</v>
       </c>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
@@ -5866,19 +6516,19 @@
     </row>
     <row r="69" ht="46" spans="1:22">
       <c r="A69" s="3" t="s">
-        <v>295</v>
+        <v>366</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>280</v>
+        <v>354</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F69" s="6">
         <v>15</v>
@@ -5890,25 +6540,25 @@
         <v>42.4</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>296</v>
+        <v>367</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>105</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>260</v>
+        <v>292</v>
       </c>
       <c r="L69" s="3" t="s">
         <v>131</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="N69" s="3" t="s">
-        <v>294</v>
+        <v>172</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>298</v>
+        <v>368</v>
       </c>
       <c r="P69" s="3" t="s">
         <v>59</v>
@@ -5917,7 +6567,7 @@
         <v>127</v>
       </c>
       <c r="R69" s="3" t="s">
-        <v>299</v>
+        <v>369</v>
       </c>
       <c r="S69" s="3" t="s">
         <v>110</v>
@@ -5928,19 +6578,19 @@
     </row>
     <row r="70" ht="46" spans="1:22">
       <c r="A70" s="3" t="s">
-        <v>295</v>
+        <v>366</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>280</v>
+        <v>354</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F70" s="6">
         <v>50</v>
@@ -5952,34 +6602,34 @@
         <v>50.6</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>300</v>
+        <v>370</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>301</v>
+        <v>371</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>302</v>
+        <v>372</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>303</v>
+        <v>373</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>304</v>
+        <v>374</v>
       </c>
       <c r="N70" s="3" t="s">
-        <v>294</v>
+        <v>172</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>305</v>
+        <v>375</v>
       </c>
       <c r="P70" s="3" t="s">
-        <v>306</v>
+        <v>376</v>
       </c>
       <c r="Q70" s="3" t="s">
-        <v>307</v>
+        <v>377</v>
       </c>
       <c r="R70" s="3" t="s">
-        <v>308</v>
+        <v>378</v>
       </c>
       <c r="S70" s="3" t="s">
         <v>110</v>
@@ -5990,19 +6640,19 @@
     </row>
     <row r="71" ht="46" spans="1:22">
       <c r="A71" s="3" t="s">
-        <v>295</v>
+        <v>366</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>280</v>
+        <v>354</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F71" s="6">
         <v>100</v>
@@ -6014,37 +6664,37 @@
         <v>51</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>309</v>
+        <v>379</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>310</v>
+        <v>380</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>311</v>
+        <v>381</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>312</v>
+        <v>382</v>
       </c>
       <c r="N71" s="3" t="s">
         <v>110</v>
       </c>
       <c r="O71" s="3" t="s">
-        <v>313</v>
+        <v>383</v>
       </c>
       <c r="P71" s="3" t="s">
         <v>59</v>
       </c>
       <c r="Q71" s="3" t="s">
-        <v>307</v>
+        <v>377</v>
       </c>
       <c r="R71" s="3" t="s">
-        <v>314</v>
+        <v>384</v>
       </c>
       <c r="S71" s="3" t="s">
-        <v>315</v>
+        <v>385</v>
       </c>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
@@ -6052,19 +6702,19 @@
     </row>
     <row r="72" ht="92" spans="1:22">
       <c r="A72" s="3" t="s">
-        <v>316</v>
+        <v>386</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>317</v>
+        <v>387</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>318</v>
+        <v>388</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>319</v>
+        <v>389</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F72" s="6">
         <v>50</v>
@@ -6076,37 +6726,37 @@
         <v>48.59</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>320</v>
+        <v>390</v>
       </c>
       <c r="J72" s="3" t="s">
         <v>146</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>303</v>
+        <v>373</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>312</v>
+        <v>382</v>
       </c>
       <c r="N72" s="3" t="s">
-        <v>321</v>
+        <v>391</v>
       </c>
       <c r="O72" s="3" t="s">
-        <v>322</v>
+        <v>392</v>
       </c>
       <c r="P72" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q72" s="3" t="s">
-        <v>323</v>
+        <v>393</v>
       </c>
       <c r="R72" s="3" t="s">
-        <v>324</v>
+        <v>394</v>
       </c>
       <c r="S72" s="3" t="s">
-        <v>315</v>
+        <v>385</v>
       </c>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
@@ -6114,19 +6764,19 @@
     </row>
     <row r="73" ht="92" spans="1:22">
       <c r="A73" s="3" t="s">
-        <v>316</v>
+        <v>386</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>317</v>
+        <v>387</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>318</v>
+        <v>388</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>319</v>
+        <v>389</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="F73" s="6">
         <v>100</v>
@@ -6138,34 +6788,34 @@
         <v>53.1</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>325</v>
+        <v>395</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>112</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>274</v>
+        <v>348</v>
       </c>
       <c r="M73" s="3" t="s">
         <v>125</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>321</v>
+        <v>391</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>326</v>
+        <v>396</v>
       </c>
       <c r="P73" s="3" t="s">
         <v>91</v>
       </c>
       <c r="Q73" s="3" t="s">
-        <v>323</v>
+        <v>393</v>
       </c>
       <c r="R73" s="3" t="s">
-        <v>327</v>
+        <v>397</v>
       </c>
       <c r="S73" s="3" t="s">
         <v>52</v>
@@ -6176,16 +6826,16 @@
     </row>
     <row r="74" ht="46" spans="1:22">
       <c r="A74" s="3" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>329</v>
+        <v>399</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>330</v>
+        <v>400</v>
       </c>
       <c r="E74" s="9" t="s">
         <v>164</v>
@@ -6214,16 +6864,16 @@
     </row>
     <row r="75" ht="46" spans="1:22">
       <c r="A75" s="3" t="s">
-        <v>328</v>
+        <v>398</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>329</v>
+        <v>399</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>330</v>
+        <v>400</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>164</v>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with new verified data to maintain accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="422">
   <si>
     <t>Model</t>
   </si>
@@ -1221,6 +1221,69 @@
   </si>
   <si>
     <t>9.06/17</t>
+  </si>
+  <si>
+    <t>CoACT-1</t>
+  </si>
+  <si>
+    <t>Salesforce &amp; University of Southern California &amp; University of Washington</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Song et al., '25</t>
+  </si>
+  <si>
+    <t>143.71/361</t>
+  </si>
+  <si>
+    <t>14.00/46</t>
+  </si>
+  <si>
+    <t>24.00/47</t>
+  </si>
+  <si>
+    <t>22.15/93</t>
+  </si>
+  <si>
+    <t>16.00/24</t>
+  </si>
+  <si>
+    <t>9.60/17</t>
+  </si>
+  <si>
+    <t>203.55/361</t>
+  </si>
+  <si>
+    <t>32.00/47</t>
+  </si>
+  <si>
+    <t>39.40/93</t>
+  </si>
+  <si>
+    <t>11.23/17</t>
+  </si>
+  <si>
+    <t>18.00/23</t>
+  </si>
+  <si>
+    <t>216.34/361</t>
+  </si>
+  <si>
+    <t>33.00/47</t>
+  </si>
+  <si>
+    <t>23.63/47</t>
+  </si>
+  <si>
+    <t>44.52/93</t>
+  </si>
+  <si>
+    <t>219.34/361</t>
+  </si>
+  <si>
+    <t>12.23/17</t>
   </si>
   <si>
     <t>aguvis-72b</t>
@@ -2428,8 +2491,8 @@
   </sheetPr>
   <dimension ref="A1:AC1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -6824,103 +6887,319 @@
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
     </row>
-    <row r="74" ht="46" spans="1:22">
+    <row r="74" ht="92" spans="1:22">
       <c r="A74" s="3" t="s">
         <v>398</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="C74" s="4" t="s">
         <v>399</v>
       </c>
+      <c r="C74" s="3" t="s">
+        <v>400</v>
+      </c>
       <c r="D74" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>164</v>
+        <v>401</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>333</v>
       </c>
       <c r="F74" s="6">
         <v>15</v>
       </c>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
-      <c r="M74" s="3"/>
-      <c r="N74" s="3"/>
-      <c r="O74" s="3"/>
-      <c r="P74" s="3"/>
-      <c r="Q74" s="3"/>
-      <c r="R74" s="3"/>
-      <c r="S74" s="3"/>
+      <c r="G74" s="7">
+        <v>45873</v>
+      </c>
+      <c r="H74" s="6">
+        <v>39.81</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L74" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="M74" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="N74" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O74" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="P74" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="Q74" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="R74" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="S74" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
       <c r="V74" s="1"/>
     </row>
-    <row r="75" ht="46" spans="1:22">
+    <row r="75" ht="92" spans="1:22">
       <c r="A75" s="3" t="s">
         <v>398</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="C75" s="4" t="s">
         <v>399</v>
       </c>
+      <c r="C75" s="3" t="s">
+        <v>400</v>
+      </c>
       <c r="D75" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>164</v>
+        <v>401</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>333</v>
       </c>
       <c r="F75" s="6">
-        <v>100</v>
-      </c>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
-      <c r="M75" s="3"/>
-      <c r="N75" s="3"/>
-      <c r="O75" s="3"/>
-      <c r="P75" s="3"/>
-      <c r="Q75" s="3"/>
-      <c r="R75" s="3"/>
-      <c r="S75" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="G75" s="7">
+        <v>45873</v>
+      </c>
+      <c r="H75" s="6">
+        <v>56.39</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="K75" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="L75" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="M75" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N75" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="O75" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="P75" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q75" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R75" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="S75" s="3" t="s">
+        <v>412</v>
+      </c>
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
       <c r="V75" s="1"/>
     </row>
-    <row r="76" ht="15.2" spans="7:11">
-      <c r="G76" s="12"/>
-      <c r="J76" s="13"/>
-      <c r="K76" s="14"/>
-    </row>
-    <row r="77" spans="7:11">
-      <c r="G77" s="12"/>
-      <c r="J77" s="13"/>
-      <c r="K77" s="14"/>
-    </row>
-    <row r="78" spans="7:11">
-      <c r="G78" s="12"/>
-      <c r="J78" s="13"/>
-      <c r="K78" s="14"/>
-    </row>
-    <row r="79" spans="7:11">
-      <c r="G79" s="12"/>
-      <c r="J79" s="13"/>
-      <c r="K79" s="14"/>
-    </row>
-    <row r="80" spans="7:11">
+    <row r="76" ht="92" spans="1:19">
+      <c r="A76" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F76" s="6">
+        <v>100</v>
+      </c>
+      <c r="G76" s="7">
+        <v>45873</v>
+      </c>
+      <c r="H76" s="6">
+        <v>59.93</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="M76" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="N76" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="O76" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="P76" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q76" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R76" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="S76" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="77" ht="92" spans="1:19">
+      <c r="A77" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F77" s="6">
+        <v>150</v>
+      </c>
+      <c r="G77" s="7">
+        <v>45873</v>
+      </c>
+      <c r="H77" s="6">
+        <v>60.76</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="K77" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="L77" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="M77" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="N77" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="O77" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="P77" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q77" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="R77" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="S77" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="78" ht="46" spans="1:19">
+      <c r="A78" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F78" s="6">
+        <v>15</v>
+      </c>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+    </row>
+    <row r="79" ht="46" spans="1:19">
+      <c r="A79" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F79" s="6">
+        <v>100</v>
+      </c>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3"/>
+    </row>
+    <row r="80" ht="15.2" spans="7:11">
       <c r="G80" s="12"/>
       <c r="J80" s="13"/>
       <c r="K80" s="14"/>
@@ -11819,8 +12098,8 @@
     <hyperlink ref="C71" r:id="rId14" display="https://osworld-grounding.github.io/" tooltip="https://osworld-grounding.github.io/"/>
     <hyperlink ref="C72" r:id="rId15" display="https://arxiv.org/abs/2507.05791" tooltip="https://arxiv.org/abs/2507.05791"/>
     <hyperlink ref="C73" r:id="rId15" display="https://arxiv.org/abs/2507.05791" tooltip="https://arxiv.org/abs/2507.05791"/>
-    <hyperlink ref="C74" r:id="rId16" display="https://aguvis-project.github.io/" tooltip="https://aguvis-project.github.io/"/>
-    <hyperlink ref="C75" r:id="rId16" display="https://aguvis-project.github.io/" tooltip="https://aguvis-project.github.io/"/>
+    <hyperlink ref="C78" r:id="rId16" display="https://aguvis-project.github.io/" tooltip="https://aguvis-project.github.io/"/>
+    <hyperlink ref="C79" r:id="rId16" display="https://aguvis-project.github.io/" tooltip="https://aguvis-project.github.io/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with new verified data to ensure continued accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="431">
   <si>
     <t>Model</t>
   </si>
@@ -1014,6 +1014,33 @@
   </si>
   <si>
     <t>Kimi Team, '25</t>
+  </si>
+  <si>
+    <t>35.00/360</t>
+  </si>
+  <si>
+    <t>11.00/45</t>
+  </si>
+  <si>
+    <t>4.00/26</t>
+  </si>
+  <si>
+    <t>1.00/93</t>
+  </si>
+  <si>
+    <t>0.00/24</t>
+  </si>
+  <si>
+    <t>36.95/360</t>
+  </si>
+  <si>
+    <t>10.91/46</t>
+  </si>
+  <si>
+    <t>3.00/25</t>
+  </si>
+  <si>
+    <t>3.04/47</t>
   </si>
   <si>
     <t>agent s2 w/ gemini-2.5-pro</t>
@@ -2491,8 +2518,8 @@
   </sheetPr>
   <dimension ref="A1:AC1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -6032,17 +6059,39 @@
       <c r="H58" s="6">
         <v>9.7</v>
       </c>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
-      <c r="S58" s="3"/>
+      <c r="I58" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="S58" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="T58" s="11"/>
       <c r="U58" s="11"/>
       <c r="V58" s="11"/>
@@ -6072,36 +6121,58 @@
       <c r="H59" s="6">
         <v>10.3</v>
       </c>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-      <c r="Q59" s="3"/>
-      <c r="R59" s="3"/>
-      <c r="S59" s="3"/>
+      <c r="I59" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q59" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R59" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="S59" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="T59" s="11"/>
       <c r="U59" s="11"/>
       <c r="V59" s="11"/>
     </row>
     <row r="60" ht="31" spans="1:22">
       <c r="A60" s="3" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F60" s="6">
         <v>15</v>
@@ -6129,19 +6200,19 @@
     </row>
     <row r="61" ht="31" spans="1:22">
       <c r="A61" s="3" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F61" s="6">
         <v>50</v>
@@ -6153,7 +6224,7 @@
         <v>45.76</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>279</v>
@@ -6162,7 +6233,7 @@
         <v>292</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="M61" s="3" t="s">
         <v>107</v>
@@ -6171,7 +6242,7 @@
         <v>43</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="P61" s="3" t="s">
         <v>91</v>
@@ -6180,7 +6251,7 @@
         <v>41</v>
       </c>
       <c r="R61" s="3" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="S61" s="3" t="s">
         <v>43</v>
@@ -6191,19 +6262,19 @@
     </row>
     <row r="62" ht="31" spans="1:22">
       <c r="A62" s="3" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F62" s="6">
         <v>15</v>
@@ -6231,19 +6302,19 @@
     </row>
     <row r="63" ht="31" spans="1:22">
       <c r="A63" s="3" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F63" s="6">
         <v>50</v>
@@ -6255,37 +6326,37 @@
         <v>54.2</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>105</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="N63" s="3" t="s">
         <v>34</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="P63" s="3" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="Q63" s="3" t="s">
         <v>127</v>
       </c>
       <c r="R63" s="3" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
@@ -6293,19 +6364,19 @@
     </row>
     <row r="64" ht="31" spans="1:22">
       <c r="A64" s="3" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F64" s="6">
         <v>100</v>
@@ -6317,37 +6388,37 @@
         <v>56</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>105</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="N64" s="3" t="s">
         <v>34</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="P64" s="3" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="Q64" s="3" t="s">
         <v>127</v>
       </c>
       <c r="R64" s="3" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
@@ -6355,26 +6426,26 @@
     </row>
     <row r="65" ht="31" spans="1:22">
       <c r="A65" s="3" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F65" s="6">
         <v>50</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
@@ -6393,19 +6464,19 @@
     </row>
     <row r="66" ht="46" spans="1:22">
       <c r="A66" s="3" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F66" s="6">
         <v>15</v>
@@ -6417,10 +6488,10 @@
         <v>26.8</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="K66" s="3" t="s">
         <v>289</v>
@@ -6429,13 +6500,13 @@
         <v>209</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="N66" s="3" t="s">
         <v>34</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="P66" s="3" t="s">
         <v>31</v>
@@ -6444,7 +6515,7 @@
         <v>60</v>
       </c>
       <c r="R66" s="3" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="S66" s="3" t="s">
         <v>133</v>
@@ -6455,19 +6526,19 @@
     </row>
     <row r="67" ht="46" spans="1:22">
       <c r="A67" s="3" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F67" s="6">
         <v>50</v>
@@ -6479,7 +6550,7 @@
         <v>27</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>234</v>
@@ -6491,13 +6562,13 @@
         <v>209</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="N67" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="P67" s="3" t="s">
         <v>31</v>
@@ -6506,7 +6577,7 @@
         <v>32</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="S67" s="3" t="s">
         <v>34</v>
@@ -6517,19 +6588,19 @@
     </row>
     <row r="68" ht="46" spans="1:22">
       <c r="A68" s="3" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F68" s="6">
         <v>100</v>
@@ -6541,13 +6612,13 @@
         <v>29.3</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>271</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="L68" s="3" t="s">
         <v>83</v>
@@ -6559,7 +6630,7 @@
         <v>170</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="P68" s="3" t="s">
         <v>59</v>
@@ -6579,19 +6650,19 @@
     </row>
     <row r="69" ht="46" spans="1:22">
       <c r="A69" s="3" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F69" s="6">
         <v>15</v>
@@ -6603,7 +6674,7 @@
         <v>42.4</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>105</v>
@@ -6621,7 +6692,7 @@
         <v>172</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="P69" s="3" t="s">
         <v>59</v>
@@ -6630,7 +6701,7 @@
         <v>127</v>
       </c>
       <c r="R69" s="3" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="S69" s="3" t="s">
         <v>110</v>
@@ -6641,19 +6712,19 @@
     </row>
     <row r="70" ht="46" spans="1:22">
       <c r="A70" s="3" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F70" s="6">
         <v>50</v>
@@ -6665,34 +6736,34 @@
         <v>50.6</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="K70" s="3" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="L70" s="3" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="N70" s="3" t="s">
         <v>172</v>
       </c>
       <c r="O70" s="3" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="P70" s="3" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="Q70" s="3" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="R70" s="3" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="S70" s="3" t="s">
         <v>110</v>
@@ -6703,19 +6774,19 @@
     </row>
     <row r="71" ht="46" spans="1:22">
       <c r="A71" s="3" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F71" s="6">
         <v>100</v>
@@ -6727,37 +6798,37 @@
         <v>51</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>289</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="N71" s="3" t="s">
         <v>110</v>
       </c>
       <c r="O71" s="3" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="P71" s="3" t="s">
         <v>59</v>
       </c>
       <c r="Q71" s="3" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="R71" s="3" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="S71" s="3" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
@@ -6765,19 +6836,19 @@
     </row>
     <row r="72" ht="92" spans="1:22">
       <c r="A72" s="3" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F72" s="6">
         <v>50</v>
@@ -6789,7 +6860,7 @@
         <v>48.59</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="J72" s="3" t="s">
         <v>146</v>
@@ -6798,28 +6869,28 @@
         <v>208</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="N72" s="3" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="O72" s="3" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="P72" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q72" s="3" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="R72" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="S72" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="S72" s="3" t="s">
-        <v>385</v>
       </c>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
@@ -6827,19 +6898,19 @@
     </row>
     <row r="73" ht="92" spans="1:22">
       <c r="A73" s="3" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F73" s="6">
         <v>100</v>
@@ -6851,7 +6922,7 @@
         <v>53.1</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>112</v>
@@ -6860,25 +6931,25 @@
         <v>200</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="M73" s="3" t="s">
         <v>125</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="P73" s="3" t="s">
         <v>91</v>
       </c>
       <c r="Q73" s="3" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="R73" s="3" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="S73" s="3" t="s">
         <v>52</v>
@@ -6889,19 +6960,19 @@
     </row>
     <row r="74" ht="92" spans="1:22">
       <c r="A74" s="3" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="E74" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F74" s="6">
         <v>15</v>
@@ -6913,16 +6984,16 @@
         <v>39.81</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="M74" s="3" t="s">
         <v>261</v>
@@ -6931,16 +7002,16 @@
         <v>110</v>
       </c>
       <c r="O74" s="3" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="P74" s="3" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="Q74" s="3" t="s">
         <v>189</v>
       </c>
       <c r="R74" s="3" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="S74" s="3" t="s">
         <v>52</v>
@@ -6951,19 +7022,19 @@
     </row>
     <row r="75" ht="92" spans="1:22">
       <c r="A75" s="3" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="E75" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F75" s="6">
         <v>50</v>
@@ -6975,7 +7046,7 @@
         <v>56.39</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="J75" s="3" t="s">
         <v>279</v>
@@ -6984,16 +7055,16 @@
         <v>200</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="M75" s="3" t="s">
         <v>125</v>
       </c>
       <c r="N75" s="3" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="O75" s="3" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="P75" s="3" t="s">
         <v>40</v>
@@ -7002,10 +7073,10 @@
         <v>41</v>
       </c>
       <c r="R75" s="3" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="S75" s="3" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
@@ -7013,19 +7084,19 @@
     </row>
     <row r="76" ht="92" spans="1:19">
       <c r="A76" s="3" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F76" s="6">
         <v>100</v>
@@ -7037,7 +7108,7 @@
         <v>59.93</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="J76" s="3" t="s">
         <v>105</v>
@@ -7046,45 +7117,45 @@
         <v>292</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="N76" s="3" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="O76" s="3" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="P76" s="3" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="Q76" s="3" t="s">
         <v>41</v>
       </c>
       <c r="R76" s="3" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="S76" s="3" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="77" ht="92" spans="1:19">
       <c r="A77" s="3" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="F77" s="6">
         <v>150</v>
@@ -7096,7 +7167,7 @@
         <v>60.76</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>112</v>
@@ -7105,42 +7176,42 @@
         <v>292</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="N77" s="3" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="O77" s="3" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="P77" s="3" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="Q77" s="3" t="s">
         <v>127</v>
       </c>
       <c r="R77" s="3" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="S77" s="3" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="78" ht="46" spans="1:19">
       <c r="A78" s="3" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="E78" s="9" t="s">
         <v>164</v>
@@ -7166,16 +7237,16 @@
     </row>
     <row r="79" ht="46" spans="1:19">
       <c r="A79" s="3" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="E79" s="9" t="s">
         <v>164</v>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with the latest verified data to ensure ongoing accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -1277,7 +1277,7 @@
     <t>Salesforce &amp; University of Southern California &amp; University of Washington</t>
   </si>
   <si>
-    <t>https://linxins.net/coact/</t>
+    <t>https://arxiv.org/abs/2508.03923</t>
   </si>
   <si>
     <t>Song et al., '25</t>
@@ -2545,7 +2545,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with the latest verified data to maintain accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13260"/>
+    <workbookView windowWidth="27660" windowHeight="13120"/>
   </bookViews>
   <sheets>
     <sheet name="Eval Results" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="449">
   <si>
     <t>Model</t>
   </si>
@@ -1341,6 +1341,39 @@
   </si>
   <si>
     <t>Xu et al., '24</t>
+  </si>
+  <si>
+    <t>TianXi_Action_7B</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2508.04037</t>
+  </si>
+  <si>
+    <t>Tang et al., '25</t>
+  </si>
+  <si>
+    <t>105.57/361</t>
+  </si>
+  <si>
+    <t>14.92/46</t>
+  </si>
+  <si>
+    <t>17.96/47</t>
+  </si>
+  <si>
+    <t>6.69/93</t>
+  </si>
+  <si>
+    <t>109.37/360</t>
+  </si>
+  <si>
+    <t>5.58/93</t>
+  </si>
+  <si>
+    <t>5.83/17</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1387,7 @@
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1402,6 +1435,14 @@
     <font>
       <sz val="10"/>
       <color rgb="FF5A3286"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1874,31 +1915,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1907,115 +1945,118 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2024,12 +2065,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -2056,17 +2091,23 @@
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="180" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2544,8 +2585,8 @@
   </sheetPr>
   <dimension ref="A1:AC1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -2639,16 +2680,16 @@
       <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="6">
         <v>15</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="7">
         <v>45866</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="6">
         <v>26</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -2701,16 +2742,16 @@
       <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>50</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <v>45866</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="6">
         <v>31.3</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -2763,16 +2804,16 @@
       <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>100</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>45866</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="6">
         <v>31.4</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -2825,16 +2866,16 @@
       <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <v>100</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>45866</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="6">
         <v>29.63</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -2887,7 +2928,7 @@
       <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="3"/>
@@ -2923,7 +2964,7 @@
       <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="3"/>
@@ -2959,16 +3000,16 @@
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <v>15</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>45866</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <v>9.1</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -3021,16 +3062,16 @@
       <c r="D9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <v>50</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>45866</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="6">
         <v>17.17</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -3083,16 +3124,16 @@
       <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <v>100</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>45866</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="6">
         <v>23</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -3145,16 +3186,16 @@
       <c r="D11" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <v>15</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <v>45866</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="6">
         <v>27.1</v>
       </c>
       <c r="I11" s="3" t="s">
@@ -3207,16 +3248,16 @@
       <c r="D12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <v>50</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <v>45866</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="6">
         <v>35.8</v>
       </c>
       <c r="I12" s="3" t="s">
@@ -3269,16 +3310,16 @@
       <c r="D13" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <v>100</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <v>45866</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="6">
         <v>35.6</v>
       </c>
       <c r="I13" s="3" t="s">
@@ -3331,16 +3372,16 @@
       <c r="D14" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <v>15</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <v>45866</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="6">
         <v>31.2</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -3393,16 +3434,16 @@
       <c r="D15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="6">
         <v>50</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="7">
         <v>45866</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="6">
         <v>43.9</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -3455,16 +3496,16 @@
       <c r="D16" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="6">
         <v>100</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="7">
         <v>45866</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="6">
         <v>41.4</v>
       </c>
       <c r="I16" s="3" t="s">
@@ -3524,16 +3565,16 @@
       <c r="D17" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="6">
         <v>15</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="7">
         <v>45866</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="6">
         <v>27.8</v>
       </c>
       <c r="I17" s="3" t="s">
@@ -3593,16 +3634,16 @@
       <c r="D18" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="6">
         <v>100</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="7">
         <v>45866</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="6">
         <v>33.8</v>
       </c>
       <c r="I18" s="3" t="s">
@@ -3655,16 +3696,16 @@
       <c r="D19" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="6">
         <v>15</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="7">
         <v>45866</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="6">
         <v>31.9</v>
       </c>
       <c r="I19" s="3" t="s">
@@ -3717,16 +3758,16 @@
       <c r="D20" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="6">
         <v>100</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="7">
         <v>45866</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="6">
         <v>40</v>
       </c>
       <c r="I20" s="3" t="s">
@@ -3779,16 +3820,16 @@
       <c r="D21" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="6">
         <v>15</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="7">
         <v>45866</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="6">
         <v>25.7</v>
       </c>
       <c r="I21" s="3" t="s">
@@ -3841,16 +3882,16 @@
       <c r="D22" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="6">
         <v>15</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="7">
         <v>45866</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="6">
         <v>23.3</v>
       </c>
       <c r="I22" s="3" t="s">
@@ -3903,16 +3944,16 @@
       <c r="D23" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>50</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="7">
         <v>45866</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>25.1</v>
       </c>
       <c r="I23" s="3" t="s">
@@ -3965,16 +4006,16 @@
       <c r="D24" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="6">
         <v>50</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="7">
         <v>45866</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="6">
         <v>29.4</v>
       </c>
       <c r="I24" s="3" t="s">
@@ -4027,16 +4068,16 @@
       <c r="D25" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="6">
         <v>100</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="7">
         <v>45866</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="6">
         <v>25.2</v>
       </c>
       <c r="I25" s="3" t="s">
@@ -4089,16 +4130,16 @@
       <c r="D26" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="6">
         <v>100</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="7">
         <v>45866</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="6">
         <v>29.6</v>
       </c>
       <c r="I26" s="3" t="s">
@@ -4151,16 +4192,16 @@
       <c r="D27" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="6">
         <v>15</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="7">
         <v>45866</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="6">
         <v>24</v>
       </c>
       <c r="I27" s="3" t="s">
@@ -4213,16 +4254,16 @@
       <c r="D28" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="6">
         <v>50</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="7">
         <v>45866</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="6">
         <v>25.8</v>
       </c>
       <c r="I28" s="3" t="s">
@@ -4275,16 +4316,16 @@
       <c r="D29" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="6">
         <v>100</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <v>45866</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="6">
         <v>27.1</v>
       </c>
       <c r="I29" s="3" t="s">
@@ -4337,16 +4378,16 @@
       <c r="D30" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="6">
         <v>15</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <v>45866</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="6">
         <v>16.9</v>
       </c>
       <c r="I30" s="3" t="s">
@@ -4399,16 +4440,16 @@
       <c r="D31" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="6">
         <v>50</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>45866</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="6">
         <v>19.9</v>
       </c>
       <c r="I31" s="3" t="s">
@@ -4461,16 +4502,16 @@
       <c r="D32" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="6">
         <v>100</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="7">
         <v>45866</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="6">
         <v>17.7</v>
       </c>
       <c r="I32" s="3" t="s">
@@ -4523,16 +4564,16 @@
       <c r="D33" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="6">
         <v>15</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="7">
         <v>45866</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="6">
         <v>19.9</v>
       </c>
       <c r="I33" s="3" t="s">
@@ -4585,16 +4626,16 @@
       <c r="D34" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="6">
         <v>50</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="7">
         <v>45866</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="6">
         <v>20.6</v>
       </c>
       <c r="I34" s="3" t="s">
@@ -4647,16 +4688,16 @@
       <c r="D35" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="6">
         <v>100</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="7">
         <v>45866</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="6">
         <v>23.1</v>
       </c>
       <c r="I35" s="3" t="s">
@@ -4709,16 +4750,16 @@
       <c r="D36" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="6">
         <v>15</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="7">
         <v>45866</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="6">
         <v>26.2</v>
       </c>
       <c r="I36" s="3" t="s">
@@ -4771,16 +4812,16 @@
       <c r="D37" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="6">
         <v>15</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="7">
         <v>45866</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="6">
         <v>23.6</v>
       </c>
       <c r="I37" s="3" t="s">
@@ -4833,16 +4874,16 @@
       <c r="D38" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="6">
         <v>15</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="7">
         <v>45866</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="6">
         <v>23</v>
       </c>
       <c r="I38" s="3" t="s">
@@ -4895,16 +4936,16 @@
       <c r="D39" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="6">
         <v>50</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="7">
         <v>45866</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="6">
         <v>28.8</v>
       </c>
       <c r="I39" s="3" t="s">
@@ -4957,16 +4998,16 @@
       <c r="D40" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F40" s="6">
         <v>50</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="7">
         <v>45866</v>
       </c>
-      <c r="H40" s="8">
+      <c r="H40" s="6">
         <v>27.7</v>
       </c>
       <c r="I40" s="3" t="s">
@@ -5019,16 +5060,16 @@
       <c r="D41" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="6">
         <v>50</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="7">
         <v>45866</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41" s="6">
         <v>28</v>
       </c>
       <c r="I41" s="3" t="s">
@@ -5081,16 +5122,16 @@
       <c r="D42" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="6">
         <v>100</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="7">
         <v>45866</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H42" s="6">
         <v>27.2</v>
       </c>
       <c r="I42" s="3" t="s">
@@ -5143,16 +5184,16 @@
       <c r="D43" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F43" s="6">
         <v>100</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="7">
         <v>45866</v>
       </c>
-      <c r="H43" s="8">
+      <c r="H43" s="6">
         <v>26.1</v>
       </c>
       <c r="I43" s="3" t="s">
@@ -5205,16 +5246,16 @@
       <c r="D44" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E44" s="11" t="s">
+      <c r="E44" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="6">
         <v>100</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="7">
         <v>45866</v>
       </c>
-      <c r="H44" s="8">
+      <c r="H44" s="6">
         <v>26.6</v>
       </c>
       <c r="I44" s="3" t="s">
@@ -5267,16 +5308,16 @@
       <c r="D45" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E45" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="6">
         <v>15</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="7">
         <v>45866</v>
       </c>
-      <c r="H45" s="8">
+      <c r="H45" s="6">
         <v>28.1</v>
       </c>
       <c r="I45" s="3" t="s">
@@ -5329,16 +5370,16 @@
       <c r="D46" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F46" s="6">
         <v>15</v>
       </c>
-      <c r="G46" s="9">
+      <c r="G46" s="7">
         <v>45866</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H46" s="6">
         <v>30.5</v>
       </c>
       <c r="I46" s="3" t="s">
@@ -5391,16 +5432,16 @@
       <c r="D47" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="6">
         <v>15</v>
       </c>
-      <c r="G47" s="9">
+      <c r="G47" s="7">
         <v>45866</v>
       </c>
-      <c r="H47" s="8">
+      <c r="H47" s="6">
         <v>30.4</v>
       </c>
       <c r="I47" s="3" t="s">
@@ -5453,16 +5494,16 @@
       <c r="D48" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="E48" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F48" s="6">
         <v>50</v>
       </c>
-      <c r="G48" s="9">
+      <c r="G48" s="7">
         <v>45866</v>
       </c>
-      <c r="H48" s="8">
+      <c r="H48" s="6">
         <v>33.8</v>
       </c>
       <c r="I48" s="3" t="s">
@@ -5515,16 +5556,16 @@
       <c r="D49" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F49" s="8">
+      <c r="F49" s="6">
         <v>50</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="7">
         <v>45866</v>
       </c>
-      <c r="H49" s="8">
+      <c r="H49" s="6">
         <v>33.5</v>
       </c>
       <c r="I49" s="3" t="s">
@@ -5577,16 +5618,16 @@
       <c r="D50" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E50" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F50" s="8">
+      <c r="F50" s="6">
         <v>50</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="7">
         <v>45866</v>
       </c>
-      <c r="H50" s="8">
+      <c r="H50" s="6">
         <v>35.1</v>
       </c>
       <c r="I50" s="3" t="s">
@@ -5639,16 +5680,16 @@
       <c r="D51" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E51" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F51" s="6">
         <v>100</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="7">
         <v>45866</v>
       </c>
-      <c r="H51" s="8">
+      <c r="H51" s="6">
         <v>33.8</v>
       </c>
       <c r="I51" s="3" t="s">
@@ -5701,16 +5742,16 @@
       <c r="D52" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E52" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F52" s="8">
+      <c r="F52" s="6">
         <v>100</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="7">
         <v>45866</v>
       </c>
-      <c r="H52" s="8">
+      <c r="H52" s="6">
         <v>35.7</v>
       </c>
       <c r="I52" s="3" t="s">
@@ -5763,16 +5804,16 @@
       <c r="D53" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E53" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F53" s="6">
         <v>100</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="7">
         <v>45866</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H53" s="6">
         <v>34.8</v>
       </c>
       <c r="I53" s="3" t="s">
@@ -5825,16 +5866,16 @@
       <c r="D54" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F54" s="8">
+      <c r="F54" s="6">
         <v>15</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="7">
         <v>45866</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H54" s="6">
         <v>3.04</v>
       </c>
       <c r="I54" s="3" t="s">
@@ -5887,16 +5928,16 @@
       <c r="D55" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E55" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F55" s="8">
+      <c r="F55" s="6">
         <v>100</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G55" s="7">
         <v>45866</v>
       </c>
-      <c r="H55" s="8">
+      <c r="H55" s="6">
         <v>3.88</v>
       </c>
       <c r="I55" s="3" t="s">
@@ -5949,16 +5990,16 @@
       <c r="D56" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E56" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F56" s="6">
         <v>15</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G56" s="7">
         <v>45866</v>
       </c>
-      <c r="H56" s="8">
+      <c r="H56" s="6">
         <v>4.43</v>
       </c>
       <c r="I56" s="3" t="s">
@@ -6011,16 +6052,16 @@
       <c r="D57" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F57" s="8">
+      <c r="F57" s="6">
         <v>100</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="7">
         <v>45866</v>
       </c>
-      <c r="H57" s="8">
+      <c r="H57" s="6">
         <v>5</v>
       </c>
       <c r="I57" s="3" t="s">
@@ -6073,16 +6114,16 @@
       <c r="D58" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="E58" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F58" s="8">
+      <c r="F58" s="6">
         <v>15</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G58" s="7">
         <v>45866</v>
       </c>
-      <c r="H58" s="8">
+      <c r="H58" s="6">
         <v>9.7</v>
       </c>
       <c r="I58" s="3" t="s">
@@ -6135,16 +6176,16 @@
       <c r="D59" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="8">
+      <c r="F59" s="6">
         <v>100</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G59" s="7">
         <v>45866</v>
       </c>
-      <c r="H59" s="8">
+      <c r="H59" s="6">
         <v>10.3</v>
       </c>
       <c r="I59" s="3" t="s">
@@ -6185,61 +6226,61 @@
       <c r="V59" s="3"/>
     </row>
     <row r="60" ht="31" spans="1:22">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E60" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F60" s="13">
+      <c r="F60" s="6">
         <v>15</v>
       </c>
-      <c r="G60" s="14">
+      <c r="G60" s="7">
         <v>45869</v>
       </c>
-      <c r="H60" s="13">
+      <c r="H60" s="6">
         <v>34.64</v>
       </c>
-      <c r="I60" s="5" t="s">
+      <c r="I60" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="J60" s="5" t="s">
+      <c r="J60" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="K60" s="5" t="s">
+      <c r="K60" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L60" s="5" t="s">
+      <c r="L60" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="M60" s="5" t="s">
+      <c r="M60" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="N60" s="5" t="s">
+      <c r="N60" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="O60" s="5" t="s">
+      <c r="O60" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="P60" s="5" t="s">
+      <c r="P60" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="Q60" s="5" t="s">
+      <c r="Q60" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="R60" s="5" t="s">
+      <c r="R60" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="S60" s="5" t="s">
+      <c r="S60" s="3" t="s">
         <v>43</v>
       </c>
       <c r="T60" s="1"/>
@@ -6247,61 +6288,61 @@
       <c r="V60" s="1"/>
     </row>
     <row r="61" ht="31" spans="1:22">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F61" s="13">
+      <c r="F61" s="6">
         <v>50</v>
       </c>
-      <c r="G61" s="14">
+      <c r="G61" s="7">
         <v>45866</v>
       </c>
-      <c r="H61" s="13">
+      <c r="H61" s="6">
         <v>45.76</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="J61" s="5" t="s">
+      <c r="J61" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="K61" s="5" t="s">
+      <c r="K61" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="L61" s="5" t="s">
+      <c r="L61" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="M61" s="5" t="s">
+      <c r="M61" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N61" s="5" t="s">
+      <c r="N61" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O61" s="5" t="s">
+      <c r="O61" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="P61" s="5" t="s">
+      <c r="P61" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="Q61" s="5" t="s">
+      <c r="Q61" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="R61" s="5" t="s">
+      <c r="R61" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="S61" s="5" t="s">
+      <c r="S61" s="3" t="s">
         <v>43</v>
       </c>
       <c r="T61" s="1"/>
@@ -6309,61 +6350,61 @@
       <c r="V61" s="1"/>
     </row>
     <row r="62" ht="31" spans="1:22">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E62" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F62" s="13">
+      <c r="F62" s="6">
         <v>15</v>
       </c>
-      <c r="G62" s="14">
+      <c r="G62" s="7">
         <v>45869</v>
       </c>
-      <c r="H62" s="13">
+      <c r="H62" s="6">
         <v>39</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="I62" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="J62" s="5" t="s">
+      <c r="J62" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="K62" s="5" t="s">
+      <c r="K62" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="L62" s="5" t="s">
+      <c r="L62" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="M62" s="5" t="s">
+      <c r="M62" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="N62" s="5" t="s">
+      <c r="N62" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="O62" s="5" t="s">
+      <c r="O62" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="P62" s="5" t="s">
+      <c r="P62" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Q62" s="5" t="s">
+      <c r="Q62" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="R62" s="5" t="s">
+      <c r="R62" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="S62" s="5" t="s">
+      <c r="S62" s="3" t="s">
         <v>110</v>
       </c>
       <c r="T62" s="1"/>
@@ -6371,61 +6412,61 @@
       <c r="V62" s="1"/>
     </row>
     <row r="63" ht="31" spans="1:22">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="E63" s="12" t="s">
+      <c r="E63" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F63" s="13">
+      <c r="F63" s="6">
         <v>50</v>
       </c>
-      <c r="G63" s="14">
+      <c r="G63" s="7">
         <v>45869</v>
       </c>
-      <c r="H63" s="13">
+      <c r="H63" s="6">
         <v>54.2</v>
       </c>
-      <c r="I63" s="5" t="s">
+      <c r="I63" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="J63" s="5" t="s">
+      <c r="J63" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="K63" s="5" t="s">
+      <c r="K63" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="L63" s="5" t="s">
+      <c r="L63" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="M63" s="5" t="s">
+      <c r="M63" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="N63" s="5" t="s">
+      <c r="N63" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O63" s="5" t="s">
+      <c r="O63" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="P63" s="5" t="s">
+      <c r="P63" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="Q63" s="5" t="s">
+      <c r="Q63" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="R63" s="5" t="s">
+      <c r="R63" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="S63" s="5" t="s">
+      <c r="S63" s="3" t="s">
         <v>364</v>
       </c>
       <c r="T63" s="1"/>
@@ -6433,61 +6474,61 @@
       <c r="V63" s="1"/>
     </row>
     <row r="64" ht="31" spans="1:22">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F64" s="13">
+      <c r="F64" s="6">
         <v>100</v>
       </c>
-      <c r="G64" s="14">
+      <c r="G64" s="7">
         <v>45869</v>
       </c>
-      <c r="H64" s="13">
+      <c r="H64" s="6">
         <v>56</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="I64" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="J64" s="5" t="s">
+      <c r="J64" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="K64" s="5" t="s">
+      <c r="K64" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="L64" s="5" t="s">
+      <c r="L64" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="M64" s="5" t="s">
+      <c r="M64" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="N64" s="5" t="s">
+      <c r="N64" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="O64" s="5" t="s">
+      <c r="O64" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="P64" s="5" t="s">
+      <c r="P64" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="Q64" s="5" t="s">
+      <c r="Q64" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="R64" s="5" t="s">
+      <c r="R64" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="S64" s="5" t="s">
+      <c r="S64" s="3" t="s">
         <v>364</v>
       </c>
       <c r="T64" s="1"/>
@@ -6507,10 +6548,10 @@
       <c r="D65" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="E65" s="15" t="s">
+      <c r="E65" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F65" s="8">
+      <c r="F65" s="6">
         <v>50</v>
       </c>
       <c r="G65" s="3"/>
@@ -6545,16 +6586,16 @@
       <c r="D66" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F66" s="8">
+      <c r="F66" s="6">
         <v>15</v>
       </c>
-      <c r="G66" s="9">
+      <c r="G66" s="7">
         <v>45866</v>
       </c>
-      <c r="H66" s="8">
+      <c r="H66" s="6">
         <v>26.8</v>
       </c>
       <c r="I66" s="3" t="s">
@@ -6607,16 +6648,16 @@
       <c r="D67" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="E67" s="15" t="s">
+      <c r="E67" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F67" s="8">
+      <c r="F67" s="6">
         <v>50</v>
       </c>
-      <c r="G67" s="9">
+      <c r="G67" s="7">
         <v>45866</v>
       </c>
-      <c r="H67" s="8">
+      <c r="H67" s="6">
         <v>27</v>
       </c>
       <c r="I67" s="3" t="s">
@@ -6669,16 +6710,16 @@
       <c r="D68" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="E68" s="15" t="s">
+      <c r="E68" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F68" s="8">
+      <c r="F68" s="6">
         <v>100</v>
       </c>
-      <c r="G68" s="9">
+      <c r="G68" s="7">
         <v>45866</v>
       </c>
-      <c r="H68" s="8">
+      <c r="H68" s="6">
         <v>29.3</v>
       </c>
       <c r="I68" s="3" t="s">
@@ -6731,16 +6772,16 @@
       <c r="D69" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="E69" s="15" t="s">
+      <c r="E69" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F69" s="8">
+      <c r="F69" s="6">
         <v>15</v>
       </c>
-      <c r="G69" s="9">
+      <c r="G69" s="7">
         <v>45866</v>
       </c>
-      <c r="H69" s="8">
+      <c r="H69" s="6">
         <v>42.4</v>
       </c>
       <c r="I69" s="3" t="s">
@@ -6793,16 +6834,16 @@
       <c r="D70" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="E70" s="15" t="s">
+      <c r="E70" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F70" s="8">
+      <c r="F70" s="6">
         <v>50</v>
       </c>
-      <c r="G70" s="9">
+      <c r="G70" s="7">
         <v>45866</v>
       </c>
-      <c r="H70" s="8">
+      <c r="H70" s="6">
         <v>50.6</v>
       </c>
       <c r="I70" s="3" t="s">
@@ -6855,16 +6896,16 @@
       <c r="D71" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="E71" s="15" t="s">
+      <c r="E71" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F71" s="8">
+      <c r="F71" s="6">
         <v>100</v>
       </c>
-      <c r="G71" s="9">
+      <c r="G71" s="7">
         <v>45866</v>
       </c>
-      <c r="H71" s="8">
+      <c r="H71" s="6">
         <v>51</v>
       </c>
       <c r="I71" s="3" t="s">
@@ -6917,16 +6958,16 @@
       <c r="D72" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E72" s="15" t="s">
+      <c r="E72" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F72" s="8">
+      <c r="F72" s="6">
         <v>50</v>
       </c>
-      <c r="G72" s="9">
+      <c r="G72" s="7">
         <v>45866</v>
       </c>
-      <c r="H72" s="8">
+      <c r="H72" s="6">
         <v>48.59</v>
       </c>
       <c r="I72" s="3" t="s">
@@ -6979,16 +7020,16 @@
       <c r="D73" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E73" s="15" t="s">
+      <c r="E73" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F73" s="8">
+      <c r="F73" s="6">
         <v>100</v>
       </c>
-      <c r="G73" s="9">
+      <c r="G73" s="7">
         <v>45866</v>
       </c>
-      <c r="H73" s="8">
+      <c r="H73" s="6">
         <v>53.1</v>
       </c>
       <c r="I73" s="3" t="s">
@@ -7041,16 +7082,16 @@
       <c r="D74" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="E74" s="15" t="s">
+      <c r="E74" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F74" s="8">
+      <c r="F74" s="6">
         <v>15</v>
       </c>
-      <c r="G74" s="9">
+      <c r="G74" s="7">
         <v>45873</v>
       </c>
-      <c r="H74" s="8">
+      <c r="H74" s="6">
         <v>39.81</v>
       </c>
       <c r="I74" s="3" t="s">
@@ -7103,16 +7144,16 @@
       <c r="D75" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="E75" s="15" t="s">
+      <c r="E75" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F75" s="8">
+      <c r="F75" s="6">
         <v>50</v>
       </c>
-      <c r="G75" s="9">
+      <c r="G75" s="7">
         <v>45873</v>
       </c>
-      <c r="H75" s="8">
+      <c r="H75" s="6">
         <v>56.39</v>
       </c>
       <c r="I75" s="3" t="s">
@@ -7165,16 +7206,16 @@
       <c r="D76" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="E76" s="15" t="s">
+      <c r="E76" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F76" s="8">
+      <c r="F76" s="6">
         <v>100</v>
       </c>
-      <c r="G76" s="9">
+      <c r="G76" s="7">
         <v>45873</v>
       </c>
-      <c r="H76" s="8">
+      <c r="H76" s="6">
         <v>59.93</v>
       </c>
       <c r="I76" s="3" t="s">
@@ -7224,16 +7265,16 @@
       <c r="D77" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="E77" s="15" t="s">
+      <c r="E77" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="F77" s="8">
+      <c r="F77" s="6">
         <v>150</v>
       </c>
-      <c r="G77" s="9">
+      <c r="G77" s="7">
         <v>45873</v>
       </c>
-      <c r="H77" s="8">
+      <c r="H77" s="6">
         <v>60.76</v>
       </c>
       <c r="I77" s="3" t="s">
@@ -7283,10 +7324,10 @@
       <c r="D78" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="E78" s="11" t="s">
+      <c r="E78" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F78" s="8">
+      <c r="F78" s="6">
         <v>15</v>
       </c>
       <c r="G78" s="3"/>
@@ -7318,10 +7359,10 @@
       <c r="D79" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="E79" s="11" t="s">
+      <c r="E79" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F79" s="8">
+      <c r="F79" s="6">
         <v>100</v>
       </c>
       <c r="G79" s="3"/>
@@ -7340,15 +7381,123 @@
       <c r="R79" s="3"/>
       <c r="S79" s="3"/>
     </row>
-    <row r="80" ht="15.2" spans="7:11">
-      <c r="G80" s="16"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="18"/>
-    </row>
-    <row r="81" ht="15.2" spans="7:11">
-      <c r="G81" s="16"/>
-      <c r="J81" s="17"/>
-      <c r="K81" s="18"/>
+    <row r="80" ht="31" spans="1:19">
+      <c r="A80" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="E80" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="F80" s="14">
+        <v>50</v>
+      </c>
+      <c r="G80" s="15">
+        <v>45880</v>
+      </c>
+      <c r="H80" s="14">
+        <v>29.24</v>
+      </c>
+      <c r="I80" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="J80" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="K80" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="L80" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="M80" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="N80" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="O80" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="P80" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q80" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="R80" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="S80" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="81" ht="31" spans="1:19">
+      <c r="A81" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="F81" s="14">
+        <v>50</v>
+      </c>
+      <c r="G81" s="15">
+        <v>45880</v>
+      </c>
+      <c r="H81" s="14">
+        <v>30.38</v>
+      </c>
+      <c r="I81" s="11" t="s">
+        <v>446</v>
+      </c>
+      <c r="J81" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="K81" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="L81" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="M81" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="N81" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="O81" s="11" t="s">
+        <v>447</v>
+      </c>
+      <c r="P81" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q81" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="R81" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="S81" s="11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="82" ht="15.2" spans="7:11">
       <c r="G82" s="16"/>
@@ -12241,6 +12390,8 @@
     <hyperlink ref="C62" r:id="rId13" display="https://github.com/simular-ai/Agent-S" tooltip="https://github.com/simular-ai/Agent-S"/>
     <hyperlink ref="C63" r:id="rId13" display="https://github.com/simular-ai/Agent-S" tooltip="https://github.com/simular-ai/Agent-S"/>
     <hyperlink ref="C64" r:id="rId13" display="https://github.com/simular-ai/Agent-S" tooltip="https://github.com/simular-ai/Agent-S"/>
+    <hyperlink ref="C80" r:id="rId17" display="http://arxiv.org/abs/2508.04037" tooltip="http://arxiv.org/abs/2508.04037"/>
+    <hyperlink ref="C81" r:id="rId17" display="http://arxiv.org/abs/2508.04037" tooltip="http://arxiv.org/abs/2508.04037"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with the latest verified data to ensure precision in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="517">
   <si>
     <t>Model</t>
   </si>
@@ -1530,6 +1530,54 @@
   </si>
   <si>
     <t>9.49/17</t>
+  </si>
+  <si>
+    <t>DeepMiner-Mano-7B</t>
+  </si>
+  <si>
+    <t>Mininglamp Technology</t>
+  </si>
+  <si>
+    <t>https://www.mininglamp.com/news/6394/</t>
+  </si>
+  <si>
+    <t>DeepMiner-Mano Team</t>
+  </si>
+  <si>
+    <t>141.96/358</t>
+  </si>
+  <si>
+    <t>15.00/43</t>
+  </si>
+  <si>
+    <t>16.00/93</t>
+  </si>
+  <si>
+    <t>aworldGUIAgent-v1</t>
+  </si>
+  <si>
+    <t>inclusionAI</t>
+  </si>
+  <si>
+    <t>https://github.com/inclusionAI/AWorld/tree/main/examples/osworld</t>
+  </si>
+  <si>
+    <t>Aworld Team</t>
+  </si>
+  <si>
+    <t>209.55/361</t>
+  </si>
+  <si>
+    <t>22.96/46</t>
+  </si>
+  <si>
+    <t>28.39/47</t>
+  </si>
+  <si>
+    <t>40.41/93</t>
+  </si>
+  <si>
+    <t>9.79/17</t>
   </si>
 </sst>
 </file>
@@ -2757,8 +2805,8 @@
   </sheetPr>
   <dimension ref="A1:AC1044"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -8478,15 +8526,135 @@
         <v>404</v>
       </c>
     </row>
-    <row r="89" ht="15.2" spans="7:11">
-      <c r="G89" s="15"/>
-      <c r="J89" s="18"/>
-      <c r="K89" s="19"/>
-    </row>
-    <row r="90" ht="15.2" spans="7:11">
-      <c r="G90" s="15"/>
-      <c r="J90" s="18"/>
-      <c r="K90" s="19"/>
+    <row r="89" ht="31" spans="1:21">
+      <c r="A89" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F89" s="6">
+        <v>100</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I89" s="17">
+        <v>45918</v>
+      </c>
+      <c r="J89" s="6">
+        <v>39.65</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="L89" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="M89" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="N89" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="O89" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="P89" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q89" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="R89" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S89" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T89" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="U89" s="3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="90" ht="31" spans="1:21">
+      <c r="A90" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="F90" s="6">
+        <v>50</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I90" s="17">
+        <v>45918</v>
+      </c>
+      <c r="J90" s="6">
+        <v>58.04</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="M90" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="O90" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="P90" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q90" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T90" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="91" ht="15.2" spans="7:11">
       <c r="G91" s="15"/>
@@ -13346,6 +13514,8 @@
     <hyperlink ref="C85" r:id="rId20" display="https://arxiv.org/abs/2508.15144" tooltip="https://arxiv.org/abs/2508.15144"/>
     <hyperlink ref="C86" r:id="rId21" display="https://arxiv.org/abs/2509.11067" tooltip="https://arxiv.org/abs/2509.11067"/>
     <hyperlink ref="C87" r:id="rId22" display="https://arxiv.org/pdf/2509.02544" tooltip="https://arxiv.org/pdf/2509.02544"/>
+    <hyperlink ref="C89" r:id="rId23" display="https://www.mininglamp.com/news/6394/" tooltip="https://www.mininglamp.com/news/6394/"/>
+    <hyperlink ref="C90" r:id="rId24" display="https://github.com/inclusionAI/AWorld/tree/main/examples/osworld" tooltip="https://github.com/inclusionAI/AWorld/tree/main/examples/osworld"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with the latest verified data to ensure continued precision in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -1544,10 +1544,10 @@
     <t>DeepMiner-Mano Team</t>
   </si>
   <si>
-    <t>141.96/358</t>
-  </si>
-  <si>
-    <t>15.00/43</t>
+    <t>144.96/361</t>
+  </si>
+  <si>
+    <t>18.00/46</t>
   </si>
   <si>
     <t>16.00/93</t>
@@ -2806,7 +2806,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -8555,7 +8555,7 @@
         <v>45918</v>
       </c>
       <c r="J89" s="6">
-        <v>39.65</v>
+        <v>40.15</v>
       </c>
       <c r="K89" s="3" t="s">
         <v>505</v>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with the latest verified data to ensure ongoing precision in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -1532,7 +1532,7 @@
     <t>9.49/17</t>
   </si>
   <si>
-    <t>DeepMiner-Mano-7B</t>
+    <t>DeepMiner-Mano</t>
   </si>
   <si>
     <t>Mininglamp Technology</t>
@@ -2806,7 +2806,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with the latest verified data to uphold accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="525">
   <si>
     <t>Model</t>
   </si>
@@ -1578,6 +1578,30 @@
   </si>
   <si>
     <t>9.79/17</t>
+  </si>
+  <si>
+    <t>autoglm-os-9b-20250925</t>
+  </si>
+  <si>
+    <t>169.24/361</t>
+  </si>
+  <si>
+    <t>26.46/93</t>
+  </si>
+  <si>
+    <t>19.00/24</t>
+  </si>
+  <si>
+    <t>11.82/17</t>
+  </si>
+  <si>
+    <t>172.92/360</t>
+  </si>
+  <si>
+    <t>25.97/93</t>
+  </si>
+  <si>
+    <t>10.99/17</t>
   </si>
 </sst>
 </file>
@@ -2806,7 +2830,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -8656,15 +8680,135 @@
         <v>46</v>
       </c>
     </row>
-    <row r="91" ht="15.2" spans="7:11">
-      <c r="G91" s="15"/>
-      <c r="J91" s="18"/>
-      <c r="K91" s="19"/>
-    </row>
-    <row r="92" ht="15.2" spans="7:11">
-      <c r="G92" s="15"/>
-      <c r="J92" s="18"/>
-      <c r="K92" s="19"/>
+    <row r="91" ht="46" spans="1:21">
+      <c r="A91" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F91" s="6">
+        <v>15</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I91" s="17">
+        <v>45925</v>
+      </c>
+      <c r="J91" s="6">
+        <v>46.88</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="L91" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M91" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="N91" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="O91" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P91" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q91" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="R91" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="S91" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="T91" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="U91" s="3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="92" ht="46" spans="1:21">
+      <c r="A92" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F92" s="6">
+        <v>50</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I92" s="17">
+        <v>45925</v>
+      </c>
+      <c r="J92" s="6">
+        <v>48.03</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N92" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="O92" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P92" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q92" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="R92" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="T92" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="U92" s="3" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="93" ht="15.2" spans="7:11">
       <c r="G93" s="15"/>
@@ -13516,6 +13660,8 @@
     <hyperlink ref="C87" r:id="rId22" display="https://arxiv.org/pdf/2509.02544" tooltip="https://arxiv.org/pdf/2509.02544"/>
     <hyperlink ref="C89" r:id="rId23" display="https://arxiv.org/abs/2509.17336" tooltip="https://www.mininglamp.com/news/6394/"/>
     <hyperlink ref="C90" r:id="rId24" display="https://github.com/inclusionAI/AWorld/tree/main/examples/osworld" tooltip="https://github.com/inclusionAI/AWorld/tree/main/examples/osworld"/>
+    <hyperlink ref="C91" r:id="rId19" display="https://arxiv.org/pdf/2508.14040" tooltip="https://arxiv.org/pdf/2508.14040"/>
+    <hyperlink ref="C92" r:id="rId19" display="https://arxiv.org/pdf/2508.14040" tooltip="https://arxiv.org/pdf/2508.14040"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Refresh osworld_verified_results.xlsx with updated verified data to enhance accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="547">
   <si>
     <t>Model</t>
   </si>
@@ -1647,6 +1647,27 @@
   </si>
   <si>
     <t>10.99/17</t>
+  </si>
+  <si>
+    <t>GTA1 w/ GPT-5</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2507.05791</t>
+  </si>
+  <si>
+    <t>228.92/361</t>
+  </si>
+  <si>
+    <t>30.00/47</t>
+  </si>
+  <si>
+    <t>30.80/47</t>
+  </si>
+  <si>
+    <t>47.35/93</t>
+  </si>
+  <si>
+    <t>9.84/17</t>
   </si>
 </sst>
 </file>
@@ -2875,7 +2896,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -9180,10 +9201,70 @@
         <v>422</v>
       </c>
     </row>
-    <row r="98" ht="15.2" spans="7:11">
-      <c r="G98" s="15"/>
-      <c r="J98" s="18"/>
-      <c r="K98" s="19"/>
+    <row r="98" ht="92" spans="1:21">
+      <c r="A98" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="E98" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="F98" s="6">
+        <v>100</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="I98" s="17">
+        <v>45933</v>
+      </c>
+      <c r="J98" s="6">
+        <v>63.41</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="L98" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="M98" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="N98" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="O98" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="P98" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="Q98" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="R98" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="S98" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="T98" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="U98" s="3" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="99" ht="15.2" spans="7:11">
       <c r="G99" s="15"/>
@@ -14012,6 +14093,7 @@
     <hyperlink ref="C95" r:id="rId24" display="https://github.com/inclusionAI/AWorld/tree/main/examples/osworld" tooltip="https://github.com/inclusionAI/AWorld/tree/main/examples/osworld"/>
     <hyperlink ref="C96" r:id="rId19" display="https://arxiv.org/pdf/2508.14040" tooltip="https://arxiv.org/pdf/2508.14040"/>
     <hyperlink ref="C97" r:id="rId19" display="https://arxiv.org/pdf/2508.14040" tooltip="https://arxiv.org/pdf/2508.14040"/>
+    <hyperlink ref="C98" r:id="rId25" display="https://arxiv.org/pdf/2507.05791" tooltip="https://arxiv.org/pdf/2507.05791"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Refresh osworld_verified_results.xlsx with updated verified data to maintain accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13260"/>
+    <workbookView windowWidth="27660" windowHeight="13120"/>
   </bookViews>
   <sheets>
     <sheet name="Eval Results" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="608">
   <si>
     <t>Model</t>
   </si>
@@ -1830,6 +1830,27 @@
   </si>
   <si>
     <t>11.99/17</t>
+  </si>
+  <si>
+    <t>UI-TARS-2-2509</t>
+  </si>
+  <si>
+    <t>191.69/361</t>
+  </si>
+  <si>
+    <t>28.96/46</t>
+  </si>
+  <si>
+    <t>31.00/47</t>
+  </si>
+  <si>
+    <t>26.50/47</t>
+  </si>
+  <si>
+    <t>31.74/93</t>
+  </si>
+  <si>
+    <t>8.49/17</t>
   </si>
 </sst>
 </file>
@@ -3058,7 +3079,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="G80" sqref="A1:V109"/>
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -10395,10 +10416,73 @@
         <v>451</v>
       </c>
     </row>
-    <row r="110" ht="15.2" spans="7:11">
-      <c r="G110" s="15"/>
-      <c r="J110" s="18"/>
-      <c r="K110" s="19"/>
+    <row r="110" ht="16" spans="1:22">
+      <c r="A110" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F110" s="6">
+        <v>100</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J110" s="17">
+        <v>45944</v>
+      </c>
+      <c r="K110" s="6">
+        <v>53.1</v>
+      </c>
+      <c r="L110" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="M110" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="N110" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O110" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="P110" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="Q110" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R110" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="S110" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="T110" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="U110" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="V110" s="3" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="111" ht="15.2" spans="7:11">
       <c r="G111" s="15"/>
@@ -15168,8 +15252,7 @@
     <hyperlink ref="C96" r:id="rId19" display="https://arxiv.org/pdf/2508.14040" tooltip="https://arxiv.org/pdf/2508.14040"/>
     <hyperlink ref="C97" r:id="rId19" display="https://arxiv.org/pdf/2508.14040" tooltip="https://arxiv.org/pdf/2508.14040"/>
     <hyperlink ref="C98" r:id="rId25" display="https://arxiv.org/pdf/2507.05791" tooltip="https://arxiv.org/pdf/2507.05791"/>
-    <hyperlink ref="C99" r:id="rId26" display="https://arxiv.org/abs/2510.02250" tooltip="https://arxiv.org/abs/2510.02250"/>
-    <hyperlink ref="C100" r:id="rId26" display="https://arxiv.org/abs/2510.02250" tooltip="https://arxiv.org/abs/2510.02250"/>
+    <hyperlink ref="C110" r:id="rId22" display="https://arxiv.org/pdf/2509.02544" tooltip="https://arxiv.org/pdf/2509.02544"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Refresh osworld_verified_results.xlsx with the latest verified data to ensure continued accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -2296,12 +2296,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2426,7 +2441,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2438,34 +2453,34 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2553,50 +2568,50 @@
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="180" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -3079,7 +3094,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+      <selection activeCell="G82" sqref="A1:V110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -7088,7 +7103,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="60" ht="31" spans="1:22">
+    <row r="60" ht="31.75" spans="1:22">
       <c r="A60" s="3" t="s">
         <v>331</v>
       </c>
@@ -7156,7 +7171,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="61" ht="31" spans="1:22">
+    <row r="61" ht="31.75" spans="1:22">
       <c r="A61" s="3" t="s">
         <v>344</v>
       </c>
@@ -7224,7 +7239,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="62" ht="31" spans="1:22">
+    <row r="62" ht="31.75" spans="1:22">
       <c r="A62" s="3" t="s">
         <v>344</v>
       </c>
@@ -7292,7 +7307,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="63" ht="16" spans="1:22">
+    <row r="63" ht="16.75" spans="1:22">
       <c r="A63" s="3" t="s">
         <v>352</v>
       </c>
@@ -7360,7 +7375,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" ht="16" spans="1:22">
+    <row r="64" ht="16.75" spans="1:22">
       <c r="A64" s="3" t="s">
         <v>352</v>
       </c>
@@ -7428,7 +7443,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="65" ht="31" spans="1:22">
+    <row r="65" ht="31.75" spans="1:22">
       <c r="A65" s="3" t="s">
         <v>365</v>
       </c>
@@ -7496,7 +7511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" ht="31" spans="1:22">
+    <row r="66" ht="31.75" spans="1:22">
       <c r="A66" s="3" t="s">
         <v>365</v>
       </c>
@@ -7564,7 +7579,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" ht="31" spans="1:22">
+    <row r="67" ht="31.75" spans="1:22">
       <c r="A67" s="3" t="s">
         <v>377</v>
       </c>
@@ -7632,7 +7647,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="68" ht="31" spans="1:22">
+    <row r="68" ht="31.75" spans="1:22">
       <c r="A68" s="3" t="s">
         <v>377</v>
       </c>
@@ -7700,7 +7715,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="69" ht="31" spans="1:22">
+    <row r="69" ht="31.75" spans="1:22">
       <c r="A69" s="3" t="s">
         <v>377</v>
       </c>
@@ -7768,7 +7783,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="70" ht="31" spans="1:22">
+    <row r="70" ht="31.75" spans="1:22">
       <c r="A70" s="3" t="s">
         <v>391</v>
       </c>
@@ -7812,7 +7827,7 @@
       <c r="U70" s="3"/>
       <c r="V70" s="3"/>
     </row>
-    <row r="71" ht="46" spans="1:22">
+    <row r="71" ht="46.75" spans="1:22">
       <c r="A71" s="3" t="s">
         <v>393</v>
       </c>
@@ -7880,7 +7895,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" ht="46" spans="1:22">
+    <row r="72" ht="46.75" spans="1:22">
       <c r="A72" s="3" t="s">
         <v>393</v>
       </c>
@@ -7948,7 +7963,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" ht="46" spans="1:22">
+    <row r="73" ht="46.75" spans="1:22">
       <c r="A73" s="3" t="s">
         <v>393</v>
       </c>
@@ -8016,7 +8031,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" ht="46" spans="1:22">
+    <row r="74" ht="46.75" spans="1:22">
       <c r="A74" s="3" t="s">
         <v>407</v>
       </c>
@@ -8084,7 +8099,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="75" ht="46" spans="1:22">
+    <row r="75" ht="46.75" spans="1:22">
       <c r="A75" s="3" t="s">
         <v>407</v>
       </c>
@@ -8152,7 +8167,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="76" ht="46" spans="1:22">
+    <row r="76" ht="46.75" spans="1:22">
       <c r="A76" s="3" t="s">
         <v>407</v>
       </c>
@@ -8220,7 +8235,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="77" ht="92" spans="1:22">
+    <row r="77" ht="92.75" spans="1:22">
       <c r="A77" s="3" t="s">
         <v>424</v>
       </c>
@@ -8288,7 +8303,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="78" ht="92" spans="1:22">
+    <row r="78" ht="92.75" spans="1:22">
       <c r="A78" s="3" t="s">
         <v>424</v>
       </c>
@@ -8356,7 +8371,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" ht="92" spans="1:22">
+    <row r="79" ht="92.75" spans="1:22">
       <c r="A79" s="3" t="s">
         <v>437</v>
       </c>
@@ -8424,7 +8439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="80" ht="92" spans="1:22">
+    <row r="80" ht="92.75" spans="1:22">
       <c r="A80" s="3" t="s">
         <v>437</v>
       </c>
@@ -8492,7 +8507,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="81" ht="92" spans="1:22">
+    <row r="81" ht="92.75" spans="1:22">
       <c r="A81" s="3" t="s">
         <v>437</v>
       </c>
@@ -8560,7 +8575,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="82" ht="92" spans="1:22">
+    <row r="82" ht="92.75" spans="1:22">
       <c r="A82" s="3" t="s">
         <v>437</v>
       </c>
@@ -8628,7 +8643,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="83" ht="46" spans="1:22">
+    <row r="83" ht="46.75" spans="1:22">
       <c r="A83" s="3" t="s">
         <v>458</v>
       </c>
@@ -8672,7 +8687,7 @@
       <c r="U83" s="3"/>
       <c r="V83" s="3"/>
     </row>
-    <row r="84" ht="46" spans="1:22">
+    <row r="84" ht="46.75" spans="1:22">
       <c r="A84" s="3" t="s">
         <v>458</v>
       </c>
@@ -8716,7 +8731,7 @@
       <c r="U84" s="3"/>
       <c r="V84" s="3"/>
     </row>
-    <row r="85" ht="16" spans="1:22">
+    <row r="85" ht="16.75" spans="1:22">
       <c r="A85" s="3" t="s">
         <v>461</v>
       </c>
@@ -8784,7 +8799,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="86" ht="16" spans="1:22">
+    <row r="86" ht="16.75" spans="1:22">
       <c r="A86" s="3" t="s">
         <v>461</v>
       </c>
@@ -8852,7 +8867,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="87" ht="46" spans="1:22">
+    <row r="87" ht="46.75" spans="1:22">
       <c r="A87" s="3" t="s">
         <v>472</v>
       </c>
@@ -8920,7 +8935,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" ht="46" spans="1:22">
+    <row r="88" ht="46.75" spans="1:22">
       <c r="A88" s="3" t="s">
         <v>472</v>
       </c>
@@ -8988,7 +9003,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="89" ht="31" spans="1:22">
+    <row r="89" ht="31.75" spans="1:22">
       <c r="A89" s="3" t="s">
         <v>485</v>
       </c>
@@ -9056,7 +9071,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" ht="31" spans="1:22">
+    <row r="90" ht="31.75" spans="1:22">
       <c r="A90" s="3" t="s">
         <v>491</v>
       </c>
@@ -9124,7 +9139,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="91" ht="16" spans="1:22">
+    <row r="91" ht="16.75" spans="1:22">
       <c r="A91" s="3" t="s">
         <v>495</v>
       </c>
@@ -9192,7 +9207,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="92" ht="16" spans="1:22">
+    <row r="92" ht="16.75" spans="1:22">
       <c r="A92" s="3" t="s">
         <v>505</v>
       </c>
@@ -9260,7 +9275,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="93" ht="46" spans="1:22">
+    <row r="93" ht="46.75" spans="1:22">
       <c r="A93" s="12" t="s">
         <v>510</v>
       </c>
@@ -9328,7 +9343,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="94" ht="31" spans="1:22">
+    <row r="94" ht="31.75" spans="1:22">
       <c r="A94" s="3" t="s">
         <v>518</v>
       </c>
@@ -9396,7 +9411,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="95" ht="16" spans="1:22">
+    <row r="95" ht="16.75" spans="1:22">
       <c r="A95" s="3" t="s">
         <v>525</v>
       </c>
@@ -9464,7 +9479,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" ht="46" spans="1:22">
+    <row r="96" ht="46.75" spans="1:22">
       <c r="A96" s="3" t="s">
         <v>533</v>
       </c>
@@ -9532,7 +9547,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="97" ht="46" spans="1:22">
+    <row r="97" ht="46.75" spans="1:22">
       <c r="A97" s="3" t="s">
         <v>533</v>
       </c>
@@ -9600,7 +9615,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="98" ht="92" spans="1:22">
+    <row r="98" ht="92.75" spans="1:22">
       <c r="A98" s="3" t="s">
         <v>541</v>
       </c>
@@ -9668,7 +9683,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="99" ht="31" spans="1:22">
+    <row r="99" ht="31.75" spans="1:22">
       <c r="A99" s="3" t="s">
         <v>548</v>
       </c>
@@ -9736,7 +9751,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="100" ht="31" spans="1:22">
+    <row r="100" ht="31.75" spans="1:22">
       <c r="A100" s="3" t="s">
         <v>559</v>
       </c>
@@ -9804,7 +9819,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="101" ht="31" spans="1:22">
+    <row r="101" ht="31.75" spans="1:22">
       <c r="A101" s="3" t="s">
         <v>559</v>
       </c>
@@ -9872,7 +9887,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="102" ht="31" spans="1:22">
+    <row r="102" ht="31.75" spans="1:22">
       <c r="A102" s="3" t="s">
         <v>559</v>
       </c>
@@ -9940,7 +9955,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="103" ht="31" spans="1:22">
+    <row r="103" ht="31.75" spans="1:22">
       <c r="A103" s="3" t="s">
         <v>559</v>
       </c>
@@ -10008,7 +10023,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="104" ht="31" spans="1:22">
+    <row r="104" ht="31.75" spans="1:22">
       <c r="A104" s="3" t="s">
         <v>559</v>
       </c>
@@ -10076,7 +10091,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="105" ht="31" spans="1:22">
+    <row r="105" ht="31.75" spans="1:22">
       <c r="A105" s="3" t="s">
         <v>559</v>
       </c>
@@ -10144,7 +10159,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="106" ht="31" spans="1:22">
+    <row r="106" ht="31.75" spans="1:22">
       <c r="A106" s="3" t="s">
         <v>559</v>
       </c>
@@ -10212,7 +10227,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="107" ht="31" spans="1:22">
+    <row r="107" ht="31.75" spans="1:22">
       <c r="A107" s="3" t="s">
         <v>559</v>
       </c>
@@ -10280,7 +10295,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="108" ht="31" spans="1:22">
+    <row r="108" ht="31.75" spans="1:22">
       <c r="A108" s="3" t="s">
         <v>559</v>
       </c>
@@ -10348,7 +10363,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="109" ht="31" spans="1:22">
+    <row r="109" ht="31.75" spans="1:22">
       <c r="A109" s="3" t="s">
         <v>559</v>
       </c>
@@ -10416,7 +10431,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="110" ht="16" spans="1:22">
+    <row r="110" ht="16.75" spans="1:22">
       <c r="A110" s="3" t="s">
         <v>601</v>
       </c>
@@ -10439,7 +10454,7 @@
         <v>27</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>428</v>
+        <v>27</v>
       </c>
       <c r="I110" s="3" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Remove temporary backup file and update osworld_verified_results.xlsx with the latest verified data for improved accuracy in analysis and reporting.
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13120"/>
+    <workbookView windowWidth="27660" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Eval Results" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2081" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="642">
   <si>
     <t>Model</t>
   </si>
@@ -1878,6 +1878,81 @@
   </si>
   <si>
     <t>8.49/17</t>
+  </si>
+  <si>
+    <t>agi-0</t>
+  </si>
+  <si>
+    <t>AGI Inc</t>
+  </si>
+  <si>
+    <t>https://www.theagi.company/blog/osworld</t>
+  </si>
+  <si>
+    <t>AGI Inc research team</t>
+  </si>
+  <si>
+    <t>274.52/360</t>
+  </si>
+  <si>
+    <t>35.96/46</t>
+  </si>
+  <si>
+    <t>32.96/47</t>
+  </si>
+  <si>
+    <t>18.97/23</t>
+  </si>
+  <si>
+    <t>66.82/92</t>
+  </si>
+  <si>
+    <t>22.00/24</t>
+  </si>
+  <si>
+    <t>13.82/17</t>
+  </si>
+  <si>
+    <t>qwen3-vl-flash-2025-10-25</t>
+  </si>
+  <si>
+    <t>Qwen Team, Alibaba Group</t>
+  </si>
+  <si>
+    <t>https://qwen.ai/blog?id=99f0335c4ad9ff6153e517418d48535ab6d8afef&amp;from=research.latest-advancements-list</t>
+  </si>
+  <si>
+    <t>Alibaba Qwen</t>
+  </si>
+  <si>
+    <t>150.07/361</t>
+  </si>
+  <si>
+    <t>10.83/47</t>
+  </si>
+  <si>
+    <t>23.96/47</t>
+  </si>
+  <si>
+    <t>20.47/93</t>
+  </si>
+  <si>
+    <t>5.85/17</t>
+  </si>
+  <si>
+    <t>DeepMiner-Mano-72B</t>
+  </si>
+  <si>
+    <t>https://www.mininglamp.com/news/6394/</t>
+  </si>
+  <si>
+    <t>194.62/361</t>
+  </si>
+  <si>
+    <t>23.00/26</t>
+  </si>
+  <si>
+    <t>22.70/93</t>
   </si>
 </sst>
 </file>
@@ -3106,7 +3181,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="A113" sqref="$A113:$XFD113"/>
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -10647,39 +10722,209 @@
         <v>318</v>
       </c>
     </row>
-    <row r="113" ht="15.2" spans="1:22">
-      <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="6"/>
-      <c r="G113" s="3"/>
-      <c r="H113" s="3"/>
-      <c r="I113" s="3"/>
-      <c r="J113" s="17"/>
-      <c r="K113" s="6"/>
-      <c r="L113" s="3"/>
-      <c r="M113" s="3"/>
-      <c r="N113" s="3"/>
-      <c r="O113" s="3"/>
-      <c r="P113" s="3"/>
-      <c r="Q113" s="3"/>
-      <c r="R113" s="3"/>
-      <c r="S113" s="3"/>
-      <c r="T113" s="3"/>
-      <c r="U113" s="3"/>
-      <c r="V113" s="3"/>
-    </row>
-    <row r="114" ht="15.2" spans="7:11">
-      <c r="G114" s="15"/>
-      <c r="J114" s="18"/>
-      <c r="K114" s="19"/>
-    </row>
-    <row r="115" ht="15.2" spans="7:11">
-      <c r="G115" s="15"/>
-      <c r="J115" s="18"/>
-      <c r="K115" s="19"/>
+    <row r="113" ht="31" spans="1:22">
+      <c r="A113" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="E113" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F113" s="6">
+        <v>50</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J113" s="17">
+        <v>45952</v>
+      </c>
+      <c r="K113" s="6">
+        <v>76.26</v>
+      </c>
+      <c r="L113" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="M113" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="N113" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="O113" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="P113" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="Q113" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="R113" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="S113" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="T113" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="U113" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="V113" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="114" ht="31" spans="1:22">
+      <c r="A114" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="E114" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F114" s="6">
+        <v>100</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J114" s="17">
+        <v>45953</v>
+      </c>
+      <c r="K114" s="6">
+        <v>41.57</v>
+      </c>
+      <c r="L114" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="M114" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="N114" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="O114" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="P114" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q114" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="R114" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="S114" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="T114" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="U114" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="V114" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="115" ht="31" spans="1:22">
+      <c r="A115" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F115" s="6">
+        <v>100</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J115" s="17">
+        <v>45961</v>
+      </c>
+      <c r="K115" s="6">
+        <v>53.91</v>
+      </c>
+      <c r="L115" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="M115" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="N115" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="O115" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="P115" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q115" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="R115" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="S115" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="T115" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="U115" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="V115" s="3" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="116" ht="15.2" spans="7:11">
       <c r="G116" s="15"/>
@@ -15427,6 +15672,9 @@
     <hyperlink ref="C99" r:id="rId19" display="https://arxiv.org/pdf/2508.14040" tooltip="https://arxiv.org/pdf/2508.14040"/>
     <hyperlink ref="C100" r:id="rId25" display="https://arxiv.org/pdf/2507.05791" tooltip="https://arxiv.org/pdf/2507.05791"/>
     <hyperlink ref="C112" r:id="rId22" display="https://arxiv.org/pdf/2509.02544" tooltip="https://arxiv.org/pdf/2509.02544"/>
+    <hyperlink ref="C113" r:id="rId26" display="https://www.theagi.company/blog/osworld" tooltip="https://www.theagi.company/blog/osworld"/>
+    <hyperlink ref="C114" r:id="rId27" display="https://qwen.ai/blog?id=99f0335c4ad9ff6153e517418d48535ab6d8afef&amp;from=research.latest-advancements-list" tooltip="https://qwen.ai/blog?id=99f0335c4ad9ff6153e517418d48535ab6d8afef&amp;from=research.latest-advancements-list"/>
+    <hyperlink ref="C115" r:id="rId23" display="https://www.mininglamp.com/news/6394/" tooltip="https://www.mininglamp.com/news/6394/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Remove temporary verified results file and update main verified results file
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2195" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2233" uniqueCount="664">
   <si>
     <t>Model</t>
   </si>
@@ -1133,24 +1133,27 @@
     <t>https://github.com/simular-ai/Agent-S</t>
   </si>
   <si>
+    <t>Simular Research, 25</t>
+  </si>
+  <si>
+    <t>Agentic framework</t>
+  </si>
+  <si>
+    <t>128.81/369</t>
+  </si>
+  <si>
+    <t>12.96/47</t>
+  </si>
+  <si>
+    <t>14.00/101</t>
+  </si>
+  <si>
+    <t>6.89/17</t>
+  </si>
+  <si>
     <t>Simular Research, '25</t>
   </si>
   <si>
-    <t>Agentic framework</t>
-  </si>
-  <si>
-    <t>128.81/369</t>
-  </si>
-  <si>
-    <t>12.96/47</t>
-  </si>
-  <si>
-    <t>14.00/101</t>
-  </si>
-  <si>
-    <t>6.89/17</t>
-  </si>
-  <si>
     <t>168.84/369</t>
   </si>
   <si>
@@ -1712,9 +1715,6 @@
     <t>https://arxiv.org/abs/2510.02250</t>
   </si>
   <si>
-    <t>Gonzalez-Pumariega et. al, '25</t>
-  </si>
-  <si>
     <t>252.35/361</t>
   </si>
   <si>
@@ -1860,6 +1860,45 @@
   </si>
   <si>
     <t>11.99/17</t>
+  </si>
+  <si>
+    <t>agent s3 w/ Opus 4.5 + GPT-5 bBoN (N=10)</t>
+  </si>
+  <si>
+    <t>262.02/361</t>
+  </si>
+  <si>
+    <t>33.96/47</t>
+  </si>
+  <si>
+    <t>19.97/23</t>
+  </si>
+  <si>
+    <t>59.43/93</t>
+  </si>
+  <si>
+    <t>10.70/17</t>
+  </si>
+  <si>
+    <t>agent s3 w/ Opus 4.5</t>
+  </si>
+  <si>
+    <t>243.52/361</t>
+  </si>
+  <si>
+    <t>30.96/46</t>
+  </si>
+  <si>
+    <t>40.00/47</t>
+  </si>
+  <si>
+    <t>30.99/47</t>
+  </si>
+  <si>
+    <t>54.87/93</t>
+  </si>
+  <si>
+    <t>12.70/17</t>
   </si>
   <si>
     <t>UI-TARS-2-2509</t>
@@ -2758,7 +2797,7 @@
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
     <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Explanatory Text" xfId="11" builtinId="53"/>
     <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
     <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
@@ -3223,7 +3262,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F112" sqref="A1:V118"/>
+      <selection activeCell="C112" sqref="A1:V120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -7651,7 +7690,7 @@
         <v>367</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>369</v>
@@ -7675,7 +7714,7 @@
         <v>45.76</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="M66" s="3" t="s">
         <v>283</v>
@@ -7684,7 +7723,7 @@
         <v>296</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="P66" s="3" t="s">
         <v>112</v>
@@ -7693,7 +7732,7 @@
         <v>47</v>
       </c>
       <c r="R66" s="3" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="S66" s="3" t="s">
         <v>96</v>
@@ -7710,7 +7749,7 @@
     </row>
     <row r="67" ht="31.75" spans="1:22">
       <c r="A67" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>366</v>
@@ -7719,7 +7758,7 @@
         <v>367</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>369</v>
@@ -7743,7 +7782,7 @@
         <v>39</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="M67" s="3" t="s">
         <v>238</v>
@@ -7752,7 +7791,7 @@
         <v>171</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="P67" s="3" t="s">
         <v>316</v>
@@ -7761,7 +7800,7 @@
         <v>108</v>
       </c>
       <c r="R67" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="S67" s="3" t="s">
         <v>44</v>
@@ -7770,7 +7809,7 @@
         <v>45</v>
       </c>
       <c r="U67" s="3" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="V67" s="3" t="s">
         <v>115</v>
@@ -7778,7 +7817,7 @@
     </row>
     <row r="68" ht="31.75" spans="1:22">
       <c r="A68" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>366</v>
@@ -7787,7 +7826,7 @@
         <v>367</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>369</v>
@@ -7811,7 +7850,7 @@
         <v>54.2</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M68" s="3" t="s">
         <v>110</v>
@@ -7820,25 +7859,25 @@
         <v>315</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="P68" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="Q68" s="3" t="s">
         <v>38</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="T68" s="3" t="s">
         <v>132</v>
       </c>
       <c r="U68" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="V68" s="3" t="s">
         <v>318</v>
@@ -7846,7 +7885,7 @@
     </row>
     <row r="69" ht="31.75" spans="1:22">
       <c r="A69" s="3" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>366</v>
@@ -7855,7 +7894,7 @@
         <v>367</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>369</v>
@@ -7879,7 +7918,7 @@
         <v>56</v>
       </c>
       <c r="L69" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="M69" s="3" t="s">
         <v>110</v>
@@ -7888,25 +7927,25 @@
         <v>315</v>
       </c>
       <c r="O69" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="P69" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="Q69" s="3" t="s">
         <v>38</v>
       </c>
       <c r="R69" s="3" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="T69" s="3" t="s">
         <v>132</v>
       </c>
       <c r="U69" s="3" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="V69" s="3" t="s">
         <v>318</v>
@@ -7914,7 +7953,7 @@
     </row>
     <row r="70" ht="31.75" spans="1:22">
       <c r="A70" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>366</v>
@@ -7923,7 +7962,7 @@
         <v>367</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>369</v>
@@ -7942,7 +7981,7 @@
       </c>
       <c r="J70" s="3"/>
       <c r="K70" s="3" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
@@ -7958,16 +7997,16 @@
     </row>
     <row r="71" ht="46.75" spans="1:22">
       <c r="A71" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>369</v>
@@ -7991,10 +8030,10 @@
         <v>26.8</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N71" s="3" t="s">
         <v>293</v>
@@ -8003,13 +8042,13 @@
         <v>213</v>
       </c>
       <c r="P71" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="Q71" s="3" t="s">
         <v>38</v>
       </c>
       <c r="R71" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="S71" s="3" t="s">
         <v>35</v>
@@ -8018,7 +8057,7 @@
         <v>64</v>
       </c>
       <c r="U71" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="V71" s="3" t="s">
         <v>138</v>
@@ -8026,16 +8065,16 @@
     </row>
     <row r="72" ht="46.75" spans="1:22">
       <c r="A72" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>369</v>
@@ -8059,7 +8098,7 @@
         <v>27</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M72" s="3" t="s">
         <v>238</v>
@@ -8071,13 +8110,13 @@
         <v>213</v>
       </c>
       <c r="P72" s="3" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="Q72" s="3" t="s">
         <v>33</v>
       </c>
       <c r="R72" s="3" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="S72" s="3" t="s">
         <v>35</v>
@@ -8086,7 +8125,7 @@
         <v>36</v>
       </c>
       <c r="U72" s="3" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="V72" s="3" t="s">
         <v>38</v>
@@ -8094,16 +8133,16 @@
     </row>
     <row r="73" ht="46.75" spans="1:22">
       <c r="A73" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>369</v>
@@ -8127,7 +8166,7 @@
         <v>29.3</v>
       </c>
       <c r="L73" s="3" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="M73" s="3" t="s">
         <v>275</v>
@@ -8145,7 +8184,7 @@
         <v>174</v>
       </c>
       <c r="R73" s="3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="S73" s="3" t="s">
         <v>63</v>
@@ -8162,16 +8201,16 @@
     </row>
     <row r="74" ht="46.75" spans="1:22">
       <c r="A74" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>369</v>
@@ -8195,7 +8234,7 @@
         <v>42.4</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M74" s="3" t="s">
         <v>110</v>
@@ -8213,7 +8252,7 @@
         <v>176</v>
       </c>
       <c r="R74" s="3" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="S74" s="3" t="s">
         <v>63</v>
@@ -8222,7 +8261,7 @@
         <v>132</v>
       </c>
       <c r="U74" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="V74" s="3" t="s">
         <v>115</v>
@@ -8230,16 +8269,16 @@
     </row>
     <row r="75" ht="46.75" spans="1:22">
       <c r="A75" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E75" s="11" t="s">
         <v>369</v>
@@ -8263,16 +8302,16 @@
         <v>50.6</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="N75" s="3" t="s">
         <v>310</v>
       </c>
       <c r="O75" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="P75" s="3" t="s">
         <v>316</v>
@@ -8281,16 +8320,16 @@
         <v>176</v>
       </c>
       <c r="R75" s="3" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="S75" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="T75" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U75" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="V75" s="3" t="s">
         <v>115</v>
@@ -8298,16 +8337,16 @@
     </row>
     <row r="76" ht="46.75" spans="1:22">
       <c r="A76" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>369</v>
@@ -8331,51 +8370,51 @@
         <v>51</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="N76" s="3" t="s">
         <v>293</v>
       </c>
       <c r="O76" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="P76" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="Q76" s="3" t="s">
         <v>115</v>
       </c>
       <c r="R76" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="S76" s="3" t="s">
         <v>63</v>
       </c>
       <c r="T76" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U76" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="V76" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="77" ht="92.75" spans="1:22">
       <c r="A77" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>369</v>
@@ -8387,7 +8426,7 @@
         <v>27</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I77" s="3" t="s">
         <v>27</v>
@@ -8399,7 +8438,7 @@
         <v>48.59</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M77" s="3" t="s">
         <v>151</v>
@@ -8408,42 +8447,42 @@
         <v>212</v>
       </c>
       <c r="O77" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="P77" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="Q77" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="R77" s="3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="S77" s="3" t="s">
         <v>54</v>
       </c>
       <c r="T77" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="U77" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="V77" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="78" ht="92.75" spans="1:22">
       <c r="A78" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>369</v>
@@ -8455,7 +8494,7 @@
         <v>27</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I78" s="3" t="s">
         <v>27</v>
@@ -8467,7 +8506,7 @@
         <v>53.1</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="M78" s="3" t="s">
         <v>117</v>
@@ -8476,25 +8515,25 @@
         <v>204</v>
       </c>
       <c r="O78" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="P78" s="3" t="s">
         <v>130</v>
       </c>
       <c r="Q78" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="R78" s="3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="S78" s="3" t="s">
         <v>96</v>
       </c>
       <c r="T78" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="U78" s="3" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="V78" s="3" t="s">
         <v>56</v>
@@ -8502,16 +8541,16 @@
     </row>
     <row r="79" ht="92.75" spans="1:22">
       <c r="A79" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E79" s="11" t="s">
         <v>369</v>
@@ -8523,7 +8562,7 @@
         <v>27</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>27</v>
@@ -8535,16 +8574,16 @@
         <v>39.81</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="N79" s="3" t="s">
         <v>30</v>
       </c>
       <c r="O79" s="3" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="P79" s="3" t="s">
         <v>265</v>
@@ -8553,16 +8592,16 @@
         <v>115</v>
       </c>
       <c r="R79" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="S79" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="T79" s="3" t="s">
         <v>193</v>
       </c>
       <c r="U79" s="3" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="V79" s="3" t="s">
         <v>56</v>
@@ -8570,16 +8609,16 @@
     </row>
     <row r="80" ht="92.75" spans="1:22">
       <c r="A80" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>369</v>
@@ -8591,7 +8630,7 @@
         <v>27</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I80" s="3" t="s">
         <v>27</v>
@@ -8603,7 +8642,7 @@
         <v>56.39</v>
       </c>
       <c r="L80" s="3" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="M80" s="3" t="s">
         <v>283</v>
@@ -8612,7 +8651,7 @@
         <v>204</v>
       </c>
       <c r="O80" s="3" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="P80" s="3" t="s">
         <v>130</v>
@@ -8621,7 +8660,7 @@
         <v>318</v>
       </c>
       <c r="R80" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="S80" s="3" t="s">
         <v>44</v>
@@ -8630,24 +8669,24 @@
         <v>45</v>
       </c>
       <c r="U80" s="3" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="V80" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="81" ht="92.75" spans="1:22">
       <c r="A81" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>369</v>
@@ -8659,7 +8698,7 @@
         <v>27</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I81" s="3" t="s">
         <v>27</v>
@@ -8671,7 +8710,7 @@
         <v>59.93</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="M81" s="3" t="s">
         <v>110</v>
@@ -8680,42 +8719,42 @@
         <v>296</v>
       </c>
       <c r="O81" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="P81" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="Q81" s="3" t="s">
         <v>318</v>
       </c>
       <c r="R81" s="3" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="S81" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="T81" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U81" s="3" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="V81" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="82" ht="92.75" spans="1:22">
       <c r="A82" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>369</v>
@@ -8727,7 +8766,7 @@
         <v>27</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I82" s="3" t="s">
         <v>27</v>
@@ -8739,7 +8778,7 @@
         <v>60.76</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="M82" s="3" t="s">
         <v>117</v>
@@ -8748,42 +8787,42 @@
         <v>296</v>
       </c>
       <c r="O82" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="P82" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="Q82" s="3" t="s">
         <v>318</v>
       </c>
       <c r="R82" s="3" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="S82" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="T82" s="3" t="s">
         <v>132</v>
       </c>
       <c r="U82" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="V82" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="83" ht="46.75" spans="1:22">
       <c r="A83" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>26</v>
@@ -8818,16 +8857,16 @@
     </row>
     <row r="84" ht="46.75" spans="1:22">
       <c r="A84" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>26</v>
@@ -8862,16 +8901,16 @@
     </row>
     <row r="85" ht="16.75" spans="1:22">
       <c r="A85" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>26</v>
@@ -8895,10 +8934,10 @@
         <v>29.24</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="N85" s="3" t="s">
         <v>150</v>
@@ -8907,13 +8946,13 @@
         <v>213</v>
       </c>
       <c r="P85" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="Q85" s="3" t="s">
         <v>138</v>
       </c>
       <c r="R85" s="3" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="S85" s="3" t="s">
         <v>273</v>
@@ -8930,16 +8969,16 @@
     </row>
     <row r="86" ht="16.75" spans="1:22">
       <c r="A86" s="3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>26</v>
@@ -8963,7 +9002,7 @@
         <v>30.38</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M86" s="3" t="s">
         <v>105</v>
@@ -8981,7 +9020,7 @@
         <v>115</v>
       </c>
       <c r="R86" s="3" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="S86" s="3" t="s">
         <v>174</v>
@@ -8990,7 +9029,7 @@
         <v>193</v>
       </c>
       <c r="U86" s="3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="V86" s="3" t="s">
         <v>47</v>
@@ -8998,16 +9037,16 @@
     </row>
     <row r="87" ht="46.75" spans="1:22">
       <c r="A87" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>26</v>
@@ -9016,10 +9055,10 @@
         <v>15</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I87" s="3" t="s">
         <v>27</v>
@@ -9031,16 +9070,16 @@
         <v>46.26</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="N87" s="3" t="s">
         <v>150</v>
       </c>
       <c r="O87" s="3" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="P87" s="3" t="s">
         <v>32</v>
@@ -9049,16 +9088,16 @@
         <v>138</v>
       </c>
       <c r="R87" s="3" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="S87" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="T87" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U87" s="3" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="V87" s="3" t="s">
         <v>56</v>
@@ -9066,16 +9105,16 @@
     </row>
     <row r="88" ht="46.75" spans="1:22">
       <c r="A88" s="3" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>26</v>
@@ -9084,10 +9123,10 @@
         <v>50</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I88" s="3" t="s">
         <v>27</v>
@@ -9099,16 +9138,16 @@
         <v>47.26</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="N88" s="3" t="s">
         <v>171</v>
       </c>
       <c r="O88" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="P88" s="3" t="s">
         <v>371</v>
@@ -9117,16 +9156,16 @@
         <v>138</v>
       </c>
       <c r="R88" s="3" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="S88" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="T88" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U88" s="3" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="V88" s="3" t="s">
         <v>47</v>
@@ -9134,16 +9173,16 @@
     </row>
     <row r="89" ht="31.75" spans="1:22">
       <c r="A89" s="3" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>26</v>
@@ -9167,7 +9206,7 @@
         <v>32.11</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="M89" s="3" t="s">
         <v>105</v>
@@ -9179,7 +9218,7 @@
         <v>125</v>
       </c>
       <c r="P89" s="3" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="Q89" s="3" t="s">
         <v>138</v>
@@ -9202,16 +9241,16 @@
     </row>
     <row r="90" ht="31.75" spans="1:22">
       <c r="A90" s="3" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E90" s="11" t="s">
         <v>369</v>
@@ -9235,10 +9274,10 @@
         <v>38.91</v>
       </c>
       <c r="L90" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="N90" s="3" t="s">
         <v>204</v>
@@ -9253,7 +9292,7 @@
         <v>138</v>
       </c>
       <c r="R90" s="3" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="S90" s="3" t="s">
         <v>54</v>
@@ -9262,24 +9301,24 @@
         <v>55</v>
       </c>
       <c r="U90" s="3" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="V90" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="91" ht="16.75" spans="1:22">
       <c r="A91" s="3" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>369</v>
@@ -9291,7 +9330,7 @@
         <v>27</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I91" s="3" t="s">
         <v>27</v>
@@ -9303,34 +9342,34 @@
         <v>57.07</v>
       </c>
       <c r="L91" s="3" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="N91" s="3" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="O91" s="3" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="Q91" s="3" t="s">
         <v>47</v>
       </c>
       <c r="R91" s="3" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="S91" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="T91" s="3" t="s">
         <v>132</v>
       </c>
       <c r="U91" s="3" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="V91" s="3" t="s">
         <v>318</v>
@@ -9338,16 +9377,16 @@
     </row>
     <row r="92" ht="16.75" spans="1:22">
       <c r="A92" s="3" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E92" s="11" t="s">
         <v>369</v>
@@ -9359,7 +9398,7 @@
         <v>27</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>27</v>
@@ -9371,34 +9410,34 @@
         <v>56.73</v>
       </c>
       <c r="L92" s="3" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="N92" s="3" t="s">
         <v>212</v>
       </c>
       <c r="O92" s="3" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="Q92" s="3" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="R92" s="3" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="S92" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="T92" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U92" s="3" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="V92" s="3" t="s">
         <v>47</v>
@@ -9406,16 +9445,16 @@
     </row>
     <row r="93" ht="16.75" spans="1:22">
       <c r="A93" s="3" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>369</v>
@@ -9427,7 +9466,7 @@
         <v>27</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I93" s="3" t="s">
         <v>27</v>
@@ -9439,48 +9478,48 @@
         <v>61.93</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="N93" s="3" t="s">
         <v>212</v>
       </c>
       <c r="O93" s="3" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="P93" s="3" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="Q93" s="3" t="s">
         <v>176</v>
       </c>
       <c r="R93" s="3" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="S93" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="T93" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U93" s="3" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="V93" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="94" ht="16.75" spans="1:22">
       <c r="A94" s="3" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>142</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>142</v>
@@ -9507,7 +9546,7 @@
         <v>41.84</v>
       </c>
       <c r="L94" s="3" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="M94" s="3" t="s">
         <v>320</v>
@@ -9516,16 +9555,16 @@
         <v>50</v>
       </c>
       <c r="O94" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="P94" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="Q94" s="3" t="s">
         <v>56</v>
       </c>
       <c r="R94" s="3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="S94" s="3" t="s">
         <v>273</v>
@@ -9534,7 +9573,7 @@
         <v>45</v>
       </c>
       <c r="U94" s="3" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="V94" s="3" t="s">
         <v>138</v>
@@ -9542,16 +9581,16 @@
     </row>
     <row r="95" ht="46.75" spans="1:22">
       <c r="A95" s="15" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>369</v>
@@ -9575,7 +9614,7 @@
         <v>53.63</v>
       </c>
       <c r="L95" s="15" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="M95" s="3" t="s">
         <v>314</v>
@@ -9584,42 +9623,42 @@
         <v>204</v>
       </c>
       <c r="O95" s="3" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="P95" s="3" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="Q95" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="R95" s="3" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="S95" s="3" t="s">
         <v>318</v>
       </c>
       <c r="T95" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U95" s="3" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="V95" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="96" ht="31.75" spans="1:22">
       <c r="A96" s="3" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E96" s="5" t="s">
         <v>26</v>
@@ -9643,10 +9682,10 @@
         <v>40.15</v>
       </c>
       <c r="L96" s="3" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="N96" s="3" t="s">
         <v>293</v>
@@ -9661,7 +9700,7 @@
         <v>115</v>
       </c>
       <c r="R96" s="3" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="S96" s="3" t="s">
         <v>63</v>
@@ -9673,21 +9712,21 @@
         <v>107</v>
       </c>
       <c r="V96" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="97" ht="16.75" spans="1:22">
       <c r="A97" s="3" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>369</v>
@@ -9699,7 +9738,7 @@
         <v>27</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I97" s="3" t="s">
         <v>27</v>
@@ -9711,7 +9750,7 @@
         <v>58.04</v>
       </c>
       <c r="L97" s="3" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="M97" s="3" t="s">
         <v>325</v>
@@ -9720,25 +9759,25 @@
         <v>212</v>
       </c>
       <c r="O97" s="3" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="P97" s="3" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="Q97" s="3" t="s">
         <v>115</v>
       </c>
       <c r="R97" s="3" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="S97" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="T97" s="3" t="s">
         <v>132</v>
       </c>
       <c r="U97" s="3" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="V97" s="3" t="s">
         <v>47</v>
@@ -9746,16 +9785,16 @@
     </row>
     <row r="98" ht="46.75" spans="1:22">
       <c r="A98" s="3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>26</v>
@@ -9767,7 +9806,7 @@
         <v>27</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I98" s="3" t="s">
         <v>27</v>
@@ -9779,7 +9818,7 @@
         <v>46.88</v>
       </c>
       <c r="L98" s="3" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="M98" s="3" t="s">
         <v>151</v>
@@ -9788,7 +9827,7 @@
         <v>296</v>
       </c>
       <c r="O98" s="3" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="P98" s="3" t="s">
         <v>41</v>
@@ -9797,33 +9836,33 @@
         <v>138</v>
       </c>
       <c r="R98" s="3" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="S98" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="T98" s="3" t="s">
         <v>132</v>
       </c>
       <c r="U98" s="3" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="V98" s="3" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="99" ht="46.75" spans="1:22">
       <c r="A99" s="3" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>26</v>
@@ -9835,7 +9874,7 @@
         <v>27</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I99" s="3" t="s">
         <v>27</v>
@@ -9847,16 +9886,16 @@
         <v>48.03</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="N99" s="3" t="s">
         <v>204</v>
       </c>
       <c r="O99" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="P99" s="3" t="s">
         <v>41</v>
@@ -9865,33 +9904,33 @@
         <v>138</v>
       </c>
       <c r="R99" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="S99" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="T99" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U99" s="3" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="V99" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="100" ht="92.75" spans="1:22">
       <c r="A100" s="3" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E100" s="11" t="s">
         <v>369</v>
@@ -9903,7 +9942,7 @@
         <v>27</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>27</v>
@@ -9915,7 +9954,7 @@
         <v>63.41</v>
       </c>
       <c r="L100" s="3" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="M100" s="3" t="s">
         <v>314</v>
@@ -9924,42 +9963,42 @@
         <v>315</v>
       </c>
       <c r="O100" s="3" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="P100" s="3" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="Q100" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="R100" s="3" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="S100" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="T100" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U100" s="3" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="V100" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="101" ht="46.75" spans="1:22">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="101" ht="31.75" spans="1:22">
       <c r="A101" s="3" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E101" s="11" t="s">
         <v>369</v>
@@ -9971,10 +10010,10 @@
         <v>27</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="J101" s="14">
         <v>45934</v>
@@ -10004,30 +10043,30 @@
         <v>567</v>
       </c>
       <c r="S101" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="T101" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U101" s="3" t="s">
         <v>568</v>
       </c>
       <c r="V101" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="102" ht="46.75" spans="1:22">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="102" ht="31.75" spans="1:22">
       <c r="A102" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E102" s="11" t="s">
         <v>369</v>
@@ -10039,7 +10078,7 @@
         <v>27</v>
       </c>
       <c r="H102" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I102" s="3" t="s">
         <v>27</v>
@@ -10063,7 +10102,7 @@
         <v>571</v>
       </c>
       <c r="P102" s="3" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="Q102" s="3" t="s">
         <v>572</v>
@@ -10072,7 +10111,7 @@
         <v>573</v>
       </c>
       <c r="S102" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="T102" s="3" t="s">
         <v>132</v>
@@ -10084,18 +10123,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="103" ht="46.75" spans="1:22">
+    <row r="103" ht="31.75" spans="1:22">
       <c r="A103" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E103" s="11" t="s">
         <v>369</v>
@@ -10107,7 +10146,7 @@
         <v>27</v>
       </c>
       <c r="H103" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I103" s="3" t="s">
         <v>27</v>
@@ -10122,7 +10161,7 @@
         <v>575</v>
       </c>
       <c r="M103" s="3" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="N103" s="3" t="s">
         <v>204</v>
@@ -10140,7 +10179,7 @@
         <v>578</v>
       </c>
       <c r="S103" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="T103" s="3" t="s">
         <v>132</v>
@@ -10149,21 +10188,21 @@
         <v>579</v>
       </c>
       <c r="V103" s="3" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="104" ht="46.75" spans="1:22">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="104" ht="31.75" spans="1:22">
       <c r="A104" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E104" s="11" t="s">
         <v>369</v>
@@ -10175,7 +10214,7 @@
         <v>27</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I104" s="3" t="s">
         <v>27</v>
@@ -10217,21 +10256,21 @@
         <v>585</v>
       </c>
       <c r="V104" s="3" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="105" ht="46.75" spans="1:22">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="105" ht="31.75" spans="1:22">
       <c r="A105" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E105" s="11" t="s">
         <v>369</v>
@@ -10243,7 +10282,7 @@
         <v>27</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I105" s="3" t="s">
         <v>27</v>
@@ -10267,7 +10306,7 @@
         <v>576</v>
       </c>
       <c r="P105" s="3" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="Q105" s="3" t="s">
         <v>583</v>
@@ -10288,18 +10327,18 @@
         <v>318</v>
       </c>
     </row>
-    <row r="106" ht="46.75" spans="1:22">
+    <row r="106" ht="31.75" spans="1:22">
       <c r="A106" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E106" s="11" t="s">
         <v>369</v>
@@ -10311,7 +10350,7 @@
         <v>27</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I106" s="3" t="s">
         <v>27</v>
@@ -10335,7 +10374,7 @@
         <v>576</v>
       </c>
       <c r="P106" s="3" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="Q106" s="3" t="s">
         <v>572</v>
@@ -10344,7 +10383,7 @@
         <v>592</v>
       </c>
       <c r="S106" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="T106" s="3" t="s">
         <v>132</v>
@@ -10353,21 +10392,21 @@
         <v>593</v>
       </c>
       <c r="V106" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="107" ht="46.75" spans="1:22">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="107" ht="31.75" spans="1:22">
       <c r="A107" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E107" s="11" t="s">
         <v>369</v>
@@ -10379,7 +10418,7 @@
         <v>27</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I107" s="3" t="s">
         <v>27</v>
@@ -10412,7 +10451,7 @@
         <v>596</v>
       </c>
       <c r="S107" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="T107" s="3" t="s">
         <v>45</v>
@@ -10421,21 +10460,21 @@
         <v>568</v>
       </c>
       <c r="V107" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="108" ht="46.75" spans="1:22">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="108" ht="31.75" spans="1:22">
       <c r="A108" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E108" s="11" t="s">
         <v>369</v>
@@ -10447,7 +10486,7 @@
         <v>27</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I108" s="3" t="s">
         <v>27</v>
@@ -10480,10 +10519,10 @@
         <v>599</v>
       </c>
       <c r="S108" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="T108" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U108" s="3" t="s">
         <v>600</v>
@@ -10492,18 +10531,18 @@
         <v>318</v>
       </c>
     </row>
-    <row r="109" ht="46.75" spans="1:22">
+    <row r="109" ht="31.75" spans="1:22">
       <c r="A109" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E109" s="11" t="s">
         <v>369</v>
@@ -10515,7 +10554,7 @@
         <v>27</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I109" s="3" t="s">
         <v>27</v>
@@ -10548,30 +10587,30 @@
         <v>604</v>
       </c>
       <c r="S109" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="T109" s="3" t="s">
         <v>132</v>
       </c>
       <c r="U109" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="V109" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="110" ht="46.75" spans="1:22">
+    <row r="110" ht="31.75" spans="1:22">
       <c r="A110" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E110" s="11" t="s">
         <v>369</v>
@@ -10583,7 +10622,7 @@
         <v>27</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I110" s="3" t="s">
         <v>27</v>
@@ -10598,7 +10637,7 @@
         <v>605</v>
       </c>
       <c r="M110" s="3" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="N110" s="3" t="s">
         <v>171</v>
@@ -10619,27 +10658,27 @@
         <v>44</v>
       </c>
       <c r="T110" s="3" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="U110" s="3" t="s">
         <v>607</v>
       </c>
       <c r="V110" s="3" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="111" ht="46.75" spans="1:22">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="111" ht="31.75" spans="1:22">
       <c r="A111" s="3" t="s">
         <v>569</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>561</v>
+        <v>368</v>
       </c>
       <c r="E111" s="11" t="s">
         <v>369</v>
@@ -10651,7 +10690,7 @@
         <v>27</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I111" s="3" t="s">
         <v>27</v>
@@ -10693,24 +10732,24 @@
         <v>610</v>
       </c>
       <c r="V111" s="3" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="112" ht="16.75" spans="1:22">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="112" ht="31.75" spans="1:22">
       <c r="A112" s="3" t="s">
         <v>611</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>142</v>
+        <v>560</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>517</v>
+        <v>561</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E112" s="10" t="s">
-        <v>74</v>
+        <v>368</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>369</v>
       </c>
       <c r="F112" s="6">
         <v>100</v>
@@ -10719,40 +10758,40 @@
         <v>27</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>27</v>
+        <v>429</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>27</v>
+        <v>429</v>
       </c>
       <c r="J112" s="14">
-        <v>45944</v>
+        <v>46002</v>
       </c>
       <c r="K112" s="6">
-        <v>53.1</v>
+        <v>72.58</v>
       </c>
       <c r="L112" s="3" t="s">
         <v>612</v>
       </c>
       <c r="M112" s="3" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="N112" s="3" t="s">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="O112" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="P112" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="P112" s="3" t="s">
+      <c r="Q112" s="3" t="s">
         <v>614</v>
-      </c>
-      <c r="Q112" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="R112" s="3" t="s">
         <v>615</v>
       </c>
       <c r="S112" s="3" t="s">
-        <v>273</v>
+        <v>548</v>
       </c>
       <c r="T112" s="3" t="s">
         <v>132</v>
@@ -10761,7 +10800,7 @@
         <v>616</v>
       </c>
       <c r="V112" s="3" t="s">
-        <v>318</v>
+        <v>424</v>
       </c>
     </row>
     <row r="113" ht="31.75" spans="1:22">
@@ -10769,16 +10808,16 @@
         <v>617</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>618</v>
+        <v>560</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>619</v>
+        <v>561</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>620</v>
-      </c>
-      <c r="E113" s="10" t="s">
-        <v>74</v>
+        <v>368</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>369</v>
       </c>
       <c r="F113" s="6">
         <v>100</v>
@@ -10787,66 +10826,66 @@
         <v>27</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>27</v>
+        <v>429</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>27</v>
+        <v>429</v>
       </c>
       <c r="J113" s="14">
-        <v>45953</v>
+        <v>46002</v>
       </c>
       <c r="K113" s="6">
-        <v>41.57</v>
+        <v>67.46</v>
       </c>
       <c r="L113" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="M113" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="N113" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O113" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="P113" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="M113" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="N113" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="O113" s="3" t="s">
+      <c r="Q113" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="R113" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="P113" s="3" t="s">
+      <c r="S113" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="T113" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="U113" s="3" t="s">
         <v>623</v>
-      </c>
-      <c r="Q113" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="R113" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="S113" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="T113" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="U113" s="3" t="s">
-        <v>625</v>
       </c>
       <c r="V113" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="114" ht="31.75" spans="1:22">
+    <row r="114" ht="16.75" spans="1:22">
       <c r="A114" s="3" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>530</v>
+        <v>142</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>26</v>
+        <v>142</v>
+      </c>
+      <c r="E114" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="F114" s="6">
         <v>100</v>
@@ -10861,63 +10900,63 @@
         <v>27</v>
       </c>
       <c r="J114" s="14">
-        <v>45961</v>
+        <v>45944</v>
       </c>
       <c r="K114" s="6">
-        <v>53.91</v>
+        <v>53.1</v>
       </c>
       <c r="L114" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="M114" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="N114" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O114" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="P114" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="M114" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="N114" s="3" t="s">
+      <c r="Q114" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R114" s="3" t="s">
         <v>628</v>
       </c>
-      <c r="O114" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="P114" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="Q114" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="R114" s="3" t="s">
+      <c r="S114" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="T114" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="U114" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="S114" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="T114" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="U114" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="V114" s="3" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="115" ht="16.75" spans="1:22">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="115" ht="31.75" spans="1:22">
       <c r="A115" s="3" t="s">
         <v>630</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>101</v>
+        <v>631</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>103</v>
+        <v>633</v>
       </c>
       <c r="E115" s="10" t="s">
         <v>74</v>
       </c>
       <c r="F115" s="6">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>27</v>
@@ -10929,63 +10968,63 @@
         <v>27</v>
       </c>
       <c r="J115" s="14">
-        <v>45961</v>
+        <v>45953</v>
       </c>
       <c r="K115" s="6">
-        <v>42.88</v>
+        <v>41.57</v>
       </c>
       <c r="L115" s="3" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="M115" s="3" t="s">
-        <v>110</v>
+        <v>320</v>
       </c>
       <c r="N115" s="3" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="O115" s="3" t="s">
-        <v>126</v>
+        <v>635</v>
       </c>
       <c r="P115" s="3" t="s">
-        <v>577</v>
+        <v>636</v>
       </c>
       <c r="Q115" s="3" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="R115" s="3" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="S115" s="3" t="s">
-        <v>386</v>
+        <v>415</v>
       </c>
       <c r="T115" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U115" s="3" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="V115" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="116" ht="16.75" spans="1:22">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="116" ht="31.75" spans="1:22">
       <c r="A116" s="3" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>101</v>
+        <v>531</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>631</v>
+        <v>532</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E116" s="10" t="s">
-        <v>74</v>
+        <v>533</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="F116" s="6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>27</v>
@@ -11000,51 +11039,51 @@
         <v>45961</v>
       </c>
       <c r="K116" s="6">
-        <v>58.08</v>
+        <v>53.91</v>
       </c>
       <c r="L116" s="3" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="M116" s="3" t="s">
-        <v>320</v>
+        <v>117</v>
       </c>
       <c r="N116" s="3" t="s">
-        <v>171</v>
+        <v>641</v>
       </c>
       <c r="O116" s="3" t="s">
-        <v>613</v>
+        <v>479</v>
       </c>
       <c r="P116" s="3" t="s">
-        <v>636</v>
+        <v>508</v>
       </c>
       <c r="Q116" s="3" t="s">
-        <v>176</v>
+        <v>452</v>
       </c>
       <c r="R116" s="3" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="S116" s="3" t="s">
-        <v>44</v>
+        <v>446</v>
       </c>
       <c r="T116" s="3" t="s">
         <v>45</v>
       </c>
       <c r="U116" s="3" t="s">
-        <v>638</v>
+        <v>107</v>
       </c>
       <c r="V116" s="3" t="s">
-        <v>47</v>
+        <v>452</v>
       </c>
     </row>
     <row r="117" ht="16.75" spans="1:22">
       <c r="A117" s="3" t="s">
-        <v>630</v>
+        <v>643</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>631</v>
+        <v>644</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>103</v>
@@ -11053,7 +11092,7 @@
         <v>74</v>
       </c>
       <c r="F117" s="6">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>27</v>
@@ -11068,60 +11107,60 @@
         <v>45961</v>
       </c>
       <c r="K117" s="6">
-        <v>62.88</v>
+        <v>42.88</v>
       </c>
       <c r="L117" s="3" t="s">
-        <v>639</v>
+        <v>645</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>506</v>
+        <v>110</v>
       </c>
       <c r="N117" s="3" t="s">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="O117" s="3" t="s">
-        <v>598</v>
+        <v>126</v>
       </c>
       <c r="P117" s="3" t="s">
-        <v>640</v>
+        <v>577</v>
       </c>
       <c r="Q117" s="3" t="s">
-        <v>641</v>
+        <v>56</v>
       </c>
       <c r="R117" s="3" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="S117" s="3" t="s">
-        <v>44</v>
+        <v>387</v>
       </c>
       <c r="T117" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="U117" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="V117" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="118" s="1" customFormat="1" ht="16.75" spans="1:22">
+      <c r="A118" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="V117" s="3" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="118" s="1" customFormat="1" ht="31.75" spans="1:22">
-      <c r="A118" s="3" t="s">
+      <c r="B118" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C118" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="B118" s="4" t="s">
-        <v>645</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>646</v>
-      </c>
-      <c r="D118" s="4" t="s">
-        <v>645</v>
-      </c>
-      <c r="E118" s="11" t="s">
-        <v>369</v>
+      <c r="D118" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E118" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="F118" s="6">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>27</v>
@@ -11133,31 +11172,31 @@
         <v>27</v>
       </c>
       <c r="J118" s="14">
-        <v>45986</v>
+        <v>45961</v>
       </c>
       <c r="K118" s="6">
-        <v>64.22</v>
+        <v>58.08</v>
       </c>
       <c r="L118" s="3" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="M118" s="3" t="s">
-        <v>506</v>
+        <v>320</v>
       </c>
       <c r="N118" s="3" t="s">
-        <v>315</v>
+        <v>171</v>
       </c>
       <c r="O118" s="3" t="s">
-        <v>571</v>
+        <v>626</v>
       </c>
       <c r="P118" s="3" t="s">
-        <v>565</v>
+        <v>649</v>
       </c>
       <c r="Q118" s="3" t="s">
-        <v>307</v>
+        <v>176</v>
       </c>
       <c r="R118" s="3" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="S118" s="3" t="s">
         <v>44</v>
@@ -11166,21 +11205,147 @@
         <v>45</v>
       </c>
       <c r="U118" s="3" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="V118" s="3" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="119" ht="15.2" spans="1:22">
-      <c r="G119" s="17"/>
-      <c r="J119" s="18"/>
-      <c r="K119" s="19"/>
-    </row>
-    <row r="120" ht="15.2" spans="1:22">
-      <c r="G120" s="17"/>
-      <c r="J120" s="18"/>
-      <c r="K120" s="19"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="119" ht="16.75" spans="1:22">
+      <c r="A119" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E119" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F119" s="6">
+        <v>100</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J119" s="14">
+        <v>45961</v>
+      </c>
+      <c r="K119" s="6">
+        <v>62.88</v>
+      </c>
+      <c r="L119" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="M119" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="N119" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="O119" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="P119" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="Q119" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="R119" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="S119" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T119" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="U119" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="V119" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="120" ht="31.75" spans="1:22">
+      <c r="A120" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="E120" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="F120" s="6">
+        <v>15</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J120" s="14">
+        <v>45986</v>
+      </c>
+      <c r="K120" s="6">
+        <v>64.22</v>
+      </c>
+      <c r="L120" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="M120" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="N120" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="O120" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="P120" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="Q120" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="S120" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T120" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="U120" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="121" ht="15.2" spans="1:22">
       <c r="G121" s="17"/>
@@ -15902,15 +16067,17 @@
     <hyperlink ref="C98" r:id="rId19" display="https://arxiv.org/pdf/2508.14040" tooltip="https://arxiv.org/pdf/2508.14040"/>
     <hyperlink ref="C99" r:id="rId19" display="https://arxiv.org/pdf/2508.14040" tooltip="https://arxiv.org/pdf/2508.14040"/>
     <hyperlink ref="C100" r:id="rId25" display="https://arxiv.org/pdf/2507.05791" tooltip="https://arxiv.org/pdf/2507.05791"/>
-    <hyperlink ref="C112" r:id="rId22" display="https://arxiv.org/pdf/2509.02544" tooltip="https://arxiv.org/pdf/2509.02544"/>
-    <hyperlink ref="C113" r:id="rId26" display="https://qwen.ai/blog?id=99f0335c4ad9ff6153e517418d48535ab6d8afef&amp;from=research.latest-advancements-list" tooltip="https://qwen.ai/blog?id=99f0335c4ad9ff6153e517418d48535ab6d8afef&amp;from=research.latest-advancements-list"/>
-    <hyperlink ref="C114" r:id="rId27" display="https://arxiv.org/abs/2509.17336" tooltip="https://arxiv.org/abs/2509.17336"/>
-    <hyperlink ref="C115" r:id="rId28" display="https://www.anthropic.com/news/claude-sonnet-4-5" tooltip="https://www.anthropic.com/news/claude-sonnet-4-5"/>
-    <hyperlink ref="C116" r:id="rId28" display="https://www.anthropic.com/news/claude-sonnet-4-5" tooltip="https://www.anthropic.com/news/claude-sonnet-4-5"/>
-    <hyperlink ref="C117" r:id="rId28" display="https://www.anthropic.com/news/claude-sonnet-4-5" tooltip="https://www.anthropic.com/news/claude-sonnet-4-5"/>
-    <hyperlink ref="B118" r:id="rId29" display="GBOX.AI" tooltip="http://GBOX.AI"/>
-    <hyperlink ref="C118" r:id="rId30" display="https://github.com/babelcloud/GBOXBlog/blob/main/From_Vision_to_Action.md" tooltip="https://github.com/babelcloud/GBOXBlog/blob/main/From_Vision_to_Action.md"/>
-    <hyperlink ref="D118" r:id="rId29" display="GBOX.AI" tooltip="http://GBOX.AI"/>
+    <hyperlink ref="C112" r:id="rId26" display="https://arxiv.org/abs/2510.02250" tooltip="https://arxiv.org/abs/2510.02250"/>
+    <hyperlink ref="C113" r:id="rId26" display="https://arxiv.org/abs/2510.02250" tooltip="https://arxiv.org/abs/2510.02250"/>
+    <hyperlink ref="C114" r:id="rId22" display="https://arxiv.org/pdf/2509.02544" tooltip="https://arxiv.org/pdf/2509.02544"/>
+    <hyperlink ref="C115" r:id="rId27" display="https://qwen.ai/blog?id=99f0335c4ad9ff6153e517418d48535ab6d8afef&amp;from=research.latest-advancements-list" tooltip="https://qwen.ai/blog?id=99f0335c4ad9ff6153e517418d48535ab6d8afef&amp;from=research.latest-advancements-list"/>
+    <hyperlink ref="C116" r:id="rId28" display="https://arxiv.org/abs/2509.17336" tooltip="https://arxiv.org/abs/2509.17336"/>
+    <hyperlink ref="C117" r:id="rId29" display="https://www.anthropic.com/news/claude-sonnet-4-5" tooltip="https://www.anthropic.com/news/claude-sonnet-4-5"/>
+    <hyperlink ref="C118" r:id="rId29" display="https://www.anthropic.com/news/claude-sonnet-4-5" tooltip="https://www.anthropic.com/news/claude-sonnet-4-5"/>
+    <hyperlink ref="C119" r:id="rId29" display="https://www.anthropic.com/news/claude-sonnet-4-5" tooltip="https://www.anthropic.com/news/claude-sonnet-4-5"/>
+    <hyperlink ref="B120" r:id="rId30" display="GBOX.AI" tooltip="http://GBOX.AI"/>
+    <hyperlink ref="C120" r:id="rId31" display="https://github.com/babelcloud/GBOXBlog/blob/main/From_Vision_to_Action.md" tooltip="https://github.com/babelcloud/GBOXBlog/blob/main/From_Vision_to_Action.md"/>
+    <hyperlink ref="D120" r:id="rId30" display="GBOX.AI" tooltip="http://GBOX.AI"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update verified results file with new data
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -3262,7 +3262,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C112" sqref="A1:V120"/>
+      <selection activeCell="E112" sqref="A1:V120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -10829,7 +10829,7 @@
         <v>429</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>429</v>
+        <v>27</v>
       </c>
       <c r="J113" s="14">
         <v>46002</v>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with latest verified data
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13260"/>
+    <workbookView windowWidth="27660" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Eval Results" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2328" uniqueCount="690">
   <si>
     <t>Model</t>
   </si>
@@ -2073,6 +2073,30 @@
   </si>
   <si>
     <t>21.00/23</t>
+  </si>
+  <si>
+    <t>Seed-1.8</t>
+  </si>
+  <si>
+    <t>https://seed.bytedance.com/en/seed1_8</t>
+  </si>
+  <si>
+    <t>222.12 / 359</t>
+  </si>
+  <si>
+    <t>28.96/45</t>
+  </si>
+  <si>
+    <t>28.62/47</t>
+  </si>
+  <si>
+    <t>18.88/23</t>
+  </si>
+  <si>
+    <t>38.99/92</t>
+  </si>
+  <si>
+    <t>10.67/17</t>
   </si>
 </sst>
 </file>
@@ -3316,7 +3340,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E113" sqref="A1:V124"/>
+      <selection activeCell="C113" sqref="A1:V125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -11673,10 +11697,73 @@
         <v>681</v>
       </c>
     </row>
-    <row r="125" ht="15.2" spans="1:22">
-      <c r="G125" s="17"/>
-      <c r="J125" s="18"/>
-      <c r="K125" s="19"/>
+    <row r="125" ht="16.75" spans="1:22">
+      <c r="A125" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E125" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F125" s="6">
+        <v>100</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J125" s="14">
+        <v>46009</v>
+      </c>
+      <c r="K125" s="6">
+        <v>61.87</v>
+      </c>
+      <c r="L125" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="M125" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="N125" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="O125" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="P125" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="Q125" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="R125" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="S125" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="T125" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="U125" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="V125" s="3" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="126" ht="15.2" spans="1:22">
       <c r="G126" s="17"/>
@@ -16388,6 +16475,7 @@
     <hyperlink ref="B124" r:id="rId30" display="GBOX.AI" tooltip="http://GBOX.AI"/>
     <hyperlink ref="C124" r:id="rId31" display="https://github.com/babelcloud/GBOXBlog/blob/main/From_Vision_to_Action.md" tooltip="https://github.com/babelcloud/GBOXBlog/blob/main/From_Vision_to_Action.md"/>
     <hyperlink ref="D124" r:id="rId30" display="GBOX.AI" tooltip="http://GBOX.AI"/>
+    <hyperlink ref="C125" r:id="rId32" display="https://seed.bytedance.com/en/seed1_8" tooltip="https://seed.bytedance.com/en/seed1_8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with new verified data
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13200"/>
+    <workbookView windowWidth="27660" windowHeight="13480"/>
   </bookViews>
   <sheets>
     <sheet name="Eval Results" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2385" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="730">
   <si>
     <t>Model</t>
   </si>
@@ -2187,6 +2187,36 @@
   </si>
   <si>
     <t>8.87/17</t>
+  </si>
+  <si>
+    <t>OS-Symphony w/ GPT-5</t>
+  </si>
+  <si>
+    <t>Shanghai AI Laboratory</t>
+  </si>
+  <si>
+    <t>https://github.com/xlang-ai/OSWorld/tree/main/mm_agents/os_symphony</t>
+  </si>
+  <si>
+    <t>Shanghai AI Lab OS-Copilot Team</t>
+  </si>
+  <si>
+    <t>236.76/360</t>
+  </si>
+  <si>
+    <t>21.0/26</t>
+  </si>
+  <si>
+    <t>36.0/47</t>
+  </si>
+  <si>
+    <t>22.94/47</t>
+  </si>
+  <si>
+    <t>51.43/93</t>
+  </si>
+  <si>
+    <t>10.46/17</t>
   </si>
 </sst>
 </file>
@@ -3430,7 +3460,7 @@
   <dimension ref="A1:AC1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C109" sqref="A1:V128"/>
+      <selection activeCell="C113" sqref="A1:V129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -12059,82 +12089,145 @@
         <v>700</v>
       </c>
     </row>
-    <row r="129" ht="15.2" spans="7:11">
-      <c r="G129" s="17"/>
-      <c r="J129" s="18"/>
-      <c r="K129" s="19"/>
-    </row>
-    <row r="130" ht="15.2" spans="7:11">
+    <row r="129" ht="46.75" spans="1:22">
+      <c r="A129" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="E129" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="F129" s="6">
+        <v>50</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J129" s="14">
+        <v>46026</v>
+      </c>
+      <c r="K129" s="6">
+        <v>65.77</v>
+      </c>
+      <c r="L129" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="M129" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="N129" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="O129" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="P129" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="Q129" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="R129" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="S129" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="T129" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="U129" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="V129" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="130" ht="15.2" spans="1:22">
       <c r="G130" s="17"/>
       <c r="J130" s="18"/>
       <c r="K130" s="19"/>
     </row>
-    <row r="131" ht="15.2" spans="7:11">
+    <row r="131" ht="15.2" spans="1:22">
       <c r="G131" s="17"/>
       <c r="J131" s="18"/>
       <c r="K131" s="19"/>
     </row>
-    <row r="132" ht="15.2" spans="7:11">
+    <row r="132" ht="15.2" spans="1:22">
       <c r="G132" s="17"/>
       <c r="J132" s="18"/>
       <c r="K132" s="19"/>
     </row>
-    <row r="133" ht="15.2" spans="7:11">
+    <row r="133" ht="15.2" spans="1:22">
       <c r="G133" s="17"/>
       <c r="J133" s="18"/>
       <c r="K133" s="19"/>
     </row>
-    <row r="134" ht="15.2" spans="7:11">
+    <row r="134" ht="15.2" spans="1:22">
       <c r="G134" s="17"/>
       <c r="J134" s="18"/>
       <c r="K134" s="19"/>
     </row>
-    <row r="135" ht="15.2" spans="7:11">
+    <row r="135" ht="15.2" spans="1:22">
       <c r="G135" s="17"/>
       <c r="J135" s="18"/>
       <c r="K135" s="19"/>
     </row>
-    <row r="136" ht="15.2" spans="7:11">
+    <row r="136" ht="15.2" spans="1:22">
       <c r="G136" s="17"/>
       <c r="J136" s="18"/>
       <c r="K136" s="19"/>
     </row>
-    <row r="137" ht="15.2" spans="7:11">
+    <row r="137" ht="15.2" spans="1:22">
       <c r="G137" s="17"/>
       <c r="J137" s="18"/>
       <c r="K137" s="19"/>
     </row>
-    <row r="138" ht="15.2" spans="7:11">
+    <row r="138" ht="15.2" spans="1:22">
       <c r="G138" s="17"/>
       <c r="J138" s="18"/>
       <c r="K138" s="19"/>
     </row>
-    <row r="139" ht="15.2" spans="7:11">
+    <row r="139" ht="15.2" spans="1:22">
       <c r="G139" s="17"/>
       <c r="J139" s="18"/>
       <c r="K139" s="19"/>
     </row>
-    <row r="140" ht="15.2" spans="7:11">
+    <row r="140" ht="15.2" spans="1:22">
       <c r="G140" s="17"/>
       <c r="J140" s="18"/>
       <c r="K140" s="19"/>
     </row>
-    <row r="141" ht="15.2" spans="7:11">
+    <row r="141" ht="15.2" spans="1:22">
       <c r="G141" s="17"/>
       <c r="J141" s="18"/>
       <c r="K141" s="19"/>
     </row>
-    <row r="142" ht="15.2" spans="7:11">
+    <row r="142" ht="15.2" spans="1:22">
       <c r="G142" s="17"/>
       <c r="J142" s="18"/>
       <c r="K142" s="19"/>
     </row>
-    <row r="143" ht="15.2" spans="7:11">
+    <row r="143" ht="15.2" spans="1:22">
       <c r="G143" s="17"/>
       <c r="J143" s="18"/>
       <c r="K143" s="19"/>
     </row>
-    <row r="144" ht="15.2" spans="7:11">
+    <row r="144" ht="15.2" spans="1:22">
       <c r="G144" s="17"/>
       <c r="J144" s="18"/>
       <c r="K144" s="19"/>
@@ -16757,6 +16850,7 @@
     <hyperlink ref="C125" r:id="rId32" display="https://seed.bytedance.com/en/seed1_8" tooltip="https://seed.bytedance.com/en/seed1_8"/>
     <hyperlink ref="C126" r:id="rId33" display="https://github.com/xlang-ai/OSWorld/tree/main/mm_agents/uipath" tooltip="https://github.com/xlang-ai/OSWorld/tree/main/mm_agents/uipath"/>
     <hyperlink ref="C127" r:id="rId33" display="https://github.com/xlang-ai/OSWorld/tree/main/mm_agents/uipath" tooltip="https://github.com/xlang-ai/OSWorld/tree/main/mm_agents/uipath"/>
+    <hyperlink ref="C129" r:id="rId34" display="https://github.com/xlang-ai/OSWorld/tree/main/mm_agents/os_symphony" tooltip="https://github.com/xlang-ai/OSWorld/tree/main/mm_agents/os_symphony"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update osworld_verified_results.xlsx with additional verified data
</commit_message>
<xml_diff>
--- a/static/data/osworld_verified_results.xlsx
+++ b/static/data/osworld_verified_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="13420"/>
+    <workbookView windowWidth="27660" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="Eval Results" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2461" uniqueCount="751">
   <si>
     <t>Model</t>
   </si>
@@ -2253,6 +2253,33 @@
   </si>
   <si>
     <t>7.61/17</t>
+  </si>
+  <si>
+    <t>DART-GUI-7B-0924</t>
+  </si>
+  <si>
+    <t>BIGAI &amp; BIT &amp; DataCanvas</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2509.23866</t>
+  </si>
+  <si>
+    <t>146.08/361</t>
+  </si>
+  <si>
+    <t>7.0/47</t>
+  </si>
+  <si>
+    <t>11.0/23</t>
+  </si>
+  <si>
+    <t>16.51/93</t>
+  </si>
+  <si>
+    <t>13.0/24</t>
+  </si>
+  <si>
+    <t>10.0/15</t>
   </si>
 </sst>
 </file>
@@ -3479,7 +3506,7 @@
   <dimension ref="A1:AC1077"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:V131"/>
+      <selection activeCell="D15" sqref="A1:V132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -13199,29 +13226,73 @@
       <c r="AB131" s="4"/>
       <c r="AC131" s="4"/>
     </row>
-    <row r="132" ht="15.95" spans="1:29">
-      <c r="A132" s="4"/>
-      <c r="B132" s="4"/>
-      <c r="C132" s="4"/>
-      <c r="D132" s="4"/>
-      <c r="E132" s="4"/>
-      <c r="F132" s="4"/>
-      <c r="G132" s="4"/>
-      <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
-      <c r="J132" s="4"/>
-      <c r="K132" s="4"/>
-      <c r="L132" s="4"/>
-      <c r="M132" s="4"/>
-      <c r="N132" s="4"/>
-      <c r="O132" s="4"/>
-      <c r="P132" s="4"/>
-      <c r="Q132" s="4"/>
-      <c r="R132" s="4"/>
-      <c r="S132" s="4"/>
-      <c r="T132" s="4"/>
-      <c r="U132" s="4"/>
-      <c r="V132" s="4"/>
+    <row r="132" ht="31.75" spans="1:29">
+      <c r="A132" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F132" s="7">
+        <v>30</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J132" s="14">
+        <v>46045</v>
+      </c>
+      <c r="K132" s="7">
+        <v>40.47</v>
+      </c>
+      <c r="L132" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="M132" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="N132" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="O132" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="P132" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q132" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="R132" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="S132" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="T132" s="3" t="s">
+        <v>750</v>
+      </c>
+      <c r="U132" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="V132" s="3" t="s">
+        <v>694</v>
+      </c>
       <c r="W132" s="4"/>
       <c r="X132" s="4"/>
       <c r="Y132" s="4"/>
@@ -42647,6 +42718,7 @@
     <hyperlink ref="C129" r:id="rId35" display="https://github.com/xlang-ai/OSWorld/tree/main/mm_agents/os_symphony" tooltip="https://github.com/xlang-ai/OSWorld/tree/main/mm_agents/os_symphony"/>
     <hyperlink ref="C130" r:id="rId34" display="https://arxiv.org/abs/2601.15876" tooltip="https://arxiv.org/abs/2601.15876"/>
     <hyperlink ref="C131" r:id="rId34" display="https://arxiv.org/abs/2601.15876" tooltip="https://arxiv.org/abs/2601.15876"/>
+    <hyperlink ref="C132" r:id="rId36" display="https://arxiv.org/pdf/2509.23866" tooltip="https://arxiv.org/pdf/2509.23866"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>